<commit_message>
Feladat név módosítása, időpontok módosítása
</commit_message>
<xml_diff>
--- a/Gantt-diagram-A.xlsx
+++ b/Gantt-diagram-A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagyp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szabó Tímea\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97182E64-774D-45B2-B845-BD07682EA562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E6D57B-EFB5-438A-A6C2-CB07948055D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt-diagram" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>8.3.1. Táblákat létre hozó SQL kódok létrehozása DB-hez</t>
   </si>
   <si>
-    <t>8.3.2. Moodboard összeállítása, alap dizájn összerakása</t>
-  </si>
-  <si>
     <t>8.3.3. Felhasználók kezelése (admin, felhasználó) (CR)</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>8.4.11. Bemutató elkészítése</t>
+  </si>
+  <si>
+    <t>8.3.2. Egységes megjelenés tervezése, készítése</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1467,9 +1467,6 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1554,44 +1551,58 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1599,22 +1610,30 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1623,58 +1642,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1895,18 +1907,18 @@
   </sheetPr>
   <dimension ref="A1:CE1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T41" sqref="T41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AV3" sqref="AV3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="80.46484375" customWidth="1"/>
-    <col min="3" max="3" width="15.46484375" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="80.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="83" width="2.46484375" customWidth="1"/>
+    <col min="6" max="83" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" ht="25.5" customHeight="1">
@@ -2009,10 +2021,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="134" t="s">
+      <c r="D2" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="135"/>
+      <c r="E2" s="146"/>
       <c r="F2" s="5"/>
       <c r="G2" s="18"/>
       <c r="H2" s="6"/>
@@ -2096,10 +2108,10 @@
       <c r="A3" s="16"/>
       <c r="B3" s="19"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="134">
+      <c r="D3" s="145">
         <v>45197</v>
       </c>
-      <c r="E3" s="135"/>
+      <c r="E3" s="146"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -2185,117 +2197,117 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="138">
+      <c r="F4" s="147"/>
+      <c r="G4" s="142">
         <f>G5</f>
         <v>45194</v>
       </c>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="138">
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="142">
         <f>N5</f>
         <v>45201</v>
       </c>
-      <c r="O4" s="139"/>
-      <c r="P4" s="139"/>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="139"/>
-      <c r="T4" s="140"/>
-      <c r="U4" s="138">
+      <c r="O4" s="143"/>
+      <c r="P4" s="143"/>
+      <c r="Q4" s="143"/>
+      <c r="R4" s="143"/>
+      <c r="S4" s="143"/>
+      <c r="T4" s="144"/>
+      <c r="U4" s="142">
         <f>U5</f>
         <v>45208</v>
       </c>
-      <c r="V4" s="139"/>
-      <c r="W4" s="139"/>
-      <c r="X4" s="139"/>
-      <c r="Y4" s="139"/>
-      <c r="Z4" s="139"/>
-      <c r="AA4" s="140"/>
-      <c r="AB4" s="138">
+      <c r="V4" s="143"/>
+      <c r="W4" s="143"/>
+      <c r="X4" s="143"/>
+      <c r="Y4" s="143"/>
+      <c r="Z4" s="143"/>
+      <c r="AA4" s="144"/>
+      <c r="AB4" s="142">
         <f>AB5</f>
         <v>45215</v>
       </c>
-      <c r="AC4" s="139"/>
-      <c r="AD4" s="139"/>
-      <c r="AE4" s="139"/>
-      <c r="AF4" s="139"/>
-      <c r="AG4" s="139"/>
-      <c r="AH4" s="140"/>
-      <c r="AI4" s="138">
+      <c r="AC4" s="143"/>
+      <c r="AD4" s="143"/>
+      <c r="AE4" s="143"/>
+      <c r="AF4" s="143"/>
+      <c r="AG4" s="143"/>
+      <c r="AH4" s="144"/>
+      <c r="AI4" s="142">
         <f>AI5</f>
         <v>45222</v>
       </c>
-      <c r="AJ4" s="139"/>
-      <c r="AK4" s="139"/>
-      <c r="AL4" s="139"/>
-      <c r="AM4" s="139"/>
-      <c r="AN4" s="139"/>
-      <c r="AO4" s="140"/>
-      <c r="AP4" s="138">
+      <c r="AJ4" s="143"/>
+      <c r="AK4" s="143"/>
+      <c r="AL4" s="143"/>
+      <c r="AM4" s="143"/>
+      <c r="AN4" s="143"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="142">
         <f>AP5</f>
         <v>45229</v>
       </c>
-      <c r="AQ4" s="139"/>
-      <c r="AR4" s="139"/>
-      <c r="AS4" s="139"/>
-      <c r="AT4" s="139"/>
-      <c r="AU4" s="139"/>
-      <c r="AV4" s="140"/>
-      <c r="AW4" s="138">
+      <c r="AQ4" s="143"/>
+      <c r="AR4" s="143"/>
+      <c r="AS4" s="143"/>
+      <c r="AT4" s="143"/>
+      <c r="AU4" s="143"/>
+      <c r="AV4" s="144"/>
+      <c r="AW4" s="142">
         <f>AW5</f>
         <v>45236</v>
       </c>
-      <c r="AX4" s="139"/>
-      <c r="AY4" s="139"/>
-      <c r="AZ4" s="139"/>
-      <c r="BA4" s="139"/>
-      <c r="BB4" s="139"/>
-      <c r="BC4" s="140"/>
-      <c r="BD4" s="138">
+      <c r="AX4" s="143"/>
+      <c r="AY4" s="143"/>
+      <c r="AZ4" s="143"/>
+      <c r="BA4" s="143"/>
+      <c r="BB4" s="143"/>
+      <c r="BC4" s="144"/>
+      <c r="BD4" s="142">
         <f>BD5</f>
         <v>45243</v>
       </c>
-      <c r="BE4" s="139"/>
-      <c r="BF4" s="139"/>
-      <c r="BG4" s="139"/>
-      <c r="BH4" s="139"/>
-      <c r="BI4" s="139"/>
-      <c r="BJ4" s="140"/>
-      <c r="BK4" s="138">
+      <c r="BE4" s="143"/>
+      <c r="BF4" s="143"/>
+      <c r="BG4" s="143"/>
+      <c r="BH4" s="143"/>
+      <c r="BI4" s="143"/>
+      <c r="BJ4" s="144"/>
+      <c r="BK4" s="142">
         <f>BK5</f>
         <v>45250</v>
       </c>
-      <c r="BL4" s="139"/>
-      <c r="BM4" s="139"/>
-      <c r="BN4" s="139"/>
-      <c r="BO4" s="139"/>
-      <c r="BP4" s="139"/>
-      <c r="BQ4" s="140"/>
-      <c r="BR4" s="138">
+      <c r="BL4" s="143"/>
+      <c r="BM4" s="143"/>
+      <c r="BN4" s="143"/>
+      <c r="BO4" s="143"/>
+      <c r="BP4" s="143"/>
+      <c r="BQ4" s="144"/>
+      <c r="BR4" s="142">
         <f>BR5</f>
         <v>45257</v>
       </c>
-      <c r="BS4" s="139"/>
-      <c r="BT4" s="139"/>
-      <c r="BU4" s="139"/>
-      <c r="BV4" s="139"/>
-      <c r="BW4" s="139"/>
-      <c r="BX4" s="140"/>
-      <c r="BY4" s="138">
+      <c r="BS4" s="143"/>
+      <c r="BT4" s="143"/>
+      <c r="BU4" s="143"/>
+      <c r="BV4" s="143"/>
+      <c r="BW4" s="143"/>
+      <c r="BX4" s="144"/>
+      <c r="BY4" s="142">
         <f>BY5</f>
         <v>45264</v>
       </c>
-      <c r="BZ4" s="139"/>
-      <c r="CA4" s="139"/>
-      <c r="CB4" s="139"/>
-      <c r="CC4" s="139"/>
-      <c r="CD4" s="139"/>
-      <c r="CE4" s="140"/>
+      <c r="BZ4" s="143"/>
+      <c r="CA4" s="143"/>
+      <c r="CB4" s="143"/>
+      <c r="CC4" s="143"/>
+      <c r="CD4" s="143"/>
+      <c r="CE4" s="144"/>
     </row>
     <row r="5" spans="1:83" ht="25.5" customHeight="1" thickBot="1">
       <c r="A5" s="1"/>
@@ -2311,7 +2323,7 @@
       <c r="E5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="137"/>
+      <c r="F5" s="148"/>
       <c r="G5" s="22">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2</f>
         <v>45194</v>
@@ -2715,83 +2727,83 @@
       <c r="D7" s="31"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
-      <c r="AB7" s="126"/>
-      <c r="AC7" s="126"/>
-      <c r="AD7" s="126"/>
-      <c r="AE7" s="126"/>
-      <c r="AF7" s="126"/>
-      <c r="AG7" s="126"/>
-      <c r="AH7" s="126"/>
-      <c r="AI7" s="126"/>
-      <c r="AJ7" s="126"/>
-      <c r="AK7" s="126"/>
-      <c r="AL7" s="126"/>
-      <c r="AM7" s="126"/>
-      <c r="AN7" s="126"/>
-      <c r="AO7" s="126"/>
-      <c r="AP7" s="126"/>
-      <c r="AQ7" s="126"/>
-      <c r="AR7" s="126"/>
-      <c r="AS7" s="126"/>
-      <c r="AT7" s="126"/>
-      <c r="AU7" s="126"/>
-      <c r="AV7" s="126"/>
-      <c r="AW7" s="126"/>
-      <c r="AX7" s="126"/>
-      <c r="AY7" s="126"/>
-      <c r="AZ7" s="126"/>
-      <c r="BA7" s="126"/>
-      <c r="BB7" s="126"/>
-      <c r="BC7" s="126"/>
-      <c r="BD7" s="126"/>
-      <c r="BE7" s="126"/>
-      <c r="BF7" s="126"/>
-      <c r="BG7" s="126"/>
-      <c r="BH7" s="126"/>
-      <c r="BI7" s="126"/>
-      <c r="BJ7" s="126"/>
-      <c r="BK7" s="126"/>
-      <c r="BL7" s="126"/>
-      <c r="BM7" s="126"/>
-      <c r="BN7" s="126"/>
-      <c r="BO7" s="126"/>
-      <c r="BP7" s="126"/>
-      <c r="BQ7" s="126"/>
-      <c r="BR7" s="126"/>
-      <c r="BS7" s="126"/>
-      <c r="BT7" s="126"/>
-      <c r="BU7" s="126"/>
-      <c r="BV7" s="126"/>
-      <c r="BW7" s="126"/>
-      <c r="BX7" s="126"/>
-      <c r="BY7" s="126"/>
-      <c r="BZ7" s="126"/>
-      <c r="CA7" s="126"/>
-      <c r="CB7" s="126"/>
-      <c r="CC7" s="126"/>
-      <c r="CD7" s="126"/>
-      <c r="CE7" s="127"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="131"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="131"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="131"/>
+      <c r="U7" s="131"/>
+      <c r="V7" s="131"/>
+      <c r="W7" s="131"/>
+      <c r="X7" s="131"/>
+      <c r="Y7" s="131"/>
+      <c r="Z7" s="131"/>
+      <c r="AA7" s="131"/>
+      <c r="AB7" s="131"/>
+      <c r="AC7" s="131"/>
+      <c r="AD7" s="131"/>
+      <c r="AE7" s="131"/>
+      <c r="AF7" s="131"/>
+      <c r="AG7" s="131"/>
+      <c r="AH7" s="131"/>
+      <c r="AI7" s="131"/>
+      <c r="AJ7" s="131"/>
+      <c r="AK7" s="131"/>
+      <c r="AL7" s="131"/>
+      <c r="AM7" s="131"/>
+      <c r="AN7" s="131"/>
+      <c r="AO7" s="131"/>
+      <c r="AP7" s="131"/>
+      <c r="AQ7" s="131"/>
+      <c r="AR7" s="131"/>
+      <c r="AS7" s="131"/>
+      <c r="AT7" s="131"/>
+      <c r="AU7" s="131"/>
+      <c r="AV7" s="131"/>
+      <c r="AW7" s="131"/>
+      <c r="AX7" s="131"/>
+      <c r="AY7" s="131"/>
+      <c r="AZ7" s="131"/>
+      <c r="BA7" s="131"/>
+      <c r="BB7" s="131"/>
+      <c r="BC7" s="131"/>
+      <c r="BD7" s="131"/>
+      <c r="BE7" s="131"/>
+      <c r="BF7" s="131"/>
+      <c r="BG7" s="131"/>
+      <c r="BH7" s="131"/>
+      <c r="BI7" s="131"/>
+      <c r="BJ7" s="131"/>
+      <c r="BK7" s="131"/>
+      <c r="BL7" s="131"/>
+      <c r="BM7" s="131"/>
+      <c r="BN7" s="131"/>
+      <c r="BO7" s="131"/>
+      <c r="BP7" s="131"/>
+      <c r="BQ7" s="131"/>
+      <c r="BR7" s="131"/>
+      <c r="BS7" s="131"/>
+      <c r="BT7" s="131"/>
+      <c r="BU7" s="131"/>
+      <c r="BV7" s="131"/>
+      <c r="BW7" s="131"/>
+      <c r="BX7" s="131"/>
+      <c r="BY7" s="131"/>
+      <c r="BZ7" s="131"/>
+      <c r="CA7" s="131"/>
+      <c r="CB7" s="131"/>
+      <c r="CC7" s="131"/>
+      <c r="CD7" s="131"/>
+      <c r="CE7" s="132"/>
     </row>
     <row r="8" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
@@ -2811,9 +2823,9 @@
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
       <c r="I8" s="45"/>
-      <c r="J8" s="142"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="106"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="114"/>
+      <c r="L8" s="105"/>
       <c r="M8" s="40"/>
       <c r="N8" s="38"/>
       <c r="O8" s="38"/>
@@ -2904,9 +2916,9 @@
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
       <c r="I9" s="45"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="117"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="114"/>
       <c r="M9" s="46"/>
       <c r="N9" s="38"/>
       <c r="O9" s="38"/>
@@ -2997,10 +3009,10 @@
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="117"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="140"/>
+      <c r="M10" s="114"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
       <c r="P10" s="38"/>
@@ -3091,8 +3103,8 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
       <c r="J11" s="45"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="144"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="141"/>
       <c r="M11" s="48"/>
       <c r="N11" s="41"/>
       <c r="O11" s="41"/>
@@ -3187,10 +3199,10 @@
       <c r="K12" s="47"/>
       <c r="L12" s="39"/>
       <c r="M12" s="49"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="117"/>
+      <c r="N12" s="112"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="113"/>
+      <c r="Q12" s="114"/>
       <c r="R12" s="38"/>
       <c r="S12" s="40"/>
       <c r="T12" s="40"/>
@@ -3278,11 +3290,11 @@
       <c r="I13" s="38"/>
       <c r="J13" s="41"/>
       <c r="K13" s="50"/>
-      <c r="L13" s="145"/>
-      <c r="M13" s="114"/>
-      <c r="N13" s="141"/>
-      <c r="O13" s="141"/>
-      <c r="P13" s="146"/>
+      <c r="L13" s="136"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="137"/>
+      <c r="O13" s="137"/>
+      <c r="P13" s="138"/>
       <c r="Q13" s="55"/>
       <c r="R13" s="41"/>
       <c r="S13" s="40"/>
@@ -3373,11 +3385,11 @@
       <c r="K14" s="38"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="108"/>
-      <c r="P14" s="108"/>
-      <c r="Q14" s="108"/>
-      <c r="R14" s="109"/>
+      <c r="N14" s="123"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="108"/>
       <c r="S14" s="46"/>
       <c r="T14" s="39"/>
       <c r="U14" s="41"/>
@@ -3468,15 +3480,15 @@
       <c r="M15" s="40"/>
       <c r="N15" s="47"/>
       <c r="O15" s="52"/>
-      <c r="P15" s="147"/>
-      <c r="Q15" s="108"/>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="119"/>
-      <c r="U15" s="102"/>
-      <c r="V15" s="102"/>
-      <c r="W15" s="100"/>
-      <c r="X15" s="100"/>
+      <c r="P15" s="106"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="111"/>
+      <c r="U15" s="101"/>
+      <c r="V15" s="101"/>
+      <c r="W15" s="99"/>
+      <c r="X15" s="99"/>
       <c r="Y15" s="42"/>
       <c r="Z15" s="43"/>
       <c r="AA15" s="43"/>
@@ -3565,11 +3577,11 @@
       <c r="Q16" s="47"/>
       <c r="R16" s="47"/>
       <c r="S16" s="51"/>
-      <c r="T16" s="148"/>
-      <c r="U16" s="116"/>
-      <c r="V16" s="116"/>
-      <c r="W16" s="116"/>
-      <c r="X16" s="117"/>
+      <c r="T16" s="124"/>
+      <c r="U16" s="113"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="114"/>
       <c r="Y16" s="41"/>
       <c r="Z16" s="53"/>
       <c r="AA16" s="43"/>
@@ -3658,13 +3670,13 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
       <c r="S17" s="40"/>
-      <c r="T17" s="99"/>
+      <c r="T17" s="98"/>
       <c r="U17" s="55"/>
       <c r="V17" s="55"/>
       <c r="W17" s="56"/>
-      <c r="X17" s="149"/>
-      <c r="Y17" s="108"/>
-      <c r="Z17" s="109"/>
+      <c r="X17" s="139"/>
+      <c r="Y17" s="107"/>
+      <c r="Z17" s="108"/>
       <c r="AA17" s="43"/>
       <c r="AB17" s="28"/>
       <c r="AC17" s="28"/>
@@ -3751,13 +3763,13 @@
       <c r="Q18" s="38"/>
       <c r="R18" s="38"/>
       <c r="S18" s="51"/>
-      <c r="T18" s="133"/>
-      <c r="U18" s="108"/>
-      <c r="V18" s="108"/>
-      <c r="W18" s="108"/>
-      <c r="X18" s="108"/>
-      <c r="Y18" s="108"/>
-      <c r="Z18" s="109"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="107"/>
+      <c r="V18" s="107"/>
+      <c r="W18" s="107"/>
+      <c r="X18" s="107"/>
+      <c r="Y18" s="107"/>
+      <c r="Z18" s="108"/>
       <c r="AA18" s="43"/>
       <c r="AB18" s="28"/>
       <c r="AC18" s="28"/>
@@ -3847,12 +3859,12 @@
       <c r="S19" s="40"/>
       <c r="T19" s="40"/>
       <c r="U19" s="57"/>
-      <c r="V19" s="150"/>
-      <c r="W19" s="151"/>
-      <c r="X19" s="151"/>
-      <c r="Y19" s="151"/>
-      <c r="Z19" s="151"/>
-      <c r="AA19" s="152"/>
+      <c r="V19" s="133"/>
+      <c r="W19" s="116"/>
+      <c r="X19" s="116"/>
+      <c r="Y19" s="116"/>
+      <c r="Z19" s="116"/>
+      <c r="AA19" s="134"/>
       <c r="AB19" s="28"/>
       <c r="AC19" s="28"/>
       <c r="AD19" s="28"/>
@@ -3919,83 +3931,83 @@
       <c r="D20" s="60"/>
       <c r="E20" s="61"/>
       <c r="F20" s="37"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="126"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="126"/>
-      <c r="K20" s="126"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="126"/>
-      <c r="P20" s="126"/>
-      <c r="Q20" s="126"/>
-      <c r="R20" s="126"/>
-      <c r="S20" s="126"/>
-      <c r="T20" s="126"/>
-      <c r="U20" s="126"/>
-      <c r="V20" s="126"/>
-      <c r="W20" s="126"/>
-      <c r="X20" s="126"/>
-      <c r="Y20" s="126"/>
-      <c r="Z20" s="126"/>
-      <c r="AA20" s="126"/>
-      <c r="AB20" s="126"/>
-      <c r="AC20" s="126"/>
-      <c r="AD20" s="126"/>
-      <c r="AE20" s="126"/>
-      <c r="AF20" s="126"/>
-      <c r="AG20" s="126"/>
-      <c r="AH20" s="126"/>
-      <c r="AI20" s="126"/>
-      <c r="AJ20" s="126"/>
-      <c r="AK20" s="126"/>
-      <c r="AL20" s="126"/>
-      <c r="AM20" s="126"/>
-      <c r="AN20" s="126"/>
-      <c r="AO20" s="126"/>
-      <c r="AP20" s="126"/>
-      <c r="AQ20" s="126"/>
-      <c r="AR20" s="126"/>
-      <c r="AS20" s="126"/>
-      <c r="AT20" s="126"/>
-      <c r="AU20" s="126"/>
-      <c r="AV20" s="126"/>
-      <c r="AW20" s="126"/>
-      <c r="AX20" s="126"/>
-      <c r="AY20" s="126"/>
-      <c r="AZ20" s="126"/>
-      <c r="BA20" s="126"/>
-      <c r="BB20" s="126"/>
-      <c r="BC20" s="126"/>
-      <c r="BD20" s="126"/>
-      <c r="BE20" s="126"/>
-      <c r="BF20" s="126"/>
-      <c r="BG20" s="126"/>
-      <c r="BH20" s="126"/>
-      <c r="BI20" s="126"/>
-      <c r="BJ20" s="126"/>
-      <c r="BK20" s="126"/>
-      <c r="BL20" s="126"/>
-      <c r="BM20" s="126"/>
-      <c r="BN20" s="126"/>
-      <c r="BO20" s="126"/>
-      <c r="BP20" s="126"/>
-      <c r="BQ20" s="126"/>
-      <c r="BR20" s="126"/>
-      <c r="BS20" s="126"/>
-      <c r="BT20" s="126"/>
-      <c r="BU20" s="126"/>
-      <c r="BV20" s="126"/>
-      <c r="BW20" s="126"/>
-      <c r="BX20" s="126"/>
-      <c r="BY20" s="126"/>
-      <c r="BZ20" s="126"/>
-      <c r="CA20" s="126"/>
-      <c r="CB20" s="126"/>
-      <c r="CC20" s="126"/>
-      <c r="CD20" s="126"/>
-      <c r="CE20" s="127"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="131"/>
+      <c r="I20" s="131"/>
+      <c r="J20" s="131"/>
+      <c r="K20" s="131"/>
+      <c r="L20" s="131"/>
+      <c r="M20" s="131"/>
+      <c r="N20" s="131"/>
+      <c r="O20" s="131"/>
+      <c r="P20" s="131"/>
+      <c r="Q20" s="131"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
+      <c r="U20" s="131"/>
+      <c r="V20" s="131"/>
+      <c r="W20" s="131"/>
+      <c r="X20" s="131"/>
+      <c r="Y20" s="131"/>
+      <c r="Z20" s="131"/>
+      <c r="AA20" s="131"/>
+      <c r="AB20" s="131"/>
+      <c r="AC20" s="131"/>
+      <c r="AD20" s="131"/>
+      <c r="AE20" s="131"/>
+      <c r="AF20" s="131"/>
+      <c r="AG20" s="131"/>
+      <c r="AH20" s="131"/>
+      <c r="AI20" s="131"/>
+      <c r="AJ20" s="131"/>
+      <c r="AK20" s="131"/>
+      <c r="AL20" s="131"/>
+      <c r="AM20" s="131"/>
+      <c r="AN20" s="131"/>
+      <c r="AO20" s="131"/>
+      <c r="AP20" s="131"/>
+      <c r="AQ20" s="131"/>
+      <c r="AR20" s="131"/>
+      <c r="AS20" s="131"/>
+      <c r="AT20" s="131"/>
+      <c r="AU20" s="131"/>
+      <c r="AV20" s="131"/>
+      <c r="AW20" s="131"/>
+      <c r="AX20" s="131"/>
+      <c r="AY20" s="131"/>
+      <c r="AZ20" s="131"/>
+      <c r="BA20" s="131"/>
+      <c r="BB20" s="131"/>
+      <c r="BC20" s="131"/>
+      <c r="BD20" s="131"/>
+      <c r="BE20" s="131"/>
+      <c r="BF20" s="131"/>
+      <c r="BG20" s="131"/>
+      <c r="BH20" s="131"/>
+      <c r="BI20" s="131"/>
+      <c r="BJ20" s="131"/>
+      <c r="BK20" s="131"/>
+      <c r="BL20" s="131"/>
+      <c r="BM20" s="131"/>
+      <c r="BN20" s="131"/>
+      <c r="BO20" s="131"/>
+      <c r="BP20" s="131"/>
+      <c r="BQ20" s="131"/>
+      <c r="BR20" s="131"/>
+      <c r="BS20" s="131"/>
+      <c r="BT20" s="131"/>
+      <c r="BU20" s="131"/>
+      <c r="BV20" s="131"/>
+      <c r="BW20" s="131"/>
+      <c r="BX20" s="131"/>
+      <c r="BY20" s="131"/>
+      <c r="BZ20" s="131"/>
+      <c r="CA20" s="131"/>
+      <c r="CB20" s="131"/>
+      <c r="CC20" s="131"/>
+      <c r="CD20" s="131"/>
+      <c r="CE20" s="132"/>
     </row>
     <row r="21" spans="1:83" ht="15" customHeight="1">
       <c r="A21" s="1"/>
@@ -4032,14 +4044,14 @@
       <c r="X21" s="28"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="65"/>
-      <c r="AA21" s="147"/>
-      <c r="AB21" s="108"/>
-      <c r="AC21" s="108"/>
-      <c r="AD21" s="108"/>
-      <c r="AE21" s="108"/>
-      <c r="AF21" s="108"/>
-      <c r="AG21" s="108"/>
-      <c r="AH21" s="109"/>
+      <c r="AA21" s="106"/>
+      <c r="AB21" s="107"/>
+      <c r="AC21" s="107"/>
+      <c r="AD21" s="107"/>
+      <c r="AE21" s="107"/>
+      <c r="AF21" s="107"/>
+      <c r="AG21" s="107"/>
+      <c r="AH21" s="108"/>
       <c r="AI21" s="38"/>
       <c r="AJ21" s="28"/>
       <c r="AK21" s="28"/>
@@ -4126,12 +4138,12 @@
       <c r="Y22" s="28"/>
       <c r="Z22" s="44"/>
       <c r="AA22" s="51"/>
-      <c r="AB22" s="128"/>
-      <c r="AC22" s="108"/>
-      <c r="AD22" s="108"/>
-      <c r="AE22" s="108"/>
-      <c r="AF22" s="108"/>
-      <c r="AG22" s="109"/>
+      <c r="AB22" s="135"/>
+      <c r="AC22" s="107"/>
+      <c r="AD22" s="107"/>
+      <c r="AE22" s="107"/>
+      <c r="AF22" s="107"/>
+      <c r="AG22" s="108"/>
       <c r="AH22" s="46"/>
       <c r="AI22" s="42"/>
       <c r="AJ22" s="42"/>
@@ -4220,15 +4232,15 @@
       <c r="Z23" s="44"/>
       <c r="AA23" s="44"/>
       <c r="AB23" s="66"/>
-      <c r="AC23" s="110"/>
-      <c r="AD23" s="114"/>
-      <c r="AE23" s="114"/>
-      <c r="AF23" s="114"/>
-      <c r="AG23" s="114"/>
-      <c r="AH23" s="114"/>
-      <c r="AI23" s="114"/>
-      <c r="AJ23" s="114"/>
-      <c r="AK23" s="109"/>
+      <c r="AC23" s="123"/>
+      <c r="AD23" s="110"/>
+      <c r="AE23" s="110"/>
+      <c r="AF23" s="110"/>
+      <c r="AG23" s="110"/>
+      <c r="AH23" s="110"/>
+      <c r="AI23" s="110"/>
+      <c r="AJ23" s="110"/>
+      <c r="AK23" s="108"/>
       <c r="AL23" s="38"/>
       <c r="AM23" s="28"/>
       <c r="AN23" s="44"/>
@@ -4314,14 +4326,14 @@
       <c r="AA24" s="44"/>
       <c r="AB24" s="28"/>
       <c r="AC24" s="66"/>
-      <c r="AD24" s="148"/>
-      <c r="AE24" s="116"/>
-      <c r="AF24" s="116"/>
-      <c r="AG24" s="116"/>
-      <c r="AH24" s="116"/>
-      <c r="AI24" s="116"/>
-      <c r="AJ24" s="117"/>
-      <c r="AK24" s="104"/>
+      <c r="AD24" s="124"/>
+      <c r="AE24" s="113"/>
+      <c r="AF24" s="113"/>
+      <c r="AG24" s="113"/>
+      <c r="AH24" s="113"/>
+      <c r="AI24" s="113"/>
+      <c r="AJ24" s="114"/>
+      <c r="AK24" s="103"/>
       <c r="AL24" s="28"/>
       <c r="AM24" s="28"/>
       <c r="AN24" s="44"/>
@@ -4412,9 +4424,9 @@
       <c r="AF25" s="57"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="66"/>
-      <c r="AI25" s="153"/>
-      <c r="AJ25" s="151"/>
-      <c r="AK25" s="109"/>
+      <c r="AI25" s="125"/>
+      <c r="AJ25" s="116"/>
+      <c r="AK25" s="108"/>
       <c r="AL25" s="38"/>
       <c r="AM25" s="28"/>
       <c r="AN25" s="44"/>
@@ -4501,12 +4513,12 @@
       <c r="AB26" s="28"/>
       <c r="AC26" s="28"/>
       <c r="AD26" s="28"/>
-      <c r="AE26" s="107"/>
-      <c r="AF26" s="108"/>
-      <c r="AG26" s="108"/>
-      <c r="AH26" s="108"/>
-      <c r="AI26" s="108"/>
-      <c r="AJ26" s="109"/>
+      <c r="AE26" s="126"/>
+      <c r="AF26" s="107"/>
+      <c r="AG26" s="107"/>
+      <c r="AH26" s="107"/>
+      <c r="AI26" s="107"/>
+      <c r="AJ26" s="108"/>
       <c r="AK26" s="55"/>
       <c r="AL26" s="28"/>
       <c r="AM26" s="28"/>
@@ -4593,14 +4605,14 @@
       <c r="AA27" s="44"/>
       <c r="AB27" s="28"/>
       <c r="AC27" s="67"/>
-      <c r="AD27" s="133"/>
-      <c r="AE27" s="108"/>
-      <c r="AF27" s="108"/>
-      <c r="AG27" s="114"/>
-      <c r="AH27" s="114"/>
-      <c r="AI27" s="114"/>
-      <c r="AJ27" s="114"/>
-      <c r="AK27" s="119"/>
+      <c r="AD27" s="119"/>
+      <c r="AE27" s="107"/>
+      <c r="AF27" s="107"/>
+      <c r="AG27" s="110"/>
+      <c r="AH27" s="110"/>
+      <c r="AI27" s="110"/>
+      <c r="AJ27" s="110"/>
+      <c r="AK27" s="111"/>
       <c r="AL27" s="38"/>
       <c r="AM27" s="28"/>
       <c r="AN27" s="44"/>
@@ -4662,7 +4674,7 @@
       <c r="E28" s="64">
         <v>45225</v>
       </c>
-      <c r="F28" s="154"/>
+      <c r="F28" s="127"/>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -4689,11 +4701,11 @@
       <c r="AD28" s="57"/>
       <c r="AE28" s="57"/>
       <c r="AF28" s="66"/>
-      <c r="AG28" s="142"/>
-      <c r="AH28" s="116"/>
-      <c r="AI28" s="116"/>
-      <c r="AJ28" s="116"/>
-      <c r="AK28" s="117"/>
+      <c r="AG28" s="129"/>
+      <c r="AH28" s="113"/>
+      <c r="AI28" s="113"/>
+      <c r="AJ28" s="113"/>
+      <c r="AK28" s="114"/>
       <c r="AL28" s="38"/>
       <c r="AM28" s="28"/>
       <c r="AN28" s="44"/>
@@ -4741,7 +4753,7 @@
       <c r="CD28" s="44"/>
       <c r="CE28" s="44"/>
     </row>
-    <row r="29" spans="1:83" ht="15" customHeight="1">
+    <row r="29" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A29" s="1"/>
       <c r="B29" s="68" t="s">
         <v>37</v>
@@ -4749,86 +4761,86 @@
       <c r="C29" s="69"/>
       <c r="D29" s="70"/>
       <c r="E29" s="71"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="126"/>
-      <c r="I29" s="126"/>
-      <c r="J29" s="126"/>
-      <c r="K29" s="126"/>
-      <c r="L29" s="126"/>
-      <c r="M29" s="126"/>
-      <c r="N29" s="126"/>
-      <c r="O29" s="126"/>
-      <c r="P29" s="126"/>
-      <c r="Q29" s="126"/>
-      <c r="R29" s="126"/>
-      <c r="S29" s="126"/>
-      <c r="T29" s="126"/>
-      <c r="U29" s="126"/>
-      <c r="V29" s="126"/>
-      <c r="W29" s="126"/>
-      <c r="X29" s="126"/>
-      <c r="Y29" s="126"/>
-      <c r="Z29" s="126"/>
-      <c r="AA29" s="126"/>
-      <c r="AB29" s="126"/>
-      <c r="AC29" s="126"/>
-      <c r="AD29" s="126"/>
-      <c r="AE29" s="126"/>
-      <c r="AF29" s="126"/>
-      <c r="AG29" s="126"/>
-      <c r="AH29" s="126"/>
-      <c r="AI29" s="126"/>
-      <c r="AJ29" s="126"/>
-      <c r="AK29" s="126"/>
-      <c r="AL29" s="126"/>
-      <c r="AM29" s="126"/>
-      <c r="AN29" s="126"/>
-      <c r="AO29" s="126"/>
-      <c r="AP29" s="126"/>
-      <c r="AQ29" s="126"/>
-      <c r="AR29" s="126"/>
-      <c r="AS29" s="126"/>
-      <c r="AT29" s="126"/>
-      <c r="AU29" s="126"/>
-      <c r="AV29" s="126"/>
-      <c r="AW29" s="126"/>
-      <c r="AX29" s="126"/>
-      <c r="AY29" s="126"/>
-      <c r="AZ29" s="126"/>
-      <c r="BA29" s="126"/>
-      <c r="BB29" s="126"/>
-      <c r="BC29" s="126"/>
-      <c r="BD29" s="126"/>
-      <c r="BE29" s="126"/>
-      <c r="BF29" s="126"/>
-      <c r="BG29" s="126"/>
-      <c r="BH29" s="126"/>
-      <c r="BI29" s="126"/>
-      <c r="BJ29" s="126"/>
-      <c r="BK29" s="126"/>
-      <c r="BL29" s="126"/>
-      <c r="BM29" s="126"/>
-      <c r="BN29" s="126"/>
-      <c r="BO29" s="126"/>
-      <c r="BP29" s="126"/>
-      <c r="BQ29" s="126"/>
-      <c r="BR29" s="126"/>
-      <c r="BS29" s="126"/>
-      <c r="BT29" s="126"/>
-      <c r="BU29" s="126"/>
-      <c r="BV29" s="126"/>
-      <c r="BW29" s="126"/>
-      <c r="BX29" s="126"/>
-      <c r="BY29" s="126"/>
-      <c r="BZ29" s="126"/>
-      <c r="CA29" s="126"/>
-      <c r="CB29" s="126"/>
-      <c r="CC29" s="126"/>
-      <c r="CD29" s="126"/>
-      <c r="CE29" s="127"/>
-    </row>
-    <row r="30" spans="1:83" ht="15" customHeight="1">
+      <c r="F29" s="128"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
+      <c r="Q29" s="131"/>
+      <c r="R29" s="131"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="131"/>
+      <c r="U29" s="131"/>
+      <c r="V29" s="131"/>
+      <c r="W29" s="131"/>
+      <c r="X29" s="131"/>
+      <c r="Y29" s="131"/>
+      <c r="Z29" s="131"/>
+      <c r="AA29" s="131"/>
+      <c r="AB29" s="131"/>
+      <c r="AC29" s="131"/>
+      <c r="AD29" s="131"/>
+      <c r="AE29" s="131"/>
+      <c r="AF29" s="131"/>
+      <c r="AG29" s="131"/>
+      <c r="AH29" s="131"/>
+      <c r="AI29" s="131"/>
+      <c r="AJ29" s="131"/>
+      <c r="AK29" s="131"/>
+      <c r="AL29" s="131"/>
+      <c r="AM29" s="131"/>
+      <c r="AN29" s="131"/>
+      <c r="AO29" s="131"/>
+      <c r="AP29" s="131"/>
+      <c r="AQ29" s="131"/>
+      <c r="AR29" s="131"/>
+      <c r="AS29" s="131"/>
+      <c r="AT29" s="131"/>
+      <c r="AU29" s="131"/>
+      <c r="AV29" s="131"/>
+      <c r="AW29" s="131"/>
+      <c r="AX29" s="131"/>
+      <c r="AY29" s="131"/>
+      <c r="AZ29" s="131"/>
+      <c r="BA29" s="131"/>
+      <c r="BB29" s="131"/>
+      <c r="BC29" s="131"/>
+      <c r="BD29" s="131"/>
+      <c r="BE29" s="131"/>
+      <c r="BF29" s="131"/>
+      <c r="BG29" s="131"/>
+      <c r="BH29" s="131"/>
+      <c r="BI29" s="131"/>
+      <c r="BJ29" s="131"/>
+      <c r="BK29" s="131"/>
+      <c r="BL29" s="131"/>
+      <c r="BM29" s="131"/>
+      <c r="BN29" s="131"/>
+      <c r="BO29" s="131"/>
+      <c r="BP29" s="131"/>
+      <c r="BQ29" s="131"/>
+      <c r="BR29" s="131"/>
+      <c r="BS29" s="131"/>
+      <c r="BT29" s="131"/>
+      <c r="BU29" s="131"/>
+      <c r="BV29" s="131"/>
+      <c r="BW29" s="131"/>
+      <c r="BX29" s="131"/>
+      <c r="BY29" s="131"/>
+      <c r="BZ29" s="131"/>
+      <c r="CA29" s="131"/>
+      <c r="CB29" s="131"/>
+      <c r="CC29" s="131"/>
+      <c r="CD29" s="131"/>
+      <c r="CE29" s="132"/>
+    </row>
+    <row r="30" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A30" s="1"/>
       <c r="B30" s="72" t="s">
         <v>38</v>
@@ -4877,17 +4889,17 @@
       <c r="AL30" s="42"/>
       <c r="AM30" s="41"/>
       <c r="AN30" s="75"/>
-      <c r="AO30" s="76"/>
-      <c r="AP30" s="113"/>
-      <c r="AQ30" s="119"/>
-      <c r="AR30" s="41"/>
-      <c r="AS30" s="42"/>
-      <c r="AT30" s="42"/>
+      <c r="AO30" s="162"/>
+      <c r="AP30" s="118"/>
+      <c r="AQ30" s="111"/>
+      <c r="AR30" s="101"/>
+      <c r="AS30" s="99"/>
+      <c r="AT30" s="99"/>
       <c r="AU30" s="75"/>
       <c r="AV30" s="75"/>
-      <c r="AW30" s="28"/>
-      <c r="AX30" s="28"/>
-      <c r="AY30" s="28"/>
+      <c r="AW30" s="99"/>
+      <c r="AX30" s="99"/>
+      <c r="AY30" s="99"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="28"/>
       <c r="BB30" s="44"/>
@@ -4921,10 +4933,10 @@
       <c r="CD30" s="44"/>
       <c r="CE30" s="44"/>
     </row>
-    <row r="31" spans="1:83" ht="15" customHeight="1">
+    <row r="31" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
       <c r="B31" s="72" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>3</v>
@@ -4933,9 +4945,9 @@
         <v>45227</v>
       </c>
       <c r="E31" s="74">
-        <v>45232</v>
-      </c>
-      <c r="F31" s="77"/>
+        <v>45238</v>
+      </c>
+      <c r="F31" s="76"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -4969,19 +4981,19 @@
       <c r="AK31" s="28"/>
       <c r="AL31" s="28"/>
       <c r="AM31" s="67"/>
-      <c r="AN31" s="133"/>
-      <c r="AO31" s="108"/>
-      <c r="AP31" s="108"/>
-      <c r="AQ31" s="108"/>
-      <c r="AR31" s="108"/>
-      <c r="AS31" s="112"/>
-      <c r="AT31" s="42"/>
-      <c r="AU31" s="75"/>
-      <c r="AV31" s="75"/>
-      <c r="AW31" s="28"/>
-      <c r="AX31" s="28"/>
-      <c r="AY31" s="28"/>
-      <c r="AZ31" s="28"/>
+      <c r="AN31" s="112"/>
+      <c r="AO31" s="164"/>
+      <c r="AP31" s="164"/>
+      <c r="AQ31" s="164"/>
+      <c r="AR31" s="164"/>
+      <c r="AS31" s="164"/>
+      <c r="AT31" s="164"/>
+      <c r="AU31" s="164"/>
+      <c r="AV31" s="164"/>
+      <c r="AW31" s="164"/>
+      <c r="AX31" s="164"/>
+      <c r="AY31" s="165"/>
+      <c r="AZ31" s="161"/>
       <c r="BA31" s="28"/>
       <c r="BB31" s="75"/>
       <c r="BC31" s="75"/>
@@ -5014,12 +5026,12 @@
       <c r="CD31" s="44"/>
       <c r="CE31" s="44"/>
     </row>
-    <row r="32" spans="1:83" ht="15" customHeight="1">
+    <row r="32" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="73" t="s">
         <v>8</v>
@@ -5059,23 +5071,23 @@
       <c r="AF32" s="28"/>
       <c r="AG32" s="44"/>
       <c r="AH32" s="65"/>
-      <c r="AI32" s="130"/>
-      <c r="AJ32" s="108"/>
-      <c r="AK32" s="108"/>
-      <c r="AL32" s="108"/>
-      <c r="AM32" s="108"/>
-      <c r="AN32" s="109"/>
-      <c r="AO32" s="46"/>
+      <c r="AI32" s="109"/>
+      <c r="AJ32" s="107"/>
+      <c r="AK32" s="107"/>
+      <c r="AL32" s="107"/>
+      <c r="AM32" s="107"/>
+      <c r="AN32" s="141"/>
+      <c r="AO32" s="105"/>
       <c r="AP32" s="57"/>
       <c r="AQ32" s="57"/>
       <c r="AR32" s="57"/>
       <c r="AS32" s="57"/>
-      <c r="AT32" s="42"/>
-      <c r="AU32" s="40"/>
-      <c r="AV32" s="40"/>
-      <c r="AW32" s="28"/>
-      <c r="AX32" s="28"/>
-      <c r="AY32" s="28"/>
+      <c r="AT32" s="78"/>
+      <c r="AU32" s="163"/>
+      <c r="AV32" s="163"/>
+      <c r="AW32" s="57"/>
+      <c r="AX32" s="57"/>
+      <c r="AY32" s="57"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="28"/>
       <c r="BB32" s="44"/>
@@ -5109,10 +5121,10 @@
       <c r="CD32" s="44"/>
       <c r="CE32" s="44"/>
     </row>
-    <row r="33" spans="1:83" ht="15" customHeight="1">
+    <row r="33" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A33" s="1"/>
       <c r="B33" s="72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="73" t="s">
         <v>5</v>
@@ -5123,7 +5135,7 @@
       <c r="E33" s="74">
         <v>45228</v>
       </c>
-      <c r="F33" s="77"/>
+      <c r="F33" s="76"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -5153,12 +5165,12 @@
       <c r="AG33" s="44"/>
       <c r="AH33" s="44"/>
       <c r="AI33" s="66"/>
-      <c r="AJ33" s="156"/>
-      <c r="AK33" s="108"/>
-      <c r="AL33" s="108"/>
-      <c r="AM33" s="108"/>
-      <c r="AN33" s="108"/>
-      <c r="AO33" s="109"/>
+      <c r="AJ33" s="121"/>
+      <c r="AK33" s="107"/>
+      <c r="AL33" s="107"/>
+      <c r="AM33" s="107"/>
+      <c r="AN33" s="107"/>
+      <c r="AO33" s="108"/>
       <c r="AP33" s="41"/>
       <c r="AQ33" s="28"/>
       <c r="AR33" s="28"/>
@@ -5205,7 +5217,7 @@
     <row r="34" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A34" s="1"/>
       <c r="B34" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="73" t="s">
         <v>6</v>
@@ -5216,7 +5228,7 @@
       <c r="E34" s="74">
         <v>45229</v>
       </c>
-      <c r="F34" s="77"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -5247,12 +5259,12 @@
       <c r="AH34" s="44"/>
       <c r="AI34" s="28"/>
       <c r="AJ34" s="66"/>
-      <c r="AK34" s="123"/>
-      <c r="AL34" s="108"/>
-      <c r="AM34" s="108"/>
-      <c r="AN34" s="108"/>
-      <c r="AO34" s="108"/>
-      <c r="AP34" s="109"/>
+      <c r="AK34" s="122"/>
+      <c r="AL34" s="107"/>
+      <c r="AM34" s="107"/>
+      <c r="AN34" s="107"/>
+      <c r="AO34" s="107"/>
+      <c r="AP34" s="108"/>
       <c r="AQ34" s="41"/>
       <c r="AR34" s="28"/>
       <c r="AS34" s="28"/>
@@ -5298,7 +5310,7 @@
     <row r="35" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="1"/>
       <c r="B35" s="72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="73" t="s">
         <v>8</v>
@@ -5309,7 +5321,7 @@
       <c r="E35" s="74">
         <v>45230</v>
       </c>
-      <c r="F35" s="77"/>
+      <c r="F35" s="76"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
@@ -5341,21 +5353,21 @@
       <c r="AI35" s="28"/>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="56"/>
-      <c r="AL35" s="130"/>
-      <c r="AM35" s="108"/>
-      <c r="AN35" s="108"/>
-      <c r="AO35" s="108"/>
-      <c r="AP35" s="114"/>
-      <c r="AQ35" s="119"/>
-      <c r="AR35" s="102"/>
-      <c r="AS35" s="100"/>
-      <c r="AT35" s="100"/>
+      <c r="AL35" s="109"/>
+      <c r="AM35" s="107"/>
+      <c r="AN35" s="107"/>
+      <c r="AO35" s="107"/>
+      <c r="AP35" s="110"/>
+      <c r="AQ35" s="111"/>
+      <c r="AR35" s="101"/>
+      <c r="AS35" s="99"/>
+      <c r="AT35" s="99"/>
       <c r="AU35" s="75"/>
       <c r="AV35" s="75"/>
-      <c r="AW35" s="100"/>
-      <c r="AX35" s="100"/>
-      <c r="AY35" s="100"/>
-      <c r="AZ35" s="28"/>
+      <c r="AW35" s="99"/>
+      <c r="AX35" s="99"/>
+      <c r="AY35" s="99"/>
+      <c r="AZ35" s="99"/>
       <c r="BA35" s="28"/>
       <c r="BB35" s="44"/>
       <c r="BC35" s="44"/>
@@ -5390,8 +5402,8 @@
     </row>
     <row r="36" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="78" t="s">
-        <v>44</v>
+      <c r="B36" s="77" t="s">
+        <v>43</v>
       </c>
       <c r="C36" s="73" t="s">
         <v>3</v>
@@ -5400,9 +5412,9 @@
         <v>45229</v>
       </c>
       <c r="E36" s="74">
-        <v>45238</v>
-      </c>
-      <c r="F36" s="77"/>
+        <v>45239</v>
+      </c>
+      <c r="F36" s="76"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
@@ -5437,19 +5449,19 @@
       <c r="AL36" s="57"/>
       <c r="AM36" s="57"/>
       <c r="AN36" s="40"/>
-      <c r="AO36" s="101"/>
-      <c r="AP36" s="115"/>
-      <c r="AQ36" s="116"/>
-      <c r="AR36" s="116"/>
-      <c r="AS36" s="116"/>
-      <c r="AT36" s="116"/>
-      <c r="AU36" s="116"/>
-      <c r="AV36" s="116"/>
-      <c r="AW36" s="116"/>
-      <c r="AX36" s="116"/>
-      <c r="AY36" s="117"/>
-      <c r="AZ36" s="41"/>
-      <c r="BA36" s="42"/>
+      <c r="AO36" s="100"/>
+      <c r="AP36" s="112"/>
+      <c r="AQ36" s="164"/>
+      <c r="AR36" s="164"/>
+      <c r="AS36" s="164"/>
+      <c r="AT36" s="164"/>
+      <c r="AU36" s="164"/>
+      <c r="AV36" s="164"/>
+      <c r="AW36" s="164"/>
+      <c r="AX36" s="164"/>
+      <c r="AY36" s="164"/>
+      <c r="AZ36" s="165"/>
+      <c r="BA36" s="101"/>
       <c r="BB36" s="75"/>
       <c r="BC36" s="75"/>
       <c r="BD36" s="42"/>
@@ -5481,10 +5493,10 @@
       <c r="CD36" s="44"/>
       <c r="CE36" s="44"/>
     </row>
-    <row r="37" spans="1:83" ht="15" customHeight="1">
+    <row r="37" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A37" s="1"/>
       <c r="B37" s="72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="73" t="s">
         <v>2</v>
@@ -5495,7 +5507,7 @@
       <c r="E37" s="74">
         <v>45245</v>
       </c>
-      <c r="F37" s="77"/>
+      <c r="F37" s="76"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
@@ -5533,21 +5545,21 @@
       <c r="AO37" s="44"/>
       <c r="AP37" s="57"/>
       <c r="AQ37" s="57"/>
-      <c r="AR37" s="79"/>
-      <c r="AS37" s="79"/>
-      <c r="AT37" s="79"/>
-      <c r="AU37" s="103"/>
-      <c r="AV37" s="157"/>
-      <c r="AW37" s="151"/>
-      <c r="AX37" s="151"/>
-      <c r="AY37" s="151"/>
-      <c r="AZ37" s="108"/>
-      <c r="BA37" s="108"/>
-      <c r="BB37" s="108"/>
-      <c r="BC37" s="108"/>
-      <c r="BD37" s="108"/>
-      <c r="BE37" s="108"/>
-      <c r="BF37" s="109"/>
+      <c r="AR37" s="78"/>
+      <c r="AS37" s="78"/>
+      <c r="AT37" s="78"/>
+      <c r="AU37" s="102"/>
+      <c r="AV37" s="115"/>
+      <c r="AW37" s="116"/>
+      <c r="AX37" s="116"/>
+      <c r="AY37" s="116"/>
+      <c r="AZ37" s="116"/>
+      <c r="BA37" s="107"/>
+      <c r="BB37" s="107"/>
+      <c r="BC37" s="107"/>
+      <c r="BD37" s="107"/>
+      <c r="BE37" s="107"/>
+      <c r="BF37" s="108"/>
       <c r="BG37" s="38"/>
       <c r="BH37" s="28"/>
       <c r="BI37" s="44"/>
@@ -5577,7 +5589,7 @@
     <row r="38" spans="1:83" ht="15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="73" t="s">
         <v>4</v>
@@ -5588,7 +5600,7 @@
       <c r="E38" s="74">
         <v>45241</v>
       </c>
-      <c r="F38" s="77"/>
+      <c r="F38" s="76"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
@@ -5626,17 +5638,17 @@
       <c r="AO38" s="44"/>
       <c r="AP38" s="28"/>
       <c r="AQ38" s="67"/>
-      <c r="AR38" s="147"/>
-      <c r="AS38" s="108"/>
-      <c r="AT38" s="108"/>
-      <c r="AU38" s="108"/>
-      <c r="AV38" s="108"/>
-      <c r="AW38" s="108"/>
-      <c r="AX38" s="108"/>
-      <c r="AY38" s="108"/>
-      <c r="AZ38" s="108"/>
-      <c r="BA38" s="108"/>
-      <c r="BB38" s="109"/>
+      <c r="AR38" s="106"/>
+      <c r="AS38" s="107"/>
+      <c r="AT38" s="107"/>
+      <c r="AU38" s="107"/>
+      <c r="AV38" s="107"/>
+      <c r="AW38" s="107"/>
+      <c r="AX38" s="107"/>
+      <c r="AY38" s="107"/>
+      <c r="AZ38" s="107"/>
+      <c r="BA38" s="107"/>
+      <c r="BB38" s="108"/>
       <c r="BC38" s="46"/>
       <c r="BD38" s="57"/>
       <c r="BE38" s="57"/>
@@ -5670,7 +5682,7 @@
     <row r="39" spans="1:83" ht="15" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="73" t="s">
         <v>7</v>
@@ -5681,7 +5693,7 @@
       <c r="E39" s="74">
         <v>45242</v>
       </c>
-      <c r="F39" s="77"/>
+      <c r="F39" s="76"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
@@ -5720,17 +5732,17 @@
       <c r="AP39" s="28"/>
       <c r="AQ39" s="28"/>
       <c r="AR39" s="66"/>
-      <c r="AS39" s="158"/>
-      <c r="AT39" s="108"/>
-      <c r="AU39" s="108"/>
-      <c r="AV39" s="108"/>
-      <c r="AW39" s="108"/>
-      <c r="AX39" s="108"/>
-      <c r="AY39" s="108"/>
-      <c r="AZ39" s="108"/>
-      <c r="BA39" s="108"/>
-      <c r="BB39" s="108"/>
-      <c r="BC39" s="109"/>
+      <c r="AS39" s="117"/>
+      <c r="AT39" s="107"/>
+      <c r="AU39" s="107"/>
+      <c r="AV39" s="107"/>
+      <c r="AW39" s="107"/>
+      <c r="AX39" s="107"/>
+      <c r="AY39" s="107"/>
+      <c r="AZ39" s="107"/>
+      <c r="BA39" s="107"/>
+      <c r="BB39" s="107"/>
+      <c r="BC39" s="108"/>
       <c r="BD39" s="41"/>
       <c r="BE39" s="28"/>
       <c r="BF39" s="28"/>
@@ -5763,7 +5775,7 @@
     <row r="40" spans="1:83" ht="15" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="73" t="s">
         <v>4</v>
@@ -5774,7 +5786,7 @@
       <c r="E40" s="74">
         <v>45243</v>
       </c>
-      <c r="F40" s="77"/>
+      <c r="F40" s="76"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
@@ -5814,17 +5826,17 @@
       <c r="AQ40" s="28"/>
       <c r="AR40" s="28"/>
       <c r="AS40" s="66"/>
-      <c r="AT40" s="147"/>
-      <c r="AU40" s="108"/>
-      <c r="AV40" s="108"/>
-      <c r="AW40" s="108"/>
-      <c r="AX40" s="108"/>
-      <c r="AY40" s="108"/>
-      <c r="AZ40" s="108"/>
-      <c r="BA40" s="108"/>
-      <c r="BB40" s="108"/>
-      <c r="BC40" s="108"/>
-      <c r="BD40" s="109"/>
+      <c r="AT40" s="106"/>
+      <c r="AU40" s="107"/>
+      <c r="AV40" s="107"/>
+      <c r="AW40" s="107"/>
+      <c r="AX40" s="107"/>
+      <c r="AY40" s="107"/>
+      <c r="AZ40" s="107"/>
+      <c r="BA40" s="107"/>
+      <c r="BB40" s="107"/>
+      <c r="BC40" s="107"/>
+      <c r="BD40" s="108"/>
       <c r="BE40" s="38"/>
       <c r="BF40" s="28"/>
       <c r="BG40" s="28"/>
@@ -5856,7 +5868,7 @@
     <row r="41" spans="1:83" ht="15" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="73" t="s">
         <v>5</v>
@@ -5867,7 +5879,7 @@
       <c r="E41" s="74">
         <v>45239</v>
       </c>
-      <c r="F41" s="77"/>
+      <c r="F41" s="76"/>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
@@ -5909,15 +5921,15 @@
       <c r="AS41" s="28"/>
       <c r="AT41" s="57"/>
       <c r="AU41" s="51"/>
-      <c r="AV41" s="107"/>
-      <c r="AW41" s="108"/>
-      <c r="AX41" s="108"/>
-      <c r="AY41" s="108"/>
-      <c r="AZ41" s="109"/>
+      <c r="AV41" s="126"/>
+      <c r="AW41" s="107"/>
+      <c r="AX41" s="107"/>
+      <c r="AY41" s="107"/>
+      <c r="AZ41" s="108"/>
       <c r="BA41" s="55"/>
       <c r="BB41" s="39"/>
       <c r="BC41" s="39"/>
-      <c r="BD41" s="79"/>
+      <c r="BD41" s="78"/>
       <c r="BE41" s="42"/>
       <c r="BF41" s="42"/>
       <c r="BG41" s="28"/>
@@ -5948,8 +5960,8 @@
     </row>
     <row r="42" spans="1:83" ht="15" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="78" t="s">
-        <v>50</v>
+      <c r="B42" s="77" t="s">
+        <v>49</v>
       </c>
       <c r="C42" s="73" t="s">
         <v>7</v>
@@ -6003,16 +6015,16 @@
       <c r="AT42" s="28"/>
       <c r="AU42" s="49"/>
       <c r="AV42" s="49"/>
-      <c r="AW42" s="110"/>
-      <c r="AX42" s="108"/>
-      <c r="AY42" s="108"/>
-      <c r="AZ42" s="108"/>
-      <c r="BA42" s="108"/>
-      <c r="BB42" s="108"/>
-      <c r="BC42" s="108"/>
-      <c r="BD42" s="108"/>
-      <c r="BE42" s="108"/>
-      <c r="BF42" s="109"/>
+      <c r="AW42" s="123"/>
+      <c r="AX42" s="107"/>
+      <c r="AY42" s="107"/>
+      <c r="AZ42" s="107"/>
+      <c r="BA42" s="107"/>
+      <c r="BB42" s="107"/>
+      <c r="BC42" s="107"/>
+      <c r="BD42" s="107"/>
+      <c r="BE42" s="107"/>
+      <c r="BF42" s="108"/>
       <c r="BG42" s="41"/>
       <c r="BH42" s="42"/>
       <c r="BI42" s="75"/>
@@ -6039,10 +6051,10 @@
       <c r="CD42" s="75"/>
       <c r="CE42" s="75"/>
     </row>
-    <row r="43" spans="1:83" ht="15" customHeight="1">
+    <row r="43" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="78" t="s">
-        <v>51</v>
+      <c r="B43" s="77" t="s">
+        <v>50</v>
       </c>
       <c r="C43" s="73" t="s">
         <v>2</v>
@@ -6053,7 +6065,7 @@
       <c r="E43" s="74">
         <v>45242</v>
       </c>
-      <c r="F43" s="77"/>
+      <c r="F43" s="76"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -6095,14 +6107,14 @@
       <c r="AS43" s="28"/>
       <c r="AT43" s="28"/>
       <c r="AU43" s="53"/>
-      <c r="AV43" s="111"/>
-      <c r="AW43" s="108"/>
-      <c r="AX43" s="108"/>
-      <c r="AY43" s="108"/>
-      <c r="AZ43" s="108"/>
-      <c r="BA43" s="108"/>
-      <c r="BB43" s="108"/>
-      <c r="BC43" s="112"/>
+      <c r="AV43" s="160"/>
+      <c r="AW43" s="107"/>
+      <c r="AX43" s="107"/>
+      <c r="AY43" s="107"/>
+      <c r="AZ43" s="107"/>
+      <c r="BA43" s="107"/>
+      <c r="BB43" s="107"/>
+      <c r="BC43" s="120"/>
       <c r="BD43" s="28"/>
       <c r="BE43" s="28"/>
       <c r="BF43" s="28"/>
@@ -6132,10 +6144,10 @@
       <c r="CD43" s="44"/>
       <c r="CE43" s="44"/>
     </row>
-    <row r="44" spans="1:83" ht="15" customHeight="1">
+    <row r="44" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A44" s="1"/>
       <c r="B44" s="72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="73" t="s">
         <v>1</v>
@@ -6185,17 +6197,17 @@
       <c r="AP44" s="28"/>
       <c r="AQ44" s="28"/>
       <c r="AR44" s="28"/>
-      <c r="AS44" s="100"/>
+      <c r="AS44" s="99"/>
       <c r="AT44" s="56"/>
-      <c r="AU44" s="113"/>
-      <c r="AV44" s="114"/>
-      <c r="AW44" s="114"/>
-      <c r="AX44" s="114"/>
-      <c r="AY44" s="114"/>
-      <c r="AZ44" s="108"/>
-      <c r="BA44" s="109"/>
-      <c r="BB44" s="48"/>
-      <c r="BC44" s="40"/>
+      <c r="AU44" s="118"/>
+      <c r="AV44" s="110"/>
+      <c r="AW44" s="110"/>
+      <c r="AX44" s="110"/>
+      <c r="AY44" s="110"/>
+      <c r="AZ44" s="110"/>
+      <c r="BA44" s="111"/>
+      <c r="BB44" s="105"/>
+      <c r="BC44" s="98"/>
       <c r="BD44" s="57"/>
       <c r="BE44" s="57"/>
       <c r="BF44" s="57"/>
@@ -6225,19 +6237,19 @@
       <c r="CD44" s="44"/>
       <c r="CE44" s="44"/>
     </row>
-    <row r="45" spans="1:83" ht="15" customHeight="1">
+    <row r="45" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A45" s="1"/>
       <c r="B45" s="72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C45" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="74">
-        <v>45232</v>
+        <v>45235</v>
       </c>
       <c r="E45" s="74">
-        <v>45238</v>
+        <v>45242</v>
       </c>
       <c r="F45" s="37"/>
       <c r="G45" s="28"/>
@@ -6278,18 +6290,18 @@
       <c r="AP45" s="28"/>
       <c r="AQ45" s="28"/>
       <c r="AR45" s="67"/>
-      <c r="AS45" s="115"/>
-      <c r="AT45" s="116"/>
-      <c r="AU45" s="116"/>
-      <c r="AV45" s="116"/>
-      <c r="AW45" s="116"/>
-      <c r="AX45" s="116"/>
-      <c r="AY45" s="117"/>
-      <c r="AZ45" s="55"/>
-      <c r="BA45" s="79"/>
-      <c r="BB45" s="75"/>
-      <c r="BC45" s="75"/>
-      <c r="BD45" s="42"/>
+      <c r="AS45" s="67"/>
+      <c r="AT45" s="67"/>
+      <c r="AU45" s="112"/>
+      <c r="AV45" s="164"/>
+      <c r="AW45" s="164"/>
+      <c r="AX45" s="164"/>
+      <c r="AY45" s="164"/>
+      <c r="AZ45" s="164"/>
+      <c r="BA45" s="164"/>
+      <c r="BB45" s="164"/>
+      <c r="BC45" s="165"/>
+      <c r="BD45" s="101"/>
       <c r="BE45" s="42"/>
       <c r="BF45" s="28"/>
       <c r="BG45" s="28"/>
@@ -6321,7 +6333,7 @@
     <row r="46" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A46" s="1"/>
       <c r="B46" s="72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="73" t="s">
         <v>8</v>
@@ -6373,17 +6385,17 @@
       <c r="AR46" s="28"/>
       <c r="AS46" s="57"/>
       <c r="AT46" s="57"/>
-      <c r="AU46" s="101"/>
-      <c r="AV46" s="101"/>
-      <c r="AW46" s="79"/>
+      <c r="AU46" s="100"/>
+      <c r="AV46" s="100"/>
+      <c r="AW46" s="78"/>
       <c r="AX46" s="56"/>
-      <c r="AY46" s="118"/>
-      <c r="AZ46" s="108"/>
-      <c r="BA46" s="108"/>
-      <c r="BB46" s="108"/>
-      <c r="BC46" s="108"/>
-      <c r="BD46" s="108"/>
-      <c r="BE46" s="109"/>
+      <c r="AY46" s="153"/>
+      <c r="AZ46" s="116"/>
+      <c r="BA46" s="116"/>
+      <c r="BB46" s="116"/>
+      <c r="BC46" s="116"/>
+      <c r="BD46" s="107"/>
+      <c r="BE46" s="108"/>
       <c r="BF46" s="38"/>
       <c r="BG46" s="28"/>
       <c r="BH46" s="28"/>
@@ -6414,7 +6426,7 @@
     <row r="47" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="1"/>
       <c r="B47" s="72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="73" t="s">
         <v>7</v>
@@ -6467,14 +6479,14 @@
       <c r="AS47" s="28"/>
       <c r="AT47" s="57"/>
       <c r="AU47" s="51"/>
-      <c r="AV47" s="110"/>
-      <c r="AW47" s="108"/>
-      <c r="AX47" s="108"/>
-      <c r="AY47" s="114"/>
-      <c r="AZ47" s="114"/>
-      <c r="BA47" s="119"/>
-      <c r="BB47" s="99"/>
-      <c r="BC47" s="99"/>
+      <c r="AV47" s="123"/>
+      <c r="AW47" s="107"/>
+      <c r="AX47" s="107"/>
+      <c r="AY47" s="110"/>
+      <c r="AZ47" s="110"/>
+      <c r="BA47" s="111"/>
+      <c r="BB47" s="98"/>
+      <c r="BC47" s="98"/>
       <c r="BD47" s="57"/>
       <c r="BE47" s="57"/>
       <c r="BF47" s="28"/>
@@ -6507,7 +6519,7 @@
     <row r="48" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A48" s="1"/>
       <c r="B48" s="72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="73" t="s">
         <v>4</v>
@@ -6563,11 +6575,11 @@
       <c r="AV48" s="40"/>
       <c r="AW48" s="57"/>
       <c r="AX48" s="66"/>
-      <c r="AY48" s="159"/>
-      <c r="AZ48" s="160"/>
-      <c r="BA48" s="160"/>
-      <c r="BB48" s="160"/>
-      <c r="BC48" s="161"/>
+      <c r="AY48" s="154"/>
+      <c r="AZ48" s="155"/>
+      <c r="BA48" s="155"/>
+      <c r="BB48" s="155"/>
+      <c r="BC48" s="156"/>
       <c r="BD48" s="41"/>
       <c r="BE48" s="28"/>
       <c r="BF48" s="28"/>
@@ -6599,10 +6611,10 @@
     </row>
     <row r="49" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="72" t="s">
         <v>57</v>
-      </c>
-      <c r="B49" s="72" t="s">
-        <v>58</v>
       </c>
       <c r="C49" s="73" t="s">
         <v>8</v>
@@ -6658,12 +6670,12 @@
       <c r="AV49" s="75"/>
       <c r="AW49" s="42"/>
       <c r="AX49" s="42"/>
-      <c r="AY49" s="79"/>
+      <c r="AY49" s="78"/>
       <c r="AZ49" s="56"/>
-      <c r="BA49" s="120"/>
-      <c r="BB49" s="121"/>
-      <c r="BC49" s="121"/>
-      <c r="BD49" s="122"/>
+      <c r="BA49" s="157"/>
+      <c r="BB49" s="158"/>
+      <c r="BC49" s="158"/>
+      <c r="BD49" s="159"/>
       <c r="BE49" s="38"/>
       <c r="BF49" s="28"/>
       <c r="BG49" s="28"/>
@@ -6695,7 +6707,7 @@
     <row r="50" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A50" s="1"/>
       <c r="B50" s="72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="73" t="s">
         <v>6</v>
@@ -6747,16 +6759,16 @@
       <c r="AR50" s="28"/>
       <c r="AS50" s="28"/>
       <c r="AT50" s="66"/>
-      <c r="AU50" s="123"/>
-      <c r="AV50" s="108"/>
-      <c r="AW50" s="108"/>
-      <c r="AX50" s="108"/>
-      <c r="AY50" s="108"/>
-      <c r="AZ50" s="109"/>
+      <c r="AU50" s="122"/>
+      <c r="AV50" s="107"/>
+      <c r="AW50" s="107"/>
+      <c r="AX50" s="107"/>
+      <c r="AY50" s="107"/>
+      <c r="AZ50" s="108"/>
       <c r="BA50" s="55"/>
       <c r="BB50" s="39"/>
       <c r="BC50" s="39"/>
-      <c r="BD50" s="79"/>
+      <c r="BD50" s="78"/>
       <c r="BE50" s="42"/>
       <c r="BF50" s="42"/>
       <c r="BG50" s="28"/>
@@ -6788,7 +6800,7 @@
     <row r="51" spans="1:83" ht="15" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="73" t="s">
         <v>1</v>
@@ -6846,12 +6858,12 @@
       <c r="AX51" s="57"/>
       <c r="AY51" s="57"/>
       <c r="AZ51" s="66"/>
-      <c r="BA51" s="124"/>
-      <c r="BB51" s="108"/>
-      <c r="BC51" s="108"/>
-      <c r="BD51" s="108"/>
-      <c r="BE51" s="108"/>
-      <c r="BF51" s="109"/>
+      <c r="BA51" s="152"/>
+      <c r="BB51" s="107"/>
+      <c r="BC51" s="107"/>
+      <c r="BD51" s="107"/>
+      <c r="BE51" s="107"/>
+      <c r="BF51" s="108"/>
       <c r="BG51" s="38"/>
       <c r="BH51" s="28"/>
       <c r="BI51" s="44"/>
@@ -6880,103 +6892,103 @@
     </row>
     <row r="52" spans="1:83" ht="15" customHeight="1">
       <c r="A52" s="1"/>
-      <c r="B52" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="81"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="83"/>
+      <c r="B52" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="80"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="82"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="125"/>
-      <c r="H52" s="126"/>
-      <c r="I52" s="126"/>
-      <c r="J52" s="126"/>
-      <c r="K52" s="126"/>
-      <c r="L52" s="126"/>
-      <c r="M52" s="126"/>
-      <c r="N52" s="126"/>
-      <c r="O52" s="126"/>
-      <c r="P52" s="126"/>
-      <c r="Q52" s="126"/>
-      <c r="R52" s="126"/>
-      <c r="S52" s="126"/>
-      <c r="T52" s="126"/>
-      <c r="U52" s="126"/>
-      <c r="V52" s="126"/>
-      <c r="W52" s="126"/>
-      <c r="X52" s="126"/>
-      <c r="Y52" s="126"/>
-      <c r="Z52" s="126"/>
-      <c r="AA52" s="126"/>
-      <c r="AB52" s="126"/>
-      <c r="AC52" s="126"/>
-      <c r="AD52" s="126"/>
-      <c r="AE52" s="126"/>
-      <c r="AF52" s="126"/>
-      <c r="AG52" s="126"/>
-      <c r="AH52" s="126"/>
-      <c r="AI52" s="126"/>
-      <c r="AJ52" s="126"/>
-      <c r="AK52" s="126"/>
-      <c r="AL52" s="126"/>
-      <c r="AM52" s="126"/>
-      <c r="AN52" s="126"/>
-      <c r="AO52" s="126"/>
-      <c r="AP52" s="126"/>
-      <c r="AQ52" s="126"/>
-      <c r="AR52" s="126"/>
-      <c r="AS52" s="126"/>
-      <c r="AT52" s="126"/>
-      <c r="AU52" s="126"/>
-      <c r="AV52" s="126"/>
-      <c r="AW52" s="126"/>
-      <c r="AX52" s="126"/>
-      <c r="AY52" s="126"/>
-      <c r="AZ52" s="126"/>
-      <c r="BA52" s="126"/>
-      <c r="BB52" s="126"/>
-      <c r="BC52" s="126"/>
-      <c r="BD52" s="126"/>
-      <c r="BE52" s="126"/>
-      <c r="BF52" s="126"/>
-      <c r="BG52" s="126"/>
-      <c r="BH52" s="126"/>
-      <c r="BI52" s="126"/>
-      <c r="BJ52" s="126"/>
-      <c r="BK52" s="126"/>
-      <c r="BL52" s="126"/>
-      <c r="BM52" s="126"/>
-      <c r="BN52" s="126"/>
-      <c r="BO52" s="126"/>
-      <c r="BP52" s="126"/>
-      <c r="BQ52" s="126"/>
-      <c r="BR52" s="126"/>
-      <c r="BS52" s="126"/>
-      <c r="BT52" s="126"/>
-      <c r="BU52" s="126"/>
-      <c r="BV52" s="126"/>
-      <c r="BW52" s="126"/>
-      <c r="BX52" s="126"/>
-      <c r="BY52" s="126"/>
-      <c r="BZ52" s="126"/>
-      <c r="CA52" s="126"/>
-      <c r="CB52" s="126"/>
-      <c r="CC52" s="126"/>
-      <c r="CD52" s="126"/>
-      <c r="CE52" s="127"/>
+      <c r="G52" s="130"/>
+      <c r="H52" s="131"/>
+      <c r="I52" s="131"/>
+      <c r="J52" s="131"/>
+      <c r="K52" s="131"/>
+      <c r="L52" s="131"/>
+      <c r="M52" s="131"/>
+      <c r="N52" s="131"/>
+      <c r="O52" s="131"/>
+      <c r="P52" s="131"/>
+      <c r="Q52" s="131"/>
+      <c r="R52" s="131"/>
+      <c r="S52" s="131"/>
+      <c r="T52" s="131"/>
+      <c r="U52" s="131"/>
+      <c r="V52" s="131"/>
+      <c r="W52" s="131"/>
+      <c r="X52" s="131"/>
+      <c r="Y52" s="131"/>
+      <c r="Z52" s="131"/>
+      <c r="AA52" s="131"/>
+      <c r="AB52" s="131"/>
+      <c r="AC52" s="131"/>
+      <c r="AD52" s="131"/>
+      <c r="AE52" s="131"/>
+      <c r="AF52" s="131"/>
+      <c r="AG52" s="131"/>
+      <c r="AH52" s="131"/>
+      <c r="AI52" s="131"/>
+      <c r="AJ52" s="131"/>
+      <c r="AK52" s="131"/>
+      <c r="AL52" s="131"/>
+      <c r="AM52" s="131"/>
+      <c r="AN52" s="131"/>
+      <c r="AO52" s="131"/>
+      <c r="AP52" s="131"/>
+      <c r="AQ52" s="131"/>
+      <c r="AR52" s="131"/>
+      <c r="AS52" s="131"/>
+      <c r="AT52" s="131"/>
+      <c r="AU52" s="131"/>
+      <c r="AV52" s="131"/>
+      <c r="AW52" s="131"/>
+      <c r="AX52" s="131"/>
+      <c r="AY52" s="131"/>
+      <c r="AZ52" s="131"/>
+      <c r="BA52" s="131"/>
+      <c r="BB52" s="131"/>
+      <c r="BC52" s="131"/>
+      <c r="BD52" s="131"/>
+      <c r="BE52" s="131"/>
+      <c r="BF52" s="131"/>
+      <c r="BG52" s="131"/>
+      <c r="BH52" s="131"/>
+      <c r="BI52" s="131"/>
+      <c r="BJ52" s="131"/>
+      <c r="BK52" s="131"/>
+      <c r="BL52" s="131"/>
+      <c r="BM52" s="131"/>
+      <c r="BN52" s="131"/>
+      <c r="BO52" s="131"/>
+      <c r="BP52" s="131"/>
+      <c r="BQ52" s="131"/>
+      <c r="BR52" s="131"/>
+      <c r="BS52" s="131"/>
+      <c r="BT52" s="131"/>
+      <c r="BU52" s="131"/>
+      <c r="BV52" s="131"/>
+      <c r="BW52" s="131"/>
+      <c r="BX52" s="131"/>
+      <c r="BY52" s="131"/>
+      <c r="BZ52" s="131"/>
+      <c r="CA52" s="131"/>
+      <c r="CB52" s="131"/>
+      <c r="CC52" s="131"/>
+      <c r="CD52" s="131"/>
+      <c r="CE52" s="132"/>
     </row>
     <row r="53" spans="1:83" ht="15" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53" s="85" t="s">
+      <c r="B53" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="86">
+      <c r="D53" s="85">
         <v>45241</v>
       </c>
-      <c r="E53" s="86">
+      <c r="E53" s="85">
         <v>45244</v>
       </c>
       <c r="F53" s="37"/>
@@ -7027,10 +7039,10 @@
       <c r="AY53" s="28"/>
       <c r="AZ53" s="28"/>
       <c r="BA53" s="67"/>
-      <c r="BB53" s="123"/>
-      <c r="BC53" s="108"/>
-      <c r="BD53" s="108"/>
-      <c r="BE53" s="109"/>
+      <c r="BB53" s="122"/>
+      <c r="BC53" s="107"/>
+      <c r="BD53" s="107"/>
+      <c r="BE53" s="108"/>
       <c r="BF53" s="41"/>
       <c r="BG53" s="42"/>
       <c r="BH53" s="42"/>
@@ -7060,16 +7072,16 @@
     </row>
     <row r="54" spans="1:83" ht="15" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="85" t="s">
+      <c r="B54" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="86">
+      <c r="D54" s="85">
         <v>45245</v>
       </c>
-      <c r="E54" s="86">
+      <c r="E54" s="85">
         <v>45249</v>
       </c>
       <c r="F54" s="37"/>
@@ -7124,11 +7136,11 @@
       <c r="BC54" s="40"/>
       <c r="BD54" s="57"/>
       <c r="BE54" s="56"/>
-      <c r="BF54" s="123"/>
-      <c r="BG54" s="108"/>
-      <c r="BH54" s="108"/>
-      <c r="BI54" s="108"/>
-      <c r="BJ54" s="109"/>
+      <c r="BF54" s="122"/>
+      <c r="BG54" s="107"/>
+      <c r="BH54" s="107"/>
+      <c r="BI54" s="107"/>
+      <c r="BJ54" s="108"/>
       <c r="BK54" s="41"/>
       <c r="BL54" s="42"/>
       <c r="BM54" s="28"/>
@@ -7153,16 +7165,16 @@
     </row>
     <row r="55" spans="1:83" ht="15" customHeight="1">
       <c r="A55" s="1"/>
-      <c r="B55" s="84" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="85" t="s">
+      <c r="B55" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="86">
+      <c r="D55" s="85">
         <v>45244</v>
       </c>
-      <c r="E55" s="86">
+      <c r="E55" s="85">
         <v>45251</v>
       </c>
       <c r="F55" s="37"/>
@@ -7216,14 +7228,14 @@
       <c r="BB55" s="44"/>
       <c r="BC55" s="44"/>
       <c r="BD55" s="67"/>
-      <c r="BE55" s="110"/>
-      <c r="BF55" s="108"/>
-      <c r="BG55" s="108"/>
-      <c r="BH55" s="108"/>
-      <c r="BI55" s="108"/>
-      <c r="BJ55" s="108"/>
-      <c r="BK55" s="108"/>
-      <c r="BL55" s="109"/>
+      <c r="BE55" s="123"/>
+      <c r="BF55" s="107"/>
+      <c r="BG55" s="107"/>
+      <c r="BH55" s="107"/>
+      <c r="BI55" s="107"/>
+      <c r="BJ55" s="107"/>
+      <c r="BK55" s="107"/>
+      <c r="BL55" s="108"/>
       <c r="BM55" s="38"/>
       <c r="BN55" s="28"/>
       <c r="BO55" s="28"/>
@@ -7246,16 +7258,16 @@
     </row>
     <row r="56" spans="1:83" ht="15" customHeight="1">
       <c r="A56" s="1"/>
-      <c r="B56" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="85" t="s">
+      <c r="B56" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="86">
+      <c r="D56" s="85">
         <v>45245</v>
       </c>
-      <c r="E56" s="86">
+      <c r="E56" s="85">
         <v>45251</v>
       </c>
       <c r="F56" s="37"/>
@@ -7310,15 +7322,15 @@
       <c r="BC56" s="44"/>
       <c r="BD56" s="28"/>
       <c r="BE56" s="66"/>
-      <c r="BF56" s="129"/>
-      <c r="BG56" s="108"/>
-      <c r="BH56" s="108"/>
-      <c r="BI56" s="108"/>
-      <c r="BJ56" s="108"/>
-      <c r="BK56" s="108"/>
-      <c r="BL56" s="109"/>
+      <c r="BF56" s="149"/>
+      <c r="BG56" s="107"/>
+      <c r="BH56" s="107"/>
+      <c r="BI56" s="107"/>
+      <c r="BJ56" s="107"/>
+      <c r="BK56" s="107"/>
+      <c r="BL56" s="108"/>
       <c r="BM56" s="41"/>
-      <c r="BN56" s="87"/>
+      <c r="BN56" s="86"/>
       <c r="BO56" s="42"/>
       <c r="BP56" s="44"/>
       <c r="BQ56" s="44"/>
@@ -7339,16 +7351,16 @@
     </row>
     <row r="57" spans="1:83" ht="15" customHeight="1">
       <c r="A57" s="1"/>
-      <c r="B57" s="84" t="s">
-        <v>66</v>
-      </c>
-      <c r="C57" s="85" t="s">
+      <c r="B57" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="86">
+      <c r="D57" s="85">
         <v>45249</v>
       </c>
-      <c r="E57" s="86">
+      <c r="E57" s="85">
         <v>44524</v>
       </c>
       <c r="F57" s="37"/>
@@ -7407,12 +7419,12 @@
       <c r="BG57" s="57"/>
       <c r="BH57" s="57"/>
       <c r="BI57" s="51"/>
-      <c r="BJ57" s="130"/>
-      <c r="BK57" s="108"/>
-      <c r="BL57" s="108"/>
-      <c r="BM57" s="108"/>
-      <c r="BN57" s="108"/>
-      <c r="BO57" s="109"/>
+      <c r="BJ57" s="109"/>
+      <c r="BK57" s="107"/>
+      <c r="BL57" s="107"/>
+      <c r="BM57" s="107"/>
+      <c r="BN57" s="107"/>
+      <c r="BO57" s="108"/>
       <c r="BP57" s="53"/>
       <c r="BQ57" s="75"/>
       <c r="BR57" s="42"/>
@@ -7432,16 +7444,16 @@
     </row>
     <row r="58" spans="1:83" ht="15" customHeight="1">
       <c r="A58" s="1"/>
-      <c r="B58" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="85" t="s">
+      <c r="B58" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="86">
+      <c r="D58" s="85">
         <v>45250</v>
       </c>
-      <c r="E58" s="86">
+      <c r="E58" s="85">
         <v>44528</v>
       </c>
       <c r="F58" s="37"/>
@@ -7501,15 +7513,15 @@
       <c r="BH58" s="28"/>
       <c r="BI58" s="44"/>
       <c r="BJ58" s="51"/>
-      <c r="BK58" s="107"/>
-      <c r="BL58" s="108"/>
-      <c r="BM58" s="108"/>
-      <c r="BN58" s="108"/>
-      <c r="BO58" s="108"/>
-      <c r="BP58" s="108"/>
-      <c r="BQ58" s="108"/>
-      <c r="BR58" s="108"/>
-      <c r="BS58" s="109"/>
+      <c r="BK58" s="126"/>
+      <c r="BL58" s="107"/>
+      <c r="BM58" s="107"/>
+      <c r="BN58" s="107"/>
+      <c r="BO58" s="107"/>
+      <c r="BP58" s="107"/>
+      <c r="BQ58" s="107"/>
+      <c r="BR58" s="107"/>
+      <c r="BS58" s="108"/>
       <c r="BT58" s="38"/>
       <c r="BU58" s="28"/>
       <c r="BV58" s="28"/>
@@ -7525,16 +7537,16 @@
     </row>
     <row r="59" spans="1:83" ht="15" customHeight="1">
       <c r="A59" s="1"/>
-      <c r="B59" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="C59" s="85" t="s">
+      <c r="B59" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="86">
+      <c r="D59" s="85">
         <v>45251</v>
       </c>
-      <c r="E59" s="86">
+      <c r="E59" s="85">
         <v>45256</v>
       </c>
       <c r="F59" s="37"/>
@@ -7595,12 +7607,12 @@
       <c r="BI59" s="44"/>
       <c r="BJ59" s="51"/>
       <c r="BK59" s="57"/>
-      <c r="BL59" s="131"/>
-      <c r="BM59" s="108"/>
-      <c r="BN59" s="108"/>
-      <c r="BO59" s="108"/>
-      <c r="BP59" s="108"/>
-      <c r="BQ59" s="132"/>
+      <c r="BL59" s="150"/>
+      <c r="BM59" s="107"/>
+      <c r="BN59" s="107"/>
+      <c r="BO59" s="107"/>
+      <c r="BP59" s="107"/>
+      <c r="BQ59" s="151"/>
       <c r="BR59" s="47"/>
       <c r="BS59" s="47"/>
       <c r="BT59" s="38"/>
@@ -7618,16 +7630,16 @@
     </row>
     <row r="60" spans="1:83" ht="15" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="84" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" s="85" t="s">
+      <c r="B60" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="86">
+      <c r="D60" s="85">
         <v>45252</v>
       </c>
-      <c r="E60" s="86">
+      <c r="E60" s="85">
         <v>44528</v>
       </c>
       <c r="F60" s="37"/>
@@ -7689,13 +7701,13 @@
       <c r="BJ60" s="44"/>
       <c r="BK60" s="57"/>
       <c r="BL60" s="66"/>
-      <c r="BM60" s="133"/>
-      <c r="BN60" s="108"/>
-      <c r="BO60" s="108"/>
-      <c r="BP60" s="108"/>
-      <c r="BQ60" s="108"/>
-      <c r="BR60" s="108"/>
-      <c r="BS60" s="109"/>
+      <c r="BM60" s="119"/>
+      <c r="BN60" s="107"/>
+      <c r="BO60" s="107"/>
+      <c r="BP60" s="107"/>
+      <c r="BQ60" s="107"/>
+      <c r="BR60" s="107"/>
+      <c r="BS60" s="108"/>
       <c r="BT60" s="38"/>
       <c r="BU60" s="28"/>
       <c r="BV60" s="28"/>
@@ -7711,16 +7723,16 @@
     </row>
     <row r="61" spans="1:83" ht="15" customHeight="1">
       <c r="A61" s="1"/>
-      <c r="B61" s="84" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" s="85" t="s">
+      <c r="B61" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="86">
+      <c r="D61" s="85">
         <v>45252</v>
       </c>
-      <c r="E61" s="86">
+      <c r="E61" s="85">
         <v>44524</v>
       </c>
       <c r="F61" s="37"/>
@@ -7782,13 +7794,13 @@
       <c r="BJ61" s="44"/>
       <c r="BK61" s="28"/>
       <c r="BL61" s="67"/>
-      <c r="BM61" s="107"/>
-      <c r="BN61" s="108"/>
-      <c r="BO61" s="108"/>
-      <c r="BP61" s="108"/>
-      <c r="BQ61" s="109"/>
+      <c r="BM61" s="126"/>
+      <c r="BN61" s="107"/>
+      <c r="BO61" s="107"/>
+      <c r="BP61" s="107"/>
+      <c r="BQ61" s="108"/>
       <c r="BR61" s="55"/>
-      <c r="BS61" s="79"/>
+      <c r="BS61" s="78"/>
       <c r="BT61" s="42"/>
       <c r="BU61" s="28"/>
       <c r="BV61" s="28"/>
@@ -7804,16 +7816,16 @@
     </row>
     <row r="62" spans="1:83" ht="15" customHeight="1">
       <c r="A62" s="1"/>
-      <c r="B62" s="88" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" s="85" t="s">
+      <c r="B62" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="86">
+      <c r="D62" s="85">
         <v>45253</v>
       </c>
-      <c r="E62" s="86">
+      <c r="E62" s="85">
         <v>45259</v>
       </c>
       <c r="F62" s="37"/>
@@ -7876,13 +7888,13 @@
       <c r="BK62" s="28"/>
       <c r="BL62" s="28"/>
       <c r="BM62" s="66"/>
-      <c r="BN62" s="110"/>
-      <c r="BO62" s="108"/>
-      <c r="BP62" s="108"/>
-      <c r="BQ62" s="108"/>
-      <c r="BR62" s="108"/>
-      <c r="BS62" s="108"/>
-      <c r="BT62" s="109"/>
+      <c r="BN62" s="123"/>
+      <c r="BO62" s="107"/>
+      <c r="BP62" s="107"/>
+      <c r="BQ62" s="107"/>
+      <c r="BR62" s="107"/>
+      <c r="BS62" s="107"/>
+      <c r="BT62" s="108"/>
       <c r="BU62" s="38"/>
       <c r="BV62" s="28"/>
       <c r="BW62" s="44"/>
@@ -7897,16 +7909,16 @@
     </row>
     <row r="63" spans="1:83" ht="15" customHeight="1">
       <c r="A63" s="1"/>
-      <c r="B63" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="85" t="s">
+      <c r="B63" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="86">
+      <c r="D63" s="85">
         <v>45255</v>
       </c>
-      <c r="E63" s="86">
+      <c r="E63" s="85">
         <v>44529</v>
       </c>
       <c r="F63" s="37"/>
@@ -7971,11 +7983,11 @@
       <c r="BM63" s="28"/>
       <c r="BN63" s="57"/>
       <c r="BO63" s="66"/>
-      <c r="BP63" s="128"/>
-      <c r="BQ63" s="108"/>
-      <c r="BR63" s="108"/>
-      <c r="BS63" s="108"/>
-      <c r="BT63" s="109"/>
+      <c r="BP63" s="135"/>
+      <c r="BQ63" s="107"/>
+      <c r="BR63" s="107"/>
+      <c r="BS63" s="107"/>
+      <c r="BT63" s="108"/>
       <c r="BU63" s="38"/>
       <c r="BV63" s="28"/>
       <c r="BW63" s="44"/>
@@ -7990,887 +8002,887 @@
     </row>
     <row r="64" spans="1:83" ht="15" customHeight="1">
       <c r="A64" s="1"/>
-      <c r="B64" s="89"/>
-      <c r="C64" s="90"/>
-      <c r="D64" s="91"/>
-      <c r="E64" s="92"/>
-      <c r="F64" s="93"/>
-      <c r="G64" s="125"/>
-      <c r="H64" s="126"/>
-      <c r="I64" s="126"/>
-      <c r="J64" s="126"/>
-      <c r="K64" s="126"/>
-      <c r="L64" s="126"/>
-      <c r="M64" s="126"/>
-      <c r="N64" s="126"/>
-      <c r="O64" s="126"/>
-      <c r="P64" s="126"/>
-      <c r="Q64" s="126"/>
-      <c r="R64" s="126"/>
-      <c r="S64" s="126"/>
-      <c r="T64" s="126"/>
-      <c r="U64" s="126"/>
-      <c r="V64" s="126"/>
-      <c r="W64" s="126"/>
-      <c r="X64" s="126"/>
-      <c r="Y64" s="126"/>
-      <c r="Z64" s="126"/>
-      <c r="AA64" s="126"/>
-      <c r="AB64" s="126"/>
-      <c r="AC64" s="126"/>
-      <c r="AD64" s="126"/>
-      <c r="AE64" s="126"/>
-      <c r="AF64" s="126"/>
-      <c r="AG64" s="126"/>
-      <c r="AH64" s="126"/>
-      <c r="AI64" s="126"/>
-      <c r="AJ64" s="126"/>
-      <c r="AK64" s="126"/>
-      <c r="AL64" s="126"/>
-      <c r="AM64" s="126"/>
-      <c r="AN64" s="126"/>
-      <c r="AO64" s="126"/>
-      <c r="AP64" s="126"/>
-      <c r="AQ64" s="126"/>
-      <c r="AR64" s="126"/>
-      <c r="AS64" s="126"/>
-      <c r="AT64" s="126"/>
-      <c r="AU64" s="126"/>
-      <c r="AV64" s="126"/>
-      <c r="AW64" s="126"/>
-      <c r="AX64" s="126"/>
-      <c r="AY64" s="126"/>
-      <c r="AZ64" s="126"/>
-      <c r="BA64" s="126"/>
-      <c r="BB64" s="126"/>
-      <c r="BC64" s="126"/>
-      <c r="BD64" s="126"/>
-      <c r="BE64" s="126"/>
-      <c r="BF64" s="126"/>
-      <c r="BG64" s="126"/>
-      <c r="BH64" s="126"/>
-      <c r="BI64" s="126"/>
-      <c r="BJ64" s="126"/>
-      <c r="BK64" s="126"/>
-      <c r="BL64" s="126"/>
-      <c r="BM64" s="126"/>
-      <c r="BN64" s="126"/>
-      <c r="BO64" s="126"/>
-      <c r="BP64" s="126"/>
-      <c r="BQ64" s="126"/>
-      <c r="BR64" s="126"/>
-      <c r="BS64" s="126"/>
-      <c r="BT64" s="126"/>
-      <c r="BU64" s="126"/>
-      <c r="BV64" s="126"/>
-      <c r="BW64" s="126"/>
-      <c r="BX64" s="126"/>
-      <c r="BY64" s="126"/>
-      <c r="BZ64" s="126"/>
-      <c r="CA64" s="126"/>
-      <c r="CB64" s="126"/>
-      <c r="CC64" s="126"/>
-      <c r="CD64" s="126"/>
-      <c r="CE64" s="127"/>
+      <c r="B64" s="88"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="90"/>
+      <c r="E64" s="91"/>
+      <c r="F64" s="92"/>
+      <c r="G64" s="130"/>
+      <c r="H64" s="131"/>
+      <c r="I64" s="131"/>
+      <c r="J64" s="131"/>
+      <c r="K64" s="131"/>
+      <c r="L64" s="131"/>
+      <c r="M64" s="131"/>
+      <c r="N64" s="131"/>
+      <c r="O64" s="131"/>
+      <c r="P64" s="131"/>
+      <c r="Q64" s="131"/>
+      <c r="R64" s="131"/>
+      <c r="S64" s="131"/>
+      <c r="T64" s="131"/>
+      <c r="U64" s="131"/>
+      <c r="V64" s="131"/>
+      <c r="W64" s="131"/>
+      <c r="X64" s="131"/>
+      <c r="Y64" s="131"/>
+      <c r="Z64" s="131"/>
+      <c r="AA64" s="131"/>
+      <c r="AB64" s="131"/>
+      <c r="AC64" s="131"/>
+      <c r="AD64" s="131"/>
+      <c r="AE64" s="131"/>
+      <c r="AF64" s="131"/>
+      <c r="AG64" s="131"/>
+      <c r="AH64" s="131"/>
+      <c r="AI64" s="131"/>
+      <c r="AJ64" s="131"/>
+      <c r="AK64" s="131"/>
+      <c r="AL64" s="131"/>
+      <c r="AM64" s="131"/>
+      <c r="AN64" s="131"/>
+      <c r="AO64" s="131"/>
+      <c r="AP64" s="131"/>
+      <c r="AQ64" s="131"/>
+      <c r="AR64" s="131"/>
+      <c r="AS64" s="131"/>
+      <c r="AT64" s="131"/>
+      <c r="AU64" s="131"/>
+      <c r="AV64" s="131"/>
+      <c r="AW64" s="131"/>
+      <c r="AX64" s="131"/>
+      <c r="AY64" s="131"/>
+      <c r="AZ64" s="131"/>
+      <c r="BA64" s="131"/>
+      <c r="BB64" s="131"/>
+      <c r="BC64" s="131"/>
+      <c r="BD64" s="131"/>
+      <c r="BE64" s="131"/>
+      <c r="BF64" s="131"/>
+      <c r="BG64" s="131"/>
+      <c r="BH64" s="131"/>
+      <c r="BI64" s="131"/>
+      <c r="BJ64" s="131"/>
+      <c r="BK64" s="131"/>
+      <c r="BL64" s="131"/>
+      <c r="BM64" s="131"/>
+      <c r="BN64" s="131"/>
+      <c r="BO64" s="131"/>
+      <c r="BP64" s="131"/>
+      <c r="BQ64" s="131"/>
+      <c r="BR64" s="131"/>
+      <c r="BS64" s="131"/>
+      <c r="BT64" s="131"/>
+      <c r="BU64" s="131"/>
+      <c r="BV64" s="131"/>
+      <c r="BW64" s="131"/>
+      <c r="BX64" s="131"/>
+      <c r="BY64" s="131"/>
+      <c r="BZ64" s="131"/>
+      <c r="CA64" s="131"/>
+      <c r="CB64" s="131"/>
+      <c r="CC64" s="131"/>
+      <c r="CD64" s="131"/>
+      <c r="CE64" s="132"/>
     </row>
     <row r="65" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A65" s="94"/>
-      <c r="D65" s="95"/>
+      <c r="A65" s="93"/>
+      <c r="D65" s="94"/>
     </row>
     <row r="66" spans="1:5" ht="30" customHeight="1">
-      <c r="A66" s="94"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="97"/>
+      <c r="A66" s="93"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="94"/>
+      <c r="E66" s="96"/>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1">
-      <c r="A67" s="94"/>
-      <c r="C67" s="98"/>
-      <c r="D67" s="95"/>
+      <c r="A67" s="93"/>
+      <c r="C67" s="97"/>
+      <c r="D67" s="94"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A68" s="94"/>
-      <c r="D68" s="95"/>
+      <c r="A68" s="93"/>
+      <c r="D68" s="94"/>
     </row>
     <row r="69" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A69" s="94"/>
-      <c r="D69" s="95"/>
+      <c r="A69" s="93"/>
+      <c r="D69" s="94"/>
     </row>
     <row r="70" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A70" s="94"/>
-      <c r="D70" s="95"/>
+      <c r="A70" s="93"/>
+      <c r="D70" s="94"/>
     </row>
     <row r="71" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A71" s="94"/>
-      <c r="D71" s="95"/>
+      <c r="A71" s="93"/>
+      <c r="D71" s="94"/>
     </row>
     <row r="72" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A72" s="94"/>
-      <c r="D72" s="95"/>
+      <c r="A72" s="93"/>
+      <c r="D72" s="94"/>
     </row>
     <row r="73" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A73" s="94"/>
-      <c r="D73" s="95"/>
+      <c r="A73" s="93"/>
+      <c r="D73" s="94"/>
     </row>
     <row r="74" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A74" s="94"/>
-      <c r="D74" s="95"/>
+      <c r="A74" s="93"/>
+      <c r="D74" s="94"/>
     </row>
     <row r="75" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A75" s="94"/>
-      <c r="D75" s="95"/>
+      <c r="A75" s="93"/>
+      <c r="D75" s="94"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A76" s="94"/>
-      <c r="D76" s="95"/>
+      <c r="A76" s="93"/>
+      <c r="D76" s="94"/>
     </row>
     <row r="77" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A77" s="94"/>
-      <c r="D77" s="95"/>
+      <c r="A77" s="93"/>
+      <c r="D77" s="94"/>
     </row>
     <row r="78" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A78" s="94"/>
-      <c r="D78" s="95"/>
+      <c r="A78" s="93"/>
+      <c r="D78" s="94"/>
     </row>
     <row r="79" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A79" s="94"/>
-      <c r="D79" s="95"/>
+      <c r="A79" s="93"/>
+      <c r="D79" s="94"/>
     </row>
     <row r="80" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A80" s="94"/>
-      <c r="D80" s="95"/>
+      <c r="A80" s="93"/>
+      <c r="D80" s="94"/>
     </row>
     <row r="81" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A81" s="94"/>
-      <c r="D81" s="95"/>
+      <c r="A81" s="93"/>
+      <c r="D81" s="94"/>
     </row>
     <row r="82" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A82" s="94"/>
-      <c r="D82" s="95"/>
+      <c r="A82" s="93"/>
+      <c r="D82" s="94"/>
     </row>
     <row r="83" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A83" s="94"/>
-      <c r="D83" s="95"/>
+      <c r="A83" s="93"/>
+      <c r="D83" s="94"/>
     </row>
     <row r="84" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A84" s="94"/>
-      <c r="D84" s="95"/>
+      <c r="A84" s="93"/>
+      <c r="D84" s="94"/>
     </row>
     <row r="85" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A85" s="94"/>
-      <c r="D85" s="95"/>
+      <c r="A85" s="93"/>
+      <c r="D85" s="94"/>
     </row>
     <row r="86" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A86" s="94"/>
-      <c r="D86" s="95"/>
+      <c r="A86" s="93"/>
+      <c r="D86" s="94"/>
     </row>
     <row r="87" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A87" s="94"/>
-      <c r="D87" s="95"/>
+      <c r="A87" s="93"/>
+      <c r="D87" s="94"/>
     </row>
     <row r="88" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A88" s="94"/>
-      <c r="D88" s="95"/>
+      <c r="A88" s="93"/>
+      <c r="D88" s="94"/>
     </row>
     <row r="89" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A89" s="94"/>
-      <c r="D89" s="95"/>
+      <c r="A89" s="93"/>
+      <c r="D89" s="94"/>
     </row>
     <row r="90" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A90" s="94"/>
-      <c r="D90" s="95"/>
+      <c r="A90" s="93"/>
+      <c r="D90" s="94"/>
     </row>
     <row r="91" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A91" s="94"/>
-      <c r="D91" s="95"/>
+      <c r="A91" s="93"/>
+      <c r="D91" s="94"/>
     </row>
     <row r="92" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A92" s="94"/>
-      <c r="D92" s="95"/>
+      <c r="A92" s="93"/>
+      <c r="D92" s="94"/>
     </row>
     <row r="93" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A93" s="94"/>
-      <c r="D93" s="95"/>
+      <c r="A93" s="93"/>
+      <c r="D93" s="94"/>
     </row>
     <row r="94" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A94" s="94"/>
-      <c r="D94" s="95"/>
+      <c r="A94" s="93"/>
+      <c r="D94" s="94"/>
     </row>
     <row r="95" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A95" s="94"/>
-      <c r="D95" s="95"/>
+      <c r="A95" s="93"/>
+      <c r="D95" s="94"/>
     </row>
     <row r="96" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A96" s="94"/>
-      <c r="D96" s="95"/>
+      <c r="A96" s="93"/>
+      <c r="D96" s="94"/>
     </row>
     <row r="97" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A97" s="94"/>
-      <c r="D97" s="95"/>
+      <c r="A97" s="93"/>
+      <c r="D97" s="94"/>
     </row>
     <row r="98" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A98" s="94"/>
-      <c r="D98" s="95"/>
+      <c r="A98" s="93"/>
+      <c r="D98" s="94"/>
     </row>
     <row r="99" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A99" s="94"/>
-      <c r="D99" s="95"/>
+      <c r="A99" s="93"/>
+      <c r="D99" s="94"/>
     </row>
     <row r="100" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A100" s="94"/>
-      <c r="D100" s="95"/>
+      <c r="A100" s="93"/>
+      <c r="D100" s="94"/>
     </row>
     <row r="101" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A101" s="94"/>
-      <c r="D101" s="95"/>
+      <c r="A101" s="93"/>
+      <c r="D101" s="94"/>
     </row>
     <row r="102" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A102" s="94"/>
-      <c r="D102" s="95"/>
+      <c r="A102" s="93"/>
+      <c r="D102" s="94"/>
     </row>
     <row r="103" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A103" s="94"/>
-      <c r="D103" s="95"/>
+      <c r="A103" s="93"/>
+      <c r="D103" s="94"/>
     </row>
     <row r="104" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A104" s="94"/>
-      <c r="D104" s="95"/>
+      <c r="A104" s="93"/>
+      <c r="D104" s="94"/>
     </row>
     <row r="105" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A105" s="94"/>
-      <c r="D105" s="95"/>
+      <c r="A105" s="93"/>
+      <c r="D105" s="94"/>
     </row>
     <row r="106" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A106" s="94"/>
-      <c r="D106" s="95"/>
+      <c r="A106" s="93"/>
+      <c r="D106" s="94"/>
     </row>
     <row r="107" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A107" s="94"/>
-      <c r="D107" s="95"/>
+      <c r="A107" s="93"/>
+      <c r="D107" s="94"/>
     </row>
     <row r="108" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A108" s="94"/>
-      <c r="D108" s="95"/>
+      <c r="A108" s="93"/>
+      <c r="D108" s="94"/>
     </row>
     <row r="109" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A109" s="94"/>
-      <c r="D109" s="95"/>
+      <c r="A109" s="93"/>
+      <c r="D109" s="94"/>
     </row>
     <row r="110" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A110" s="94"/>
-      <c r="D110" s="95"/>
+      <c r="A110" s="93"/>
+      <c r="D110" s="94"/>
     </row>
     <row r="111" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A111" s="94"/>
-      <c r="D111" s="95"/>
+      <c r="A111" s="93"/>
+      <c r="D111" s="94"/>
     </row>
     <row r="112" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A112" s="94"/>
-      <c r="D112" s="95"/>
+      <c r="A112" s="93"/>
+      <c r="D112" s="94"/>
     </row>
     <row r="113" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A113" s="94"/>
-      <c r="D113" s="95"/>
+      <c r="A113" s="93"/>
+      <c r="D113" s="94"/>
     </row>
     <row r="114" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A114" s="94"/>
-      <c r="D114" s="95"/>
+      <c r="A114" s="93"/>
+      <c r="D114" s="94"/>
     </row>
     <row r="115" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A115" s="94"/>
-      <c r="D115" s="95"/>
+      <c r="A115" s="93"/>
+      <c r="D115" s="94"/>
     </row>
     <row r="116" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A116" s="94"/>
-      <c r="D116" s="95"/>
+      <c r="A116" s="93"/>
+      <c r="D116" s="94"/>
     </row>
     <row r="117" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A117" s="94"/>
-      <c r="D117" s="95"/>
+      <c r="A117" s="93"/>
+      <c r="D117" s="94"/>
     </row>
     <row r="118" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A118" s="94"/>
-      <c r="D118" s="95"/>
+      <c r="A118" s="93"/>
+      <c r="D118" s="94"/>
     </row>
     <row r="119" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A119" s="94"/>
-      <c r="D119" s="95"/>
+      <c r="A119" s="93"/>
+      <c r="D119" s="94"/>
     </row>
     <row r="120" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A120" s="94"/>
-      <c r="D120" s="95"/>
+      <c r="A120" s="93"/>
+      <c r="D120" s="94"/>
     </row>
     <row r="121" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A121" s="94"/>
-      <c r="D121" s="95"/>
+      <c r="A121" s="93"/>
+      <c r="D121" s="94"/>
     </row>
     <row r="122" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A122" s="94"/>
-      <c r="D122" s="95"/>
+      <c r="A122" s="93"/>
+      <c r="D122" s="94"/>
     </row>
     <row r="123" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A123" s="94"/>
-      <c r="D123" s="95"/>
+      <c r="A123" s="93"/>
+      <c r="D123" s="94"/>
     </row>
     <row r="124" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A124" s="94"/>
-      <c r="D124" s="95"/>
+      <c r="A124" s="93"/>
+      <c r="D124" s="94"/>
     </row>
     <row r="125" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A125" s="94"/>
-      <c r="D125" s="95"/>
+      <c r="A125" s="93"/>
+      <c r="D125" s="94"/>
     </row>
     <row r="126" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A126" s="94"/>
-      <c r="D126" s="95"/>
+      <c r="A126" s="93"/>
+      <c r="D126" s="94"/>
     </row>
     <row r="127" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A127" s="94"/>
-      <c r="D127" s="95"/>
+      <c r="A127" s="93"/>
+      <c r="D127" s="94"/>
     </row>
     <row r="128" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A128" s="94"/>
-      <c r="D128" s="95"/>
+      <c r="A128" s="93"/>
+      <c r="D128" s="94"/>
     </row>
     <row r="129" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A129" s="94"/>
-      <c r="D129" s="95"/>
+      <c r="A129" s="93"/>
+      <c r="D129" s="94"/>
     </row>
     <row r="130" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A130" s="94"/>
-      <c r="D130" s="95"/>
+      <c r="A130" s="93"/>
+      <c r="D130" s="94"/>
     </row>
     <row r="131" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A131" s="94"/>
-      <c r="D131" s="95"/>
+      <c r="A131" s="93"/>
+      <c r="D131" s="94"/>
     </row>
     <row r="132" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A132" s="94"/>
-      <c r="D132" s="95"/>
+      <c r="A132" s="93"/>
+      <c r="D132" s="94"/>
     </row>
     <row r="133" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A133" s="94"/>
-      <c r="D133" s="95"/>
+      <c r="A133" s="93"/>
+      <c r="D133" s="94"/>
     </row>
     <row r="134" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A134" s="94"/>
-      <c r="D134" s="95"/>
+      <c r="A134" s="93"/>
+      <c r="D134" s="94"/>
     </row>
     <row r="135" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A135" s="94"/>
-      <c r="D135" s="95"/>
+      <c r="A135" s="93"/>
+      <c r="D135" s="94"/>
     </row>
     <row r="136" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A136" s="94"/>
-      <c r="D136" s="95"/>
+      <c r="A136" s="93"/>
+      <c r="D136" s="94"/>
     </row>
     <row r="137" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A137" s="94"/>
-      <c r="D137" s="95"/>
+      <c r="A137" s="93"/>
+      <c r="D137" s="94"/>
     </row>
     <row r="138" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A138" s="94"/>
-      <c r="D138" s="95"/>
+      <c r="A138" s="93"/>
+      <c r="D138" s="94"/>
     </row>
     <row r="139" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A139" s="94"/>
-      <c r="D139" s="95"/>
+      <c r="A139" s="93"/>
+      <c r="D139" s="94"/>
     </row>
     <row r="140" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A140" s="94"/>
-      <c r="D140" s="95"/>
+      <c r="A140" s="93"/>
+      <c r="D140" s="94"/>
     </row>
     <row r="141" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A141" s="94"/>
-      <c r="D141" s="95"/>
+      <c r="A141" s="93"/>
+      <c r="D141" s="94"/>
     </row>
     <row r="142" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A142" s="94"/>
-      <c r="D142" s="95"/>
+      <c r="A142" s="93"/>
+      <c r="D142" s="94"/>
     </row>
     <row r="143" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A143" s="94"/>
-      <c r="D143" s="95"/>
+      <c r="A143" s="93"/>
+      <c r="D143" s="94"/>
     </row>
     <row r="144" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A144" s="94"/>
-      <c r="D144" s="95"/>
+      <c r="A144" s="93"/>
+      <c r="D144" s="94"/>
     </row>
     <row r="145" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A145" s="94"/>
-      <c r="D145" s="95"/>
+      <c r="A145" s="93"/>
+      <c r="D145" s="94"/>
     </row>
     <row r="146" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A146" s="94"/>
-      <c r="D146" s="95"/>
+      <c r="A146" s="93"/>
+      <c r="D146" s="94"/>
     </row>
     <row r="147" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A147" s="94"/>
-      <c r="D147" s="95"/>
+      <c r="A147" s="93"/>
+      <c r="D147" s="94"/>
     </row>
     <row r="148" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A148" s="94"/>
-      <c r="D148" s="95"/>
+      <c r="A148" s="93"/>
+      <c r="D148" s="94"/>
     </row>
     <row r="149" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A149" s="94"/>
-      <c r="D149" s="95"/>
+      <c r="A149" s="93"/>
+      <c r="D149" s="94"/>
     </row>
     <row r="150" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A150" s="94"/>
-      <c r="D150" s="95"/>
+      <c r="A150" s="93"/>
+      <c r="D150" s="94"/>
     </row>
     <row r="151" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A151" s="94"/>
-      <c r="D151" s="95"/>
+      <c r="A151" s="93"/>
+      <c r="D151" s="94"/>
     </row>
     <row r="152" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A152" s="94"/>
-      <c r="D152" s="95"/>
+      <c r="A152" s="93"/>
+      <c r="D152" s="94"/>
     </row>
     <row r="153" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A153" s="94"/>
-      <c r="D153" s="95"/>
+      <c r="A153" s="93"/>
+      <c r="D153" s="94"/>
     </row>
     <row r="154" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A154" s="94"/>
-      <c r="D154" s="95"/>
+      <c r="A154" s="93"/>
+      <c r="D154" s="94"/>
     </row>
     <row r="155" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A155" s="94"/>
-      <c r="D155" s="95"/>
+      <c r="A155" s="93"/>
+      <c r="D155" s="94"/>
     </row>
     <row r="156" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A156" s="94"/>
-      <c r="D156" s="95"/>
+      <c r="A156" s="93"/>
+      <c r="D156" s="94"/>
     </row>
     <row r="157" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A157" s="94"/>
-      <c r="D157" s="95"/>
+      <c r="A157" s="93"/>
+      <c r="D157" s="94"/>
     </row>
     <row r="158" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A158" s="94"/>
-      <c r="D158" s="95"/>
+      <c r="A158" s="93"/>
+      <c r="D158" s="94"/>
     </row>
     <row r="159" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A159" s="94"/>
-      <c r="D159" s="95"/>
+      <c r="A159" s="93"/>
+      <c r="D159" s="94"/>
     </row>
     <row r="160" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A160" s="94"/>
-      <c r="D160" s="95"/>
+      <c r="A160" s="93"/>
+      <c r="D160" s="94"/>
     </row>
     <row r="161" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A161" s="94"/>
-      <c r="D161" s="95"/>
+      <c r="A161" s="93"/>
+      <c r="D161" s="94"/>
     </row>
     <row r="162" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A162" s="94"/>
-      <c r="D162" s="95"/>
+      <c r="A162" s="93"/>
+      <c r="D162" s="94"/>
     </row>
     <row r="163" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A163" s="94"/>
-      <c r="D163" s="95"/>
+      <c r="A163" s="93"/>
+      <c r="D163" s="94"/>
     </row>
     <row r="164" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A164" s="94"/>
-      <c r="D164" s="95"/>
+      <c r="A164" s="93"/>
+      <c r="D164" s="94"/>
     </row>
     <row r="165" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A165" s="94"/>
-      <c r="D165" s="95"/>
+      <c r="A165" s="93"/>
+      <c r="D165" s="94"/>
     </row>
     <row r="166" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A166" s="94"/>
-      <c r="D166" s="95"/>
+      <c r="A166" s="93"/>
+      <c r="D166" s="94"/>
     </row>
     <row r="167" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A167" s="94"/>
-      <c r="D167" s="95"/>
+      <c r="A167" s="93"/>
+      <c r="D167" s="94"/>
     </row>
     <row r="168" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A168" s="94"/>
-      <c r="D168" s="95"/>
+      <c r="A168" s="93"/>
+      <c r="D168" s="94"/>
     </row>
     <row r="169" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A169" s="94"/>
-      <c r="D169" s="95"/>
+      <c r="A169" s="93"/>
+      <c r="D169" s="94"/>
     </row>
     <row r="170" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A170" s="94"/>
-      <c r="D170" s="95"/>
+      <c r="A170" s="93"/>
+      <c r="D170" s="94"/>
     </row>
     <row r="171" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A171" s="94"/>
-      <c r="D171" s="95"/>
+      <c r="A171" s="93"/>
+      <c r="D171" s="94"/>
     </row>
     <row r="172" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A172" s="94"/>
-      <c r="D172" s="95"/>
+      <c r="A172" s="93"/>
+      <c r="D172" s="94"/>
     </row>
     <row r="173" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A173" s="94"/>
-      <c r="D173" s="95"/>
+      <c r="A173" s="93"/>
+      <c r="D173" s="94"/>
     </row>
     <row r="174" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A174" s="94"/>
-      <c r="D174" s="95"/>
+      <c r="A174" s="93"/>
+      <c r="D174" s="94"/>
     </row>
     <row r="175" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A175" s="94"/>
-      <c r="D175" s="95"/>
+      <c r="A175" s="93"/>
+      <c r="D175" s="94"/>
     </row>
     <row r="176" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A176" s="94"/>
-      <c r="D176" s="95"/>
+      <c r="A176" s="93"/>
+      <c r="D176" s="94"/>
     </row>
     <row r="177" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A177" s="94"/>
-      <c r="D177" s="95"/>
+      <c r="A177" s="93"/>
+      <c r="D177" s="94"/>
     </row>
     <row r="178" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A178" s="94"/>
-      <c r="D178" s="95"/>
+      <c r="A178" s="93"/>
+      <c r="D178" s="94"/>
     </row>
     <row r="179" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A179" s="94"/>
-      <c r="D179" s="95"/>
+      <c r="A179" s="93"/>
+      <c r="D179" s="94"/>
     </row>
     <row r="180" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A180" s="94"/>
-      <c r="D180" s="95"/>
+      <c r="A180" s="93"/>
+      <c r="D180" s="94"/>
     </row>
     <row r="181" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A181" s="94"/>
-      <c r="D181" s="95"/>
+      <c r="A181" s="93"/>
+      <c r="D181" s="94"/>
     </row>
     <row r="182" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A182" s="94"/>
-      <c r="D182" s="95"/>
+      <c r="A182" s="93"/>
+      <c r="D182" s="94"/>
     </row>
     <row r="183" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A183" s="94"/>
-      <c r="D183" s="95"/>
+      <c r="A183" s="93"/>
+      <c r="D183" s="94"/>
     </row>
     <row r="184" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A184" s="94"/>
-      <c r="D184" s="95"/>
+      <c r="A184" s="93"/>
+      <c r="D184" s="94"/>
     </row>
     <row r="185" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A185" s="94"/>
-      <c r="D185" s="95"/>
+      <c r="A185" s="93"/>
+      <c r="D185" s="94"/>
     </row>
     <row r="186" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A186" s="94"/>
-      <c r="D186" s="95"/>
+      <c r="A186" s="93"/>
+      <c r="D186" s="94"/>
     </row>
     <row r="187" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A187" s="94"/>
-      <c r="D187" s="95"/>
+      <c r="A187" s="93"/>
+      <c r="D187" s="94"/>
     </row>
     <row r="188" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A188" s="94"/>
-      <c r="D188" s="95"/>
+      <c r="A188" s="93"/>
+      <c r="D188" s="94"/>
     </row>
     <row r="189" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A189" s="94"/>
-      <c r="D189" s="95"/>
+      <c r="A189" s="93"/>
+      <c r="D189" s="94"/>
     </row>
     <row r="190" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A190" s="94"/>
-      <c r="D190" s="95"/>
+      <c r="A190" s="93"/>
+      <c r="D190" s="94"/>
     </row>
     <row r="191" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A191" s="94"/>
-      <c r="D191" s="95"/>
+      <c r="A191" s="93"/>
+      <c r="D191" s="94"/>
     </row>
     <row r="192" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A192" s="94"/>
-      <c r="D192" s="95"/>
+      <c r="A192" s="93"/>
+      <c r="D192" s="94"/>
     </row>
     <row r="193" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A193" s="94"/>
-      <c r="D193" s="95"/>
+      <c r="A193" s="93"/>
+      <c r="D193" s="94"/>
     </row>
     <row r="194" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A194" s="94"/>
-      <c r="D194" s="95"/>
+      <c r="A194" s="93"/>
+      <c r="D194" s="94"/>
     </row>
     <row r="195" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A195" s="94"/>
-      <c r="D195" s="95"/>
+      <c r="A195" s="93"/>
+      <c r="D195" s="94"/>
     </row>
     <row r="196" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A196" s="94"/>
-      <c r="D196" s="95"/>
+      <c r="A196" s="93"/>
+      <c r="D196" s="94"/>
     </row>
     <row r="197" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A197" s="94"/>
-      <c r="D197" s="95"/>
+      <c r="A197" s="93"/>
+      <c r="D197" s="94"/>
     </row>
     <row r="198" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A198" s="94"/>
-      <c r="D198" s="95"/>
+      <c r="A198" s="93"/>
+      <c r="D198" s="94"/>
     </row>
     <row r="199" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A199" s="94"/>
-      <c r="D199" s="95"/>
+      <c r="A199" s="93"/>
+      <c r="D199" s="94"/>
     </row>
     <row r="200" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A200" s="94"/>
-      <c r="D200" s="95"/>
+      <c r="A200" s="93"/>
+      <c r="D200" s="94"/>
     </row>
     <row r="201" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A201" s="94"/>
-      <c r="D201" s="95"/>
+      <c r="A201" s="93"/>
+      <c r="D201" s="94"/>
     </row>
     <row r="202" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A202" s="94"/>
-      <c r="D202" s="95"/>
+      <c r="A202" s="93"/>
+      <c r="D202" s="94"/>
     </row>
     <row r="203" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A203" s="94"/>
-      <c r="D203" s="95"/>
+      <c r="A203" s="93"/>
+      <c r="D203" s="94"/>
     </row>
     <row r="204" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A204" s="94"/>
-      <c r="D204" s="95"/>
+      <c r="A204" s="93"/>
+      <c r="D204" s="94"/>
     </row>
     <row r="205" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A205" s="94"/>
-      <c r="D205" s="95"/>
+      <c r="A205" s="93"/>
+      <c r="D205" s="94"/>
     </row>
     <row r="206" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A206" s="94"/>
-      <c r="D206" s="95"/>
+      <c r="A206" s="93"/>
+      <c r="D206" s="94"/>
     </row>
     <row r="207" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A207" s="94"/>
-      <c r="D207" s="95"/>
+      <c r="A207" s="93"/>
+      <c r="D207" s="94"/>
     </row>
     <row r="208" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A208" s="94"/>
-      <c r="D208" s="95"/>
+      <c r="A208" s="93"/>
+      <c r="D208" s="94"/>
     </row>
     <row r="209" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A209" s="94"/>
-      <c r="D209" s="95"/>
+      <c r="A209" s="93"/>
+      <c r="D209" s="94"/>
     </row>
     <row r="210" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A210" s="94"/>
-      <c r="D210" s="95"/>
+      <c r="A210" s="93"/>
+      <c r="D210" s="94"/>
     </row>
     <row r="211" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A211" s="94"/>
-      <c r="D211" s="95"/>
+      <c r="A211" s="93"/>
+      <c r="D211" s="94"/>
     </row>
     <row r="212" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A212" s="94"/>
-      <c r="D212" s="95"/>
+      <c r="A212" s="93"/>
+      <c r="D212" s="94"/>
     </row>
     <row r="213" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A213" s="94"/>
-      <c r="D213" s="95"/>
+      <c r="A213" s="93"/>
+      <c r="D213" s="94"/>
     </row>
     <row r="214" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A214" s="94"/>
-      <c r="D214" s="95"/>
+      <c r="A214" s="93"/>
+      <c r="D214" s="94"/>
     </row>
     <row r="215" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A215" s="94"/>
-      <c r="D215" s="95"/>
+      <c r="A215" s="93"/>
+      <c r="D215" s="94"/>
     </row>
     <row r="216" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A216" s="94"/>
-      <c r="D216" s="95"/>
+      <c r="A216" s="93"/>
+      <c r="D216" s="94"/>
     </row>
     <row r="217" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A217" s="94"/>
-      <c r="D217" s="95"/>
+      <c r="A217" s="93"/>
+      <c r="D217" s="94"/>
     </row>
     <row r="218" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A218" s="94"/>
-      <c r="D218" s="95"/>
+      <c r="A218" s="93"/>
+      <c r="D218" s="94"/>
     </row>
     <row r="219" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A219" s="94"/>
-      <c r="D219" s="95"/>
+      <c r="A219" s="93"/>
+      <c r="D219" s="94"/>
     </row>
     <row r="220" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A220" s="94"/>
-      <c r="D220" s="95"/>
+      <c r="A220" s="93"/>
+      <c r="D220" s="94"/>
     </row>
     <row r="221" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A221" s="94"/>
-      <c r="D221" s="95"/>
+      <c r="A221" s="93"/>
+      <c r="D221" s="94"/>
     </row>
     <row r="222" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A222" s="94"/>
-      <c r="D222" s="95"/>
+      <c r="A222" s="93"/>
+      <c r="D222" s="94"/>
     </row>
     <row r="223" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A223" s="94"/>
-      <c r="D223" s="95"/>
+      <c r="A223" s="93"/>
+      <c r="D223" s="94"/>
     </row>
     <row r="224" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A224" s="94"/>
-      <c r="D224" s="95"/>
+      <c r="A224" s="93"/>
+      <c r="D224" s="94"/>
     </row>
     <row r="225" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A225" s="94"/>
-      <c r="D225" s="95"/>
+      <c r="A225" s="93"/>
+      <c r="D225" s="94"/>
     </row>
     <row r="226" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A226" s="94"/>
-      <c r="D226" s="95"/>
+      <c r="A226" s="93"/>
+      <c r="D226" s="94"/>
     </row>
     <row r="227" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A227" s="94"/>
-      <c r="D227" s="95"/>
+      <c r="A227" s="93"/>
+      <c r="D227" s="94"/>
     </row>
     <row r="228" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A228" s="94"/>
-      <c r="D228" s="95"/>
+      <c r="A228" s="93"/>
+      <c r="D228" s="94"/>
     </row>
     <row r="229" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A229" s="94"/>
-      <c r="D229" s="95"/>
+      <c r="A229" s="93"/>
+      <c r="D229" s="94"/>
     </row>
     <row r="230" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A230" s="94"/>
-      <c r="D230" s="95"/>
+      <c r="A230" s="93"/>
+      <c r="D230" s="94"/>
     </row>
     <row r="231" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A231" s="94"/>
-      <c r="D231" s="95"/>
+      <c r="A231" s="93"/>
+      <c r="D231" s="94"/>
     </row>
     <row r="232" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A232" s="94"/>
-      <c r="D232" s="95"/>
+      <c r="A232" s="93"/>
+      <c r="D232" s="94"/>
     </row>
     <row r="233" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A233" s="94"/>
-      <c r="D233" s="95"/>
+      <c r="A233" s="93"/>
+      <c r="D233" s="94"/>
     </row>
     <row r="234" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A234" s="94"/>
-      <c r="D234" s="95"/>
+      <c r="A234" s="93"/>
+      <c r="D234" s="94"/>
     </row>
     <row r="235" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A235" s="94"/>
-      <c r="D235" s="95"/>
+      <c r="A235" s="93"/>
+      <c r="D235" s="94"/>
     </row>
     <row r="236" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A236" s="94"/>
-      <c r="D236" s="95"/>
+      <c r="A236" s="93"/>
+      <c r="D236" s="94"/>
     </row>
     <row r="237" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A237" s="94"/>
-      <c r="D237" s="95"/>
+      <c r="A237" s="93"/>
+      <c r="D237" s="94"/>
     </row>
     <row r="238" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A238" s="94"/>
-      <c r="D238" s="95"/>
+      <c r="A238" s="93"/>
+      <c r="D238" s="94"/>
     </row>
     <row r="239" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A239" s="94"/>
-      <c r="D239" s="95"/>
+      <c r="A239" s="93"/>
+      <c r="D239" s="94"/>
     </row>
     <row r="240" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A240" s="94"/>
-      <c r="D240" s="95"/>
+      <c r="A240" s="93"/>
+      <c r="D240" s="94"/>
     </row>
     <row r="241" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A241" s="94"/>
-      <c r="D241" s="95"/>
+      <c r="A241" s="93"/>
+      <c r="D241" s="94"/>
     </row>
     <row r="242" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A242" s="94"/>
-      <c r="D242" s="95"/>
+      <c r="A242" s="93"/>
+      <c r="D242" s="94"/>
     </row>
     <row r="243" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A243" s="94"/>
-      <c r="D243" s="95"/>
+      <c r="A243" s="93"/>
+      <c r="D243" s="94"/>
     </row>
     <row r="244" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A244" s="94"/>
-      <c r="D244" s="95"/>
+      <c r="A244" s="93"/>
+      <c r="D244" s="94"/>
     </row>
     <row r="245" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A245" s="94"/>
-      <c r="D245" s="95"/>
+      <c r="A245" s="93"/>
+      <c r="D245" s="94"/>
     </row>
     <row r="246" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A246" s="94"/>
-      <c r="D246" s="95"/>
+      <c r="A246" s="93"/>
+      <c r="D246" s="94"/>
     </row>
     <row r="247" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A247" s="94"/>
-      <c r="D247" s="95"/>
+      <c r="A247" s="93"/>
+      <c r="D247" s="94"/>
     </row>
     <row r="248" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A248" s="94"/>
-      <c r="D248" s="95"/>
+      <c r="A248" s="93"/>
+      <c r="D248" s="94"/>
     </row>
     <row r="249" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A249" s="94"/>
-      <c r="D249" s="95"/>
+      <c r="A249" s="93"/>
+      <c r="D249" s="94"/>
     </row>
     <row r="250" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A250" s="94"/>
-      <c r="D250" s="95"/>
+      <c r="A250" s="93"/>
+      <c r="D250" s="94"/>
     </row>
     <row r="251" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A251" s="94"/>
-      <c r="D251" s="95"/>
+      <c r="A251" s="93"/>
+      <c r="D251" s="94"/>
     </row>
     <row r="252" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A252" s="94"/>
-      <c r="D252" s="95"/>
+      <c r="A252" s="93"/>
+      <c r="D252" s="94"/>
     </row>
     <row r="253" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A253" s="94"/>
-      <c r="D253" s="95"/>
+      <c r="A253" s="93"/>
+      <c r="D253" s="94"/>
     </row>
     <row r="254" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A254" s="94"/>
-      <c r="D254" s="95"/>
+      <c r="A254" s="93"/>
+      <c r="D254" s="94"/>
     </row>
     <row r="255" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A255" s="94"/>
-      <c r="D255" s="95"/>
+      <c r="A255" s="93"/>
+      <c r="D255" s="94"/>
     </row>
     <row r="256" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A256" s="94"/>
-      <c r="D256" s="95"/>
+      <c r="A256" s="93"/>
+      <c r="D256" s="94"/>
     </row>
     <row r="257" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A257" s="94"/>
-      <c r="D257" s="95"/>
+      <c r="A257" s="93"/>
+      <c r="D257" s="94"/>
     </row>
     <row r="258" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A258" s="94"/>
-      <c r="D258" s="95"/>
+      <c r="A258" s="93"/>
+      <c r="D258" s="94"/>
     </row>
     <row r="259" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A259" s="94"/>
-      <c r="D259" s="95"/>
+      <c r="A259" s="93"/>
+      <c r="D259" s="94"/>
     </row>
     <row r="260" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A260" s="94"/>
-      <c r="D260" s="95"/>
+      <c r="A260" s="93"/>
+      <c r="D260" s="94"/>
     </row>
     <row r="261" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A261" s="94"/>
-      <c r="D261" s="95"/>
+      <c r="A261" s="93"/>
+      <c r="D261" s="94"/>
     </row>
     <row r="262" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A262" s="94"/>
-      <c r="D262" s="95"/>
+      <c r="A262" s="93"/>
+      <c r="D262" s="94"/>
     </row>
     <row r="263" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A263" s="94"/>
-      <c r="D263" s="95"/>
+      <c r="A263" s="93"/>
+      <c r="D263" s="94"/>
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="265" spans="1:4" ht="15.75" customHeight="1"/>
@@ -9611,40 +9623,37 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="AT40:BD40"/>
-    <mergeCell ref="AL35:AQ35"/>
-    <mergeCell ref="AP36:AY36"/>
-    <mergeCell ref="AV37:BF37"/>
-    <mergeCell ref="AR38:BB38"/>
-    <mergeCell ref="AS39:BC39"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AN31:AS31"/>
-    <mergeCell ref="AI32:AN32"/>
-    <mergeCell ref="AJ33:AO33"/>
-    <mergeCell ref="AK34:AP34"/>
-    <mergeCell ref="AC23:AK23"/>
-    <mergeCell ref="AD24:AJ24"/>
-    <mergeCell ref="AI25:AK25"/>
-    <mergeCell ref="AE26:AJ26"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="AD27:AK27"/>
-    <mergeCell ref="AG28:AK28"/>
-    <mergeCell ref="G29:CE29"/>
-    <mergeCell ref="T18:Z18"/>
-    <mergeCell ref="V19:AA19"/>
-    <mergeCell ref="G20:CE20"/>
-    <mergeCell ref="AA21:AH21"/>
-    <mergeCell ref="AB22:AG22"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="P15:T15"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="AN31:AY31"/>
+    <mergeCell ref="AP36:AZ36"/>
+    <mergeCell ref="AU45:BC45"/>
+    <mergeCell ref="AV41:AZ41"/>
+    <mergeCell ref="AW42:BF42"/>
+    <mergeCell ref="AV43:BC43"/>
+    <mergeCell ref="AU44:BA44"/>
+    <mergeCell ref="AY46:BE46"/>
+    <mergeCell ref="AV47:BA47"/>
+    <mergeCell ref="AY48:BC48"/>
+    <mergeCell ref="BA49:BD49"/>
+    <mergeCell ref="AU50:AZ50"/>
+    <mergeCell ref="BA51:BF51"/>
+    <mergeCell ref="G52:CE52"/>
+    <mergeCell ref="BB53:BE53"/>
+    <mergeCell ref="BF54:BJ54"/>
+    <mergeCell ref="BN62:BT62"/>
+    <mergeCell ref="BP63:BT63"/>
+    <mergeCell ref="G64:CE64"/>
+    <mergeCell ref="BE55:BL55"/>
+    <mergeCell ref="BF56:BL56"/>
+    <mergeCell ref="BJ57:BO57"/>
+    <mergeCell ref="BK58:BS58"/>
+    <mergeCell ref="BL59:BQ59"/>
+    <mergeCell ref="BM60:BS60"/>
+    <mergeCell ref="BM61:BQ61"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
     <mergeCell ref="BD4:BJ4"/>
     <mergeCell ref="BK4:BQ4"/>
     <mergeCell ref="BR4:BX4"/>
@@ -9655,35 +9664,38 @@
     <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="AP4:AV4"/>
     <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="BP63:BT63"/>
-    <mergeCell ref="G64:CE64"/>
-    <mergeCell ref="BE55:BL55"/>
-    <mergeCell ref="BF56:BL56"/>
-    <mergeCell ref="BJ57:BO57"/>
-    <mergeCell ref="BK58:BS58"/>
-    <mergeCell ref="BL59:BQ59"/>
-    <mergeCell ref="BM60:BS60"/>
-    <mergeCell ref="BM61:BQ61"/>
-    <mergeCell ref="BA51:BF51"/>
-    <mergeCell ref="G52:CE52"/>
-    <mergeCell ref="BB53:BE53"/>
-    <mergeCell ref="BF54:BJ54"/>
-    <mergeCell ref="BN62:BT62"/>
-    <mergeCell ref="AY46:BE46"/>
-    <mergeCell ref="AV47:BA47"/>
-    <mergeCell ref="AY48:BC48"/>
-    <mergeCell ref="BA49:BD49"/>
-    <mergeCell ref="AU50:AZ50"/>
-    <mergeCell ref="AV41:AZ41"/>
-    <mergeCell ref="AW42:BF42"/>
-    <mergeCell ref="AV43:BC43"/>
-    <mergeCell ref="AU44:BA44"/>
-    <mergeCell ref="AS45:AY45"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="P15:T15"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="T18:Z18"/>
+    <mergeCell ref="V19:AA19"/>
+    <mergeCell ref="G20:CE20"/>
+    <mergeCell ref="AA21:AH21"/>
+    <mergeCell ref="AB22:AG22"/>
+    <mergeCell ref="AC23:AK23"/>
+    <mergeCell ref="AD24:AJ24"/>
+    <mergeCell ref="AI25:AK25"/>
+    <mergeCell ref="AE26:AJ26"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="AD27:AK27"/>
+    <mergeCell ref="AG28:AK28"/>
+    <mergeCell ref="G29:CE29"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AI32:AN32"/>
+    <mergeCell ref="AJ33:AO33"/>
+    <mergeCell ref="AK34:AP34"/>
+    <mergeCell ref="AT40:BD40"/>
+    <mergeCell ref="AL35:AQ35"/>
+    <mergeCell ref="AV37:BF37"/>
+    <mergeCell ref="AR38:BB38"/>
+    <mergeCell ref="AS39:BC39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.34722222222222199" header="0" footer="0"/>

</xml_diff>

<commit_message>
Replace Gantt-diagram-A.xlsx, mivel már nincs email-es kiértesítés c:
</commit_message>
<xml_diff>
--- a/Gantt-diagram-A.xlsx
+++ b/Gantt-diagram-A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szabó Tímea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timea\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D10D83-60D8-4E19-BD23-021E1A75E60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ECD39A-86CC-4F9B-842B-4E6E30EAE054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt-diagram" sheetId="1" r:id="rId1"/>
@@ -242,9 +242,6 @@
     <t>8.4.7. Időpont foglalás kezelésének tesztelése (TR)</t>
   </si>
   <si>
-    <t>8.4.8. Email-es funkciók tesztelése (TR)</t>
-  </si>
-  <si>
     <t>8.4.9. Biztonsági mentés tesztelése (TR)</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>8.3.20. Deploy</t>
+  </si>
+  <si>
+    <t>8.4.8. Profil funkciók tesztelése (TR)</t>
   </si>
 </sst>
 </file>
@@ -1562,88 +1562,77 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1652,39 +1641,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1907,18 +1907,18 @@
   </sheetPr>
   <dimension ref="A1:CE1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR45" sqref="AR45"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.109375" customWidth="1"/>
-    <col min="2" max="2" width="80.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="83" width="2.44140625" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="83" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" ht="25.5" customHeight="1">
@@ -2021,10 +2021,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="147" t="s">
+      <c r="D2" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="148"/>
+      <c r="E2" s="141"/>
       <c r="F2" s="5"/>
       <c r="G2" s="18"/>
       <c r="H2" s="6"/>
@@ -2108,10 +2108,10 @@
       <c r="A3" s="16"/>
       <c r="B3" s="19"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="147">
+      <c r="D3" s="140">
         <v>45197</v>
       </c>
-      <c r="E3" s="148"/>
+      <c r="E3" s="141"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -2197,7 +2197,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="149"/>
+      <c r="F4" s="142"/>
       <c r="G4" s="144">
         <f>G5</f>
         <v>45194</v>
@@ -2323,7 +2323,7 @@
       <c r="E5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="150"/>
+      <c r="F5" s="143"/>
       <c r="G5" s="22">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2</f>
         <v>45194</v>
@@ -2727,83 +2727,83 @@
       <c r="D7" s="31"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="139"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
-      <c r="T7" s="133"/>
-      <c r="U7" s="133"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="133"/>
-      <c r="AB7" s="133"/>
-      <c r="AC7" s="133"/>
-      <c r="AD7" s="133"/>
-      <c r="AE7" s="133"/>
-      <c r="AF7" s="133"/>
-      <c r="AG7" s="133"/>
-      <c r="AH7" s="133"/>
-      <c r="AI7" s="133"/>
-      <c r="AJ7" s="133"/>
-      <c r="AK7" s="133"/>
-      <c r="AL7" s="133"/>
-      <c r="AM7" s="133"/>
-      <c r="AN7" s="133"/>
-      <c r="AO7" s="133"/>
-      <c r="AP7" s="133"/>
-      <c r="AQ7" s="133"/>
-      <c r="AR7" s="133"/>
-      <c r="AS7" s="133"/>
-      <c r="AT7" s="133"/>
-      <c r="AU7" s="133"/>
-      <c r="AV7" s="133"/>
-      <c r="AW7" s="133"/>
-      <c r="AX7" s="133"/>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="133"/>
-      <c r="BA7" s="133"/>
-      <c r="BB7" s="133"/>
-      <c r="BC7" s="133"/>
-      <c r="BD7" s="133"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="133"/>
-      <c r="BG7" s="133"/>
-      <c r="BH7" s="133"/>
-      <c r="BI7" s="133"/>
-      <c r="BJ7" s="133"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="133"/>
-      <c r="BM7" s="133"/>
-      <c r="BN7" s="133"/>
-      <c r="BO7" s="133"/>
-      <c r="BP7" s="133"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="133"/>
-      <c r="BS7" s="133"/>
-      <c r="BT7" s="133"/>
-      <c r="BU7" s="133"/>
-      <c r="BV7" s="133"/>
-      <c r="BW7" s="133"/>
-      <c r="BX7" s="133"/>
-      <c r="BY7" s="133"/>
-      <c r="BZ7" s="133"/>
-      <c r="CA7" s="133"/>
-      <c r="CB7" s="133"/>
-      <c r="CC7" s="133"/>
-      <c r="CD7" s="133"/>
-      <c r="CE7" s="134"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="132"/>
+      <c r="T7" s="132"/>
+      <c r="U7" s="132"/>
+      <c r="V7" s="132"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="132"/>
+      <c r="Y7" s="132"/>
+      <c r="Z7" s="132"/>
+      <c r="AA7" s="132"/>
+      <c r="AB7" s="132"/>
+      <c r="AC7" s="132"/>
+      <c r="AD7" s="132"/>
+      <c r="AE7" s="132"/>
+      <c r="AF7" s="132"/>
+      <c r="AG7" s="132"/>
+      <c r="AH7" s="132"/>
+      <c r="AI7" s="132"/>
+      <c r="AJ7" s="132"/>
+      <c r="AK7" s="132"/>
+      <c r="AL7" s="132"/>
+      <c r="AM7" s="132"/>
+      <c r="AN7" s="132"/>
+      <c r="AO7" s="132"/>
+      <c r="AP7" s="132"/>
+      <c r="AQ7" s="132"/>
+      <c r="AR7" s="132"/>
+      <c r="AS7" s="132"/>
+      <c r="AT7" s="132"/>
+      <c r="AU7" s="132"/>
+      <c r="AV7" s="132"/>
+      <c r="AW7" s="132"/>
+      <c r="AX7" s="132"/>
+      <c r="AY7" s="132"/>
+      <c r="AZ7" s="132"/>
+      <c r="BA7" s="132"/>
+      <c r="BB7" s="132"/>
+      <c r="BC7" s="132"/>
+      <c r="BD7" s="132"/>
+      <c r="BE7" s="132"/>
+      <c r="BF7" s="132"/>
+      <c r="BG7" s="132"/>
+      <c r="BH7" s="132"/>
+      <c r="BI7" s="132"/>
+      <c r="BJ7" s="132"/>
+      <c r="BK7" s="132"/>
+      <c r="BL7" s="132"/>
+      <c r="BM7" s="132"/>
+      <c r="BN7" s="132"/>
+      <c r="BO7" s="132"/>
+      <c r="BP7" s="132"/>
+      <c r="BQ7" s="132"/>
+      <c r="BR7" s="132"/>
+      <c r="BS7" s="132"/>
+      <c r="BT7" s="132"/>
+      <c r="BU7" s="132"/>
+      <c r="BV7" s="132"/>
+      <c r="BW7" s="132"/>
+      <c r="BX7" s="132"/>
+      <c r="BY7" s="132"/>
+      <c r="BZ7" s="132"/>
+      <c r="CA7" s="132"/>
+      <c r="CB7" s="132"/>
+      <c r="CC7" s="132"/>
+      <c r="CD7" s="132"/>
+      <c r="CE7" s="133"/>
     </row>
     <row r="8" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
@@ -2823,8 +2823,8 @@
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
       <c r="I8" s="45"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="125"/>
+      <c r="J8" s="148"/>
+      <c r="K8" s="129"/>
       <c r="L8" s="105"/>
       <c r="M8" s="40"/>
       <c r="N8" s="38"/>
@@ -2916,9 +2916,9 @@
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
       <c r="I9" s="45"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="125"/>
+      <c r="J9" s="148"/>
+      <c r="K9" s="128"/>
+      <c r="L9" s="129"/>
       <c r="M9" s="46"/>
       <c r="N9" s="38"/>
       <c r="O9" s="38"/>
@@ -3011,8 +3011,8 @@
       <c r="I10" s="38"/>
       <c r="J10" s="103"/>
       <c r="K10" s="104"/>
-      <c r="L10" s="142"/>
-      <c r="M10" s="125"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="129"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
       <c r="P10" s="38"/>
@@ -3103,8 +3103,8 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
       <c r="J11" s="45"/>
-      <c r="K11" s="111"/>
-      <c r="L11" s="113"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="150"/>
       <c r="M11" s="48"/>
       <c r="N11" s="41"/>
       <c r="O11" s="41"/>
@@ -3199,10 +3199,10 @@
       <c r="K12" s="47"/>
       <c r="L12" s="39"/>
       <c r="M12" s="49"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-      <c r="Q12" s="125"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="128"/>
+      <c r="P12" s="128"/>
+      <c r="Q12" s="129"/>
       <c r="R12" s="38"/>
       <c r="S12" s="40"/>
       <c r="T12" s="40"/>
@@ -3290,11 +3290,11 @@
       <c r="I13" s="38"/>
       <c r="J13" s="41"/>
       <c r="K13" s="50"/>
-      <c r="L13" s="138"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="139"/>
-      <c r="O13" s="139"/>
-      <c r="P13" s="140"/>
+      <c r="L13" s="151"/>
+      <c r="M13" s="119"/>
+      <c r="N13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="152"/>
       <c r="Q13" s="55"/>
       <c r="R13" s="41"/>
       <c r="S13" s="40"/>
@@ -3385,11 +3385,11 @@
       <c r="K14" s="38"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51"/>
-      <c r="N14" s="122"/>
-      <c r="O14" s="112"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112"/>
-      <c r="R14" s="115"/>
+      <c r="N14" s="115"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="114"/>
       <c r="S14" s="46"/>
       <c r="T14" s="39"/>
       <c r="U14" s="41"/>
@@ -3480,11 +3480,11 @@
       <c r="M15" s="40"/>
       <c r="N15" s="47"/>
       <c r="O15" s="52"/>
-      <c r="P15" s="117"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="112"/>
-      <c r="S15" s="112"/>
-      <c r="T15" s="110"/>
+      <c r="P15" s="153"/>
+      <c r="Q15" s="113"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="120"/>
       <c r="U15" s="101"/>
       <c r="V15" s="101"/>
       <c r="W15" s="99"/>
@@ -3577,11 +3577,11 @@
       <c r="Q16" s="47"/>
       <c r="R16" s="47"/>
       <c r="S16" s="51"/>
-      <c r="T16" s="123"/>
-      <c r="U16" s="124"/>
-      <c r="V16" s="124"/>
-      <c r="W16" s="124"/>
-      <c r="X16" s="125"/>
+      <c r="T16" s="154"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
+      <c r="W16" s="128"/>
+      <c r="X16" s="129"/>
       <c r="Y16" s="41"/>
       <c r="Z16" s="53"/>
       <c r="AA16" s="43"/>
@@ -3674,9 +3674,9 @@
       <c r="U17" s="55"/>
       <c r="V17" s="55"/>
       <c r="W17" s="56"/>
-      <c r="X17" s="141"/>
-      <c r="Y17" s="112"/>
-      <c r="Z17" s="115"/>
+      <c r="X17" s="155"/>
+      <c r="Y17" s="113"/>
+      <c r="Z17" s="114"/>
       <c r="AA17" s="43"/>
       <c r="AB17" s="28"/>
       <c r="AC17" s="28"/>
@@ -3763,13 +3763,13 @@
       <c r="Q18" s="38"/>
       <c r="R18" s="38"/>
       <c r="S18" s="51"/>
-      <c r="T18" s="130"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
-      <c r="X18" s="112"/>
-      <c r="Y18" s="112"/>
-      <c r="Z18" s="115"/>
+      <c r="T18" s="139"/>
+      <c r="U18" s="113"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="113"/>
+      <c r="X18" s="113"/>
+      <c r="Y18" s="113"/>
+      <c r="Z18" s="114"/>
       <c r="AA18" s="43"/>
       <c r="AB18" s="28"/>
       <c r="AC18" s="28"/>
@@ -3859,12 +3859,12 @@
       <c r="S19" s="40"/>
       <c r="T19" s="40"/>
       <c r="U19" s="57"/>
-      <c r="V19" s="135"/>
-      <c r="W19" s="120"/>
-      <c r="X19" s="120"/>
-      <c r="Y19" s="120"/>
-      <c r="Z19" s="120"/>
-      <c r="AA19" s="136"/>
+      <c r="V19" s="156"/>
+      <c r="W19" s="122"/>
+      <c r="X19" s="122"/>
+      <c r="Y19" s="122"/>
+      <c r="Z19" s="122"/>
+      <c r="AA19" s="157"/>
       <c r="AB19" s="28"/>
       <c r="AC19" s="28"/>
       <c r="AD19" s="28"/>
@@ -3931,83 +3931,83 @@
       <c r="D20" s="60"/>
       <c r="E20" s="61"/>
       <c r="F20" s="37"/>
-      <c r="G20" s="132"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="133"/>
-      <c r="L20" s="133"/>
-      <c r="M20" s="133"/>
-      <c r="N20" s="133"/>
-      <c r="O20" s="133"/>
-      <c r="P20" s="133"/>
-      <c r="Q20" s="133"/>
-      <c r="R20" s="133"/>
-      <c r="S20" s="133"/>
-      <c r="T20" s="133"/>
-      <c r="U20" s="133"/>
-      <c r="V20" s="133"/>
-      <c r="W20" s="133"/>
-      <c r="X20" s="133"/>
-      <c r="Y20" s="133"/>
-      <c r="Z20" s="133"/>
-      <c r="AA20" s="133"/>
-      <c r="AB20" s="133"/>
-      <c r="AC20" s="133"/>
-      <c r="AD20" s="133"/>
-      <c r="AE20" s="133"/>
-      <c r="AF20" s="133"/>
-      <c r="AG20" s="133"/>
-      <c r="AH20" s="133"/>
-      <c r="AI20" s="133"/>
-      <c r="AJ20" s="133"/>
-      <c r="AK20" s="133"/>
-      <c r="AL20" s="133"/>
-      <c r="AM20" s="133"/>
-      <c r="AN20" s="133"/>
-      <c r="AO20" s="133"/>
-      <c r="AP20" s="133"/>
-      <c r="AQ20" s="133"/>
-      <c r="AR20" s="133"/>
-      <c r="AS20" s="133"/>
-      <c r="AT20" s="133"/>
-      <c r="AU20" s="133"/>
-      <c r="AV20" s="133"/>
-      <c r="AW20" s="133"/>
-      <c r="AX20" s="133"/>
-      <c r="AY20" s="133"/>
-      <c r="AZ20" s="133"/>
-      <c r="BA20" s="133"/>
-      <c r="BB20" s="133"/>
-      <c r="BC20" s="133"/>
-      <c r="BD20" s="133"/>
-      <c r="BE20" s="133"/>
-      <c r="BF20" s="133"/>
-      <c r="BG20" s="133"/>
-      <c r="BH20" s="133"/>
-      <c r="BI20" s="133"/>
-      <c r="BJ20" s="133"/>
-      <c r="BK20" s="133"/>
-      <c r="BL20" s="133"/>
-      <c r="BM20" s="133"/>
-      <c r="BN20" s="133"/>
-      <c r="BO20" s="133"/>
-      <c r="BP20" s="133"/>
-      <c r="BQ20" s="133"/>
-      <c r="BR20" s="133"/>
-      <c r="BS20" s="133"/>
-      <c r="BT20" s="133"/>
-      <c r="BU20" s="133"/>
-      <c r="BV20" s="133"/>
-      <c r="BW20" s="133"/>
-      <c r="BX20" s="133"/>
-      <c r="BY20" s="133"/>
-      <c r="BZ20" s="133"/>
-      <c r="CA20" s="133"/>
-      <c r="CB20" s="133"/>
-      <c r="CC20" s="133"/>
-      <c r="CD20" s="133"/>
-      <c r="CE20" s="134"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="132"/>
+      <c r="L20" s="132"/>
+      <c r="M20" s="132"/>
+      <c r="N20" s="132"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="132"/>
+      <c r="Q20" s="132"/>
+      <c r="R20" s="132"/>
+      <c r="S20" s="132"/>
+      <c r="T20" s="132"/>
+      <c r="U20" s="132"/>
+      <c r="V20" s="132"/>
+      <c r="W20" s="132"/>
+      <c r="X20" s="132"/>
+      <c r="Y20" s="132"/>
+      <c r="Z20" s="132"/>
+      <c r="AA20" s="132"/>
+      <c r="AB20" s="132"/>
+      <c r="AC20" s="132"/>
+      <c r="AD20" s="132"/>
+      <c r="AE20" s="132"/>
+      <c r="AF20" s="132"/>
+      <c r="AG20" s="132"/>
+      <c r="AH20" s="132"/>
+      <c r="AI20" s="132"/>
+      <c r="AJ20" s="132"/>
+      <c r="AK20" s="132"/>
+      <c r="AL20" s="132"/>
+      <c r="AM20" s="132"/>
+      <c r="AN20" s="132"/>
+      <c r="AO20" s="132"/>
+      <c r="AP20" s="132"/>
+      <c r="AQ20" s="132"/>
+      <c r="AR20" s="132"/>
+      <c r="AS20" s="132"/>
+      <c r="AT20" s="132"/>
+      <c r="AU20" s="132"/>
+      <c r="AV20" s="132"/>
+      <c r="AW20" s="132"/>
+      <c r="AX20" s="132"/>
+      <c r="AY20" s="132"/>
+      <c r="AZ20" s="132"/>
+      <c r="BA20" s="132"/>
+      <c r="BB20" s="132"/>
+      <c r="BC20" s="132"/>
+      <c r="BD20" s="132"/>
+      <c r="BE20" s="132"/>
+      <c r="BF20" s="132"/>
+      <c r="BG20" s="132"/>
+      <c r="BH20" s="132"/>
+      <c r="BI20" s="132"/>
+      <c r="BJ20" s="132"/>
+      <c r="BK20" s="132"/>
+      <c r="BL20" s="132"/>
+      <c r="BM20" s="132"/>
+      <c r="BN20" s="132"/>
+      <c r="BO20" s="132"/>
+      <c r="BP20" s="132"/>
+      <c r="BQ20" s="132"/>
+      <c r="BR20" s="132"/>
+      <c r="BS20" s="132"/>
+      <c r="BT20" s="132"/>
+      <c r="BU20" s="132"/>
+      <c r="BV20" s="132"/>
+      <c r="BW20" s="132"/>
+      <c r="BX20" s="132"/>
+      <c r="BY20" s="132"/>
+      <c r="BZ20" s="132"/>
+      <c r="CA20" s="132"/>
+      <c r="CB20" s="132"/>
+      <c r="CC20" s="132"/>
+      <c r="CD20" s="132"/>
+      <c r="CE20" s="133"/>
     </row>
     <row r="21" spans="1:83" ht="15" customHeight="1">
       <c r="A21" s="1"/>
@@ -4044,14 +4044,14 @@
       <c r="X21" s="28"/>
       <c r="Y21" s="28"/>
       <c r="Z21" s="65"/>
-      <c r="AA21" s="117"/>
-      <c r="AB21" s="112"/>
-      <c r="AC21" s="112"/>
-      <c r="AD21" s="112"/>
-      <c r="AE21" s="112"/>
-      <c r="AF21" s="112"/>
-      <c r="AG21" s="112"/>
-      <c r="AH21" s="115"/>
+      <c r="AA21" s="153"/>
+      <c r="AB21" s="113"/>
+      <c r="AC21" s="113"/>
+      <c r="AD21" s="113"/>
+      <c r="AE21" s="113"/>
+      <c r="AF21" s="113"/>
+      <c r="AG21" s="113"/>
+      <c r="AH21" s="114"/>
       <c r="AI21" s="38"/>
       <c r="AJ21" s="28"/>
       <c r="AK21" s="28"/>
@@ -4138,12 +4138,12 @@
       <c r="Y22" s="28"/>
       <c r="Z22" s="44"/>
       <c r="AA22" s="51"/>
-      <c r="AB22" s="137"/>
-      <c r="AC22" s="112"/>
-      <c r="AD22" s="112"/>
-      <c r="AE22" s="112"/>
-      <c r="AF22" s="112"/>
-      <c r="AG22" s="115"/>
+      <c r="AB22" s="134"/>
+      <c r="AC22" s="113"/>
+      <c r="AD22" s="113"/>
+      <c r="AE22" s="113"/>
+      <c r="AF22" s="113"/>
+      <c r="AG22" s="114"/>
       <c r="AH22" s="46"/>
       <c r="AI22" s="42"/>
       <c r="AJ22" s="42"/>
@@ -4232,15 +4232,15 @@
       <c r="Z23" s="44"/>
       <c r="AA23" s="44"/>
       <c r="AB23" s="66"/>
-      <c r="AC23" s="122"/>
-      <c r="AD23" s="118"/>
-      <c r="AE23" s="118"/>
-      <c r="AF23" s="118"/>
-      <c r="AG23" s="118"/>
-      <c r="AH23" s="118"/>
-      <c r="AI23" s="118"/>
-      <c r="AJ23" s="118"/>
-      <c r="AK23" s="115"/>
+      <c r="AC23" s="115"/>
+      <c r="AD23" s="119"/>
+      <c r="AE23" s="119"/>
+      <c r="AF23" s="119"/>
+      <c r="AG23" s="119"/>
+      <c r="AH23" s="119"/>
+      <c r="AI23" s="119"/>
+      <c r="AJ23" s="119"/>
+      <c r="AK23" s="114"/>
       <c r="AL23" s="38"/>
       <c r="AM23" s="28"/>
       <c r="AN23" s="44"/>
@@ -4326,13 +4326,13 @@
       <c r="AA24" s="44"/>
       <c r="AB24" s="28"/>
       <c r="AC24" s="66"/>
-      <c r="AD24" s="123"/>
-      <c r="AE24" s="124"/>
-      <c r="AF24" s="124"/>
-      <c r="AG24" s="124"/>
-      <c r="AH24" s="124"/>
-      <c r="AI24" s="124"/>
-      <c r="AJ24" s="125"/>
+      <c r="AD24" s="154"/>
+      <c r="AE24" s="128"/>
+      <c r="AF24" s="128"/>
+      <c r="AG24" s="128"/>
+      <c r="AH24" s="128"/>
+      <c r="AI24" s="128"/>
+      <c r="AJ24" s="129"/>
       <c r="AK24" s="103"/>
       <c r="AL24" s="28"/>
       <c r="AM24" s="28"/>
@@ -4424,9 +4424,9 @@
       <c r="AF25" s="57"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="66"/>
-      <c r="AI25" s="126"/>
-      <c r="AJ25" s="120"/>
-      <c r="AK25" s="115"/>
+      <c r="AI25" s="158"/>
+      <c r="AJ25" s="122"/>
+      <c r="AK25" s="114"/>
       <c r="AL25" s="38"/>
       <c r="AM25" s="28"/>
       <c r="AN25" s="44"/>
@@ -4513,12 +4513,12 @@
       <c r="AB26" s="28"/>
       <c r="AC26" s="28"/>
       <c r="AD26" s="28"/>
-      <c r="AE26" s="127"/>
-      <c r="AF26" s="112"/>
-      <c r="AG26" s="112"/>
-      <c r="AH26" s="112"/>
-      <c r="AI26" s="112"/>
-      <c r="AJ26" s="115"/>
+      <c r="AE26" s="112"/>
+      <c r="AF26" s="113"/>
+      <c r="AG26" s="113"/>
+      <c r="AH26" s="113"/>
+      <c r="AI26" s="113"/>
+      <c r="AJ26" s="114"/>
       <c r="AK26" s="55"/>
       <c r="AL26" s="28"/>
       <c r="AM26" s="28"/>
@@ -4605,14 +4605,14 @@
       <c r="AA27" s="44"/>
       <c r="AB27" s="28"/>
       <c r="AC27" s="67"/>
-      <c r="AD27" s="130"/>
-      <c r="AE27" s="112"/>
-      <c r="AF27" s="112"/>
-      <c r="AG27" s="118"/>
-      <c r="AH27" s="118"/>
-      <c r="AI27" s="118"/>
-      <c r="AJ27" s="118"/>
-      <c r="AK27" s="110"/>
+      <c r="AD27" s="139"/>
+      <c r="AE27" s="113"/>
+      <c r="AF27" s="113"/>
+      <c r="AG27" s="119"/>
+      <c r="AH27" s="119"/>
+      <c r="AI27" s="119"/>
+      <c r="AJ27" s="119"/>
+      <c r="AK27" s="120"/>
       <c r="AL27" s="38"/>
       <c r="AM27" s="28"/>
       <c r="AN27" s="44"/>
@@ -4674,7 +4674,7 @@
       <c r="E28" s="64">
         <v>45225</v>
       </c>
-      <c r="F28" s="128"/>
+      <c r="F28" s="159"/>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -4701,11 +4701,11 @@
       <c r="AD28" s="57"/>
       <c r="AE28" s="57"/>
       <c r="AF28" s="66"/>
-      <c r="AG28" s="131"/>
-      <c r="AH28" s="124"/>
-      <c r="AI28" s="124"/>
-      <c r="AJ28" s="124"/>
-      <c r="AK28" s="125"/>
+      <c r="AG28" s="148"/>
+      <c r="AH28" s="128"/>
+      <c r="AI28" s="128"/>
+      <c r="AJ28" s="128"/>
+      <c r="AK28" s="129"/>
       <c r="AL28" s="38"/>
       <c r="AM28" s="28"/>
       <c r="AN28" s="44"/>
@@ -4761,84 +4761,84 @@
       <c r="C29" s="69"/>
       <c r="D29" s="70"/>
       <c r="E29" s="71"/>
-      <c r="F29" s="129"/>
-      <c r="G29" s="132"/>
-      <c r="H29" s="133"/>
-      <c r="I29" s="133"/>
-      <c r="J29" s="133"/>
-      <c r="K29" s="133"/>
-      <c r="L29" s="133"/>
-      <c r="M29" s="133"/>
-      <c r="N29" s="133"/>
-      <c r="O29" s="133"/>
-      <c r="P29" s="133"/>
-      <c r="Q29" s="133"/>
-      <c r="R29" s="133"/>
-      <c r="S29" s="133"/>
-      <c r="T29" s="133"/>
-      <c r="U29" s="133"/>
-      <c r="V29" s="133"/>
-      <c r="W29" s="133"/>
-      <c r="X29" s="133"/>
-      <c r="Y29" s="133"/>
-      <c r="Z29" s="133"/>
-      <c r="AA29" s="133"/>
-      <c r="AB29" s="133"/>
-      <c r="AC29" s="133"/>
-      <c r="AD29" s="133"/>
-      <c r="AE29" s="133"/>
-      <c r="AF29" s="133"/>
-      <c r="AG29" s="133"/>
-      <c r="AH29" s="133"/>
-      <c r="AI29" s="133"/>
-      <c r="AJ29" s="133"/>
-      <c r="AK29" s="133"/>
-      <c r="AL29" s="133"/>
-      <c r="AM29" s="133"/>
-      <c r="AN29" s="133"/>
-      <c r="AO29" s="133"/>
-      <c r="AP29" s="133"/>
-      <c r="AQ29" s="133"/>
-      <c r="AR29" s="133"/>
-      <c r="AS29" s="133"/>
-      <c r="AT29" s="133"/>
-      <c r="AU29" s="133"/>
-      <c r="AV29" s="133"/>
-      <c r="AW29" s="133"/>
-      <c r="AX29" s="133"/>
-      <c r="AY29" s="133"/>
-      <c r="AZ29" s="133"/>
-      <c r="BA29" s="133"/>
-      <c r="BB29" s="133"/>
-      <c r="BC29" s="133"/>
-      <c r="BD29" s="133"/>
-      <c r="BE29" s="133"/>
-      <c r="BF29" s="133"/>
-      <c r="BG29" s="133"/>
-      <c r="BH29" s="133"/>
-      <c r="BI29" s="133"/>
-      <c r="BJ29" s="133"/>
-      <c r="BK29" s="133"/>
-      <c r="BL29" s="133"/>
-      <c r="BM29" s="133"/>
-      <c r="BN29" s="133"/>
-      <c r="BO29" s="133"/>
-      <c r="BP29" s="133"/>
-      <c r="BQ29" s="133"/>
-      <c r="BR29" s="133"/>
-      <c r="BS29" s="133"/>
-      <c r="BT29" s="133"/>
-      <c r="BU29" s="133"/>
-      <c r="BV29" s="133"/>
-      <c r="BW29" s="133"/>
-      <c r="BX29" s="133"/>
-      <c r="BY29" s="133"/>
-      <c r="BZ29" s="133"/>
-      <c r="CA29" s="133"/>
-      <c r="CB29" s="133"/>
-      <c r="CC29" s="133"/>
-      <c r="CD29" s="133"/>
-      <c r="CE29" s="134"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="132"/>
+      <c r="K29" s="132"/>
+      <c r="L29" s="132"/>
+      <c r="M29" s="132"/>
+      <c r="N29" s="132"/>
+      <c r="O29" s="132"/>
+      <c r="P29" s="132"/>
+      <c r="Q29" s="132"/>
+      <c r="R29" s="132"/>
+      <c r="S29" s="132"/>
+      <c r="T29" s="132"/>
+      <c r="U29" s="132"/>
+      <c r="V29" s="132"/>
+      <c r="W29" s="132"/>
+      <c r="X29" s="132"/>
+      <c r="Y29" s="132"/>
+      <c r="Z29" s="132"/>
+      <c r="AA29" s="132"/>
+      <c r="AB29" s="132"/>
+      <c r="AC29" s="132"/>
+      <c r="AD29" s="132"/>
+      <c r="AE29" s="132"/>
+      <c r="AF29" s="132"/>
+      <c r="AG29" s="132"/>
+      <c r="AH29" s="132"/>
+      <c r="AI29" s="132"/>
+      <c r="AJ29" s="132"/>
+      <c r="AK29" s="132"/>
+      <c r="AL29" s="132"/>
+      <c r="AM29" s="132"/>
+      <c r="AN29" s="132"/>
+      <c r="AO29" s="132"/>
+      <c r="AP29" s="132"/>
+      <c r="AQ29" s="132"/>
+      <c r="AR29" s="132"/>
+      <c r="AS29" s="132"/>
+      <c r="AT29" s="132"/>
+      <c r="AU29" s="132"/>
+      <c r="AV29" s="132"/>
+      <c r="AW29" s="132"/>
+      <c r="AX29" s="132"/>
+      <c r="AY29" s="132"/>
+      <c r="AZ29" s="132"/>
+      <c r="BA29" s="132"/>
+      <c r="BB29" s="132"/>
+      <c r="BC29" s="132"/>
+      <c r="BD29" s="132"/>
+      <c r="BE29" s="132"/>
+      <c r="BF29" s="132"/>
+      <c r="BG29" s="132"/>
+      <c r="BH29" s="132"/>
+      <c r="BI29" s="132"/>
+      <c r="BJ29" s="132"/>
+      <c r="BK29" s="132"/>
+      <c r="BL29" s="132"/>
+      <c r="BM29" s="132"/>
+      <c r="BN29" s="132"/>
+      <c r="BO29" s="132"/>
+      <c r="BP29" s="132"/>
+      <c r="BQ29" s="132"/>
+      <c r="BR29" s="132"/>
+      <c r="BS29" s="132"/>
+      <c r="BT29" s="132"/>
+      <c r="BU29" s="132"/>
+      <c r="BV29" s="132"/>
+      <c r="BW29" s="132"/>
+      <c r="BX29" s="132"/>
+      <c r="BY29" s="132"/>
+      <c r="BZ29" s="132"/>
+      <c r="CA29" s="132"/>
+      <c r="CB29" s="132"/>
+      <c r="CC29" s="132"/>
+      <c r="CD29" s="132"/>
+      <c r="CE29" s="133"/>
     </row>
     <row r="30" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A30" s="1"/>
@@ -4890,8 +4890,8 @@
       <c r="AM30" s="41"/>
       <c r="AN30" s="75"/>
       <c r="AO30" s="107"/>
-      <c r="AP30" s="109"/>
-      <c r="AQ30" s="110"/>
+      <c r="AP30" s="118"/>
+      <c r="AQ30" s="120"/>
       <c r="AR30" s="101"/>
       <c r="AS30" s="99"/>
       <c r="AT30" s="99"/>
@@ -4936,7 +4936,7 @@
     <row r="31" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
       <c r="B31" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>3</v>
@@ -4981,18 +4981,18 @@
       <c r="AK31" s="28"/>
       <c r="AL31" s="28"/>
       <c r="AM31" s="67"/>
-      <c r="AN31" s="143"/>
-      <c r="AO31" s="156"/>
-      <c r="AP31" s="156"/>
-      <c r="AQ31" s="156"/>
-      <c r="AR31" s="156"/>
-      <c r="AS31" s="156"/>
-      <c r="AT31" s="156"/>
-      <c r="AU31" s="156"/>
-      <c r="AV31" s="156"/>
-      <c r="AW31" s="156"/>
-      <c r="AX31" s="156"/>
-      <c r="AY31" s="157"/>
+      <c r="AN31" s="109"/>
+      <c r="AO31" s="110"/>
+      <c r="AP31" s="110"/>
+      <c r="AQ31" s="110"/>
+      <c r="AR31" s="110"/>
+      <c r="AS31" s="110"/>
+      <c r="AT31" s="110"/>
+      <c r="AU31" s="110"/>
+      <c r="AV31" s="110"/>
+      <c r="AW31" s="110"/>
+      <c r="AX31" s="110"/>
+      <c r="AY31" s="111"/>
       <c r="AZ31" s="106"/>
       <c r="BA31" s="28"/>
       <c r="BB31" s="75"/>
@@ -5071,12 +5071,12 @@
       <c r="AF32" s="28"/>
       <c r="AG32" s="44"/>
       <c r="AH32" s="65"/>
-      <c r="AI32" s="111"/>
-      <c r="AJ32" s="112"/>
-      <c r="AK32" s="112"/>
-      <c r="AL32" s="112"/>
-      <c r="AM32" s="112"/>
-      <c r="AN32" s="113"/>
+      <c r="AI32" s="136"/>
+      <c r="AJ32" s="113"/>
+      <c r="AK32" s="113"/>
+      <c r="AL32" s="113"/>
+      <c r="AM32" s="113"/>
+      <c r="AN32" s="150"/>
       <c r="AO32" s="105"/>
       <c r="AP32" s="57"/>
       <c r="AQ32" s="57"/>
@@ -5165,12 +5165,12 @@
       <c r="AG33" s="44"/>
       <c r="AH33" s="44"/>
       <c r="AI33" s="66"/>
-      <c r="AJ33" s="114"/>
-      <c r="AK33" s="112"/>
-      <c r="AL33" s="112"/>
-      <c r="AM33" s="112"/>
-      <c r="AN33" s="112"/>
-      <c r="AO33" s="115"/>
+      <c r="AJ33" s="161"/>
+      <c r="AK33" s="113"/>
+      <c r="AL33" s="113"/>
+      <c r="AM33" s="113"/>
+      <c r="AN33" s="113"/>
+      <c r="AO33" s="114"/>
       <c r="AP33" s="41"/>
       <c r="AQ33" s="28"/>
       <c r="AR33" s="28"/>
@@ -5259,12 +5259,12 @@
       <c r="AH34" s="44"/>
       <c r="AI34" s="28"/>
       <c r="AJ34" s="66"/>
-      <c r="AK34" s="116"/>
-      <c r="AL34" s="112"/>
-      <c r="AM34" s="112"/>
-      <c r="AN34" s="112"/>
-      <c r="AO34" s="112"/>
-      <c r="AP34" s="115"/>
+      <c r="AK34" s="126"/>
+      <c r="AL34" s="113"/>
+      <c r="AM34" s="113"/>
+      <c r="AN34" s="113"/>
+      <c r="AO34" s="113"/>
+      <c r="AP34" s="114"/>
       <c r="AQ34" s="41"/>
       <c r="AR34" s="28"/>
       <c r="AS34" s="28"/>
@@ -5353,12 +5353,12 @@
       <c r="AI35" s="28"/>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="56"/>
-      <c r="AL35" s="111"/>
-      <c r="AM35" s="112"/>
-      <c r="AN35" s="112"/>
-      <c r="AO35" s="112"/>
-      <c r="AP35" s="118"/>
-      <c r="AQ35" s="110"/>
+      <c r="AL35" s="136"/>
+      <c r="AM35" s="113"/>
+      <c r="AN35" s="113"/>
+      <c r="AO35" s="113"/>
+      <c r="AP35" s="119"/>
+      <c r="AQ35" s="120"/>
       <c r="AR35" s="101"/>
       <c r="AS35" s="99"/>
       <c r="AT35" s="99"/>
@@ -5450,17 +5450,17 @@
       <c r="AM36" s="57"/>
       <c r="AN36" s="40"/>
       <c r="AO36" s="100"/>
-      <c r="AP36" s="143"/>
-      <c r="AQ36" s="156"/>
-      <c r="AR36" s="156"/>
-      <c r="AS36" s="156"/>
-      <c r="AT36" s="156"/>
-      <c r="AU36" s="156"/>
-      <c r="AV36" s="156"/>
-      <c r="AW36" s="156"/>
-      <c r="AX36" s="156"/>
-      <c r="AY36" s="156"/>
-      <c r="AZ36" s="157"/>
+      <c r="AP36" s="109"/>
+      <c r="AQ36" s="110"/>
+      <c r="AR36" s="110"/>
+      <c r="AS36" s="110"/>
+      <c r="AT36" s="110"/>
+      <c r="AU36" s="110"/>
+      <c r="AV36" s="110"/>
+      <c r="AW36" s="110"/>
+      <c r="AX36" s="110"/>
+      <c r="AY36" s="110"/>
+      <c r="AZ36" s="111"/>
       <c r="BA36" s="101"/>
       <c r="BB36" s="75"/>
       <c r="BC36" s="75"/>
@@ -5549,17 +5549,17 @@
       <c r="AS37" s="78"/>
       <c r="AT37" s="78"/>
       <c r="AU37" s="102"/>
-      <c r="AV37" s="119"/>
-      <c r="AW37" s="120"/>
-      <c r="AX37" s="120"/>
-      <c r="AY37" s="120"/>
-      <c r="AZ37" s="120"/>
-      <c r="BA37" s="112"/>
-      <c r="BB37" s="112"/>
-      <c r="BC37" s="112"/>
-      <c r="BD37" s="112"/>
-      <c r="BE37" s="112"/>
-      <c r="BF37" s="115"/>
+      <c r="AV37" s="162"/>
+      <c r="AW37" s="122"/>
+      <c r="AX37" s="122"/>
+      <c r="AY37" s="122"/>
+      <c r="AZ37" s="122"/>
+      <c r="BA37" s="113"/>
+      <c r="BB37" s="113"/>
+      <c r="BC37" s="113"/>
+      <c r="BD37" s="113"/>
+      <c r="BE37" s="113"/>
+      <c r="BF37" s="114"/>
       <c r="BG37" s="38"/>
       <c r="BH37" s="28"/>
       <c r="BI37" s="44"/>
@@ -5638,17 +5638,17 @@
       <c r="AO38" s="44"/>
       <c r="AP38" s="28"/>
       <c r="AQ38" s="67"/>
-      <c r="AR38" s="117"/>
-      <c r="AS38" s="112"/>
-      <c r="AT38" s="112"/>
-      <c r="AU38" s="112"/>
-      <c r="AV38" s="112"/>
-      <c r="AW38" s="112"/>
-      <c r="AX38" s="112"/>
-      <c r="AY38" s="112"/>
-      <c r="AZ38" s="112"/>
-      <c r="BA38" s="112"/>
-      <c r="BB38" s="115"/>
+      <c r="AR38" s="153"/>
+      <c r="AS38" s="113"/>
+      <c r="AT38" s="113"/>
+      <c r="AU38" s="113"/>
+      <c r="AV38" s="113"/>
+      <c r="AW38" s="113"/>
+      <c r="AX38" s="113"/>
+      <c r="AY38" s="113"/>
+      <c r="AZ38" s="113"/>
+      <c r="BA38" s="113"/>
+      <c r="BB38" s="114"/>
       <c r="BC38" s="46"/>
       <c r="BD38" s="57"/>
       <c r="BE38" s="57"/>
@@ -5732,17 +5732,17 @@
       <c r="AP39" s="28"/>
       <c r="AQ39" s="28"/>
       <c r="AR39" s="66"/>
-      <c r="AS39" s="121"/>
-      <c r="AT39" s="112"/>
-      <c r="AU39" s="112"/>
-      <c r="AV39" s="112"/>
-      <c r="AW39" s="112"/>
-      <c r="AX39" s="112"/>
-      <c r="AY39" s="112"/>
-      <c r="AZ39" s="112"/>
-      <c r="BA39" s="112"/>
-      <c r="BB39" s="112"/>
-      <c r="BC39" s="115"/>
+      <c r="AS39" s="163"/>
+      <c r="AT39" s="113"/>
+      <c r="AU39" s="113"/>
+      <c r="AV39" s="113"/>
+      <c r="AW39" s="113"/>
+      <c r="AX39" s="113"/>
+      <c r="AY39" s="113"/>
+      <c r="AZ39" s="113"/>
+      <c r="BA39" s="113"/>
+      <c r="BB39" s="113"/>
+      <c r="BC39" s="114"/>
       <c r="BD39" s="41"/>
       <c r="BE39" s="28"/>
       <c r="BF39" s="28"/>
@@ -5826,17 +5826,17 @@
       <c r="AQ40" s="28"/>
       <c r="AR40" s="28"/>
       <c r="AS40" s="66"/>
-      <c r="AT40" s="117"/>
-      <c r="AU40" s="112"/>
-      <c r="AV40" s="112"/>
-      <c r="AW40" s="112"/>
-      <c r="AX40" s="112"/>
-      <c r="AY40" s="112"/>
-      <c r="AZ40" s="112"/>
-      <c r="BA40" s="112"/>
-      <c r="BB40" s="112"/>
-      <c r="BC40" s="112"/>
-      <c r="BD40" s="115"/>
+      <c r="AT40" s="153"/>
+      <c r="AU40" s="113"/>
+      <c r="AV40" s="113"/>
+      <c r="AW40" s="113"/>
+      <c r="AX40" s="113"/>
+      <c r="AY40" s="113"/>
+      <c r="AZ40" s="113"/>
+      <c r="BA40" s="113"/>
+      <c r="BB40" s="113"/>
+      <c r="BC40" s="113"/>
+      <c r="BD40" s="114"/>
       <c r="BE40" s="38"/>
       <c r="BF40" s="28"/>
       <c r="BG40" s="28"/>
@@ -5921,11 +5921,11 @@
       <c r="AS41" s="28"/>
       <c r="AT41" s="57"/>
       <c r="AU41" s="51"/>
-      <c r="AV41" s="127"/>
-      <c r="AW41" s="112"/>
-      <c r="AX41" s="112"/>
-      <c r="AY41" s="112"/>
-      <c r="AZ41" s="115"/>
+      <c r="AV41" s="112"/>
+      <c r="AW41" s="113"/>
+      <c r="AX41" s="113"/>
+      <c r="AY41" s="113"/>
+      <c r="AZ41" s="114"/>
       <c r="BA41" s="55"/>
       <c r="BB41" s="39"/>
       <c r="BC41" s="39"/>
@@ -6015,16 +6015,16 @@
       <c r="AT42" s="28"/>
       <c r="AU42" s="49"/>
       <c r="AV42" s="49"/>
-      <c r="AW42" s="122"/>
-      <c r="AX42" s="112"/>
-      <c r="AY42" s="112"/>
-      <c r="AZ42" s="112"/>
-      <c r="BA42" s="112"/>
-      <c r="BB42" s="112"/>
-      <c r="BC42" s="112"/>
-      <c r="BD42" s="112"/>
-      <c r="BE42" s="112"/>
-      <c r="BF42" s="115"/>
+      <c r="AW42" s="115"/>
+      <c r="AX42" s="113"/>
+      <c r="AY42" s="113"/>
+      <c r="AZ42" s="113"/>
+      <c r="BA42" s="113"/>
+      <c r="BB42" s="113"/>
+      <c r="BC42" s="113"/>
+      <c r="BD42" s="113"/>
+      <c r="BE42" s="113"/>
+      <c r="BF42" s="114"/>
       <c r="BG42" s="41"/>
       <c r="BH42" s="42"/>
       <c r="BI42" s="75"/>
@@ -6107,14 +6107,14 @@
       <c r="AS43" s="28"/>
       <c r="AT43" s="28"/>
       <c r="AU43" s="53"/>
-      <c r="AV43" s="158"/>
-      <c r="AW43" s="112"/>
-      <c r="AX43" s="112"/>
-      <c r="AY43" s="112"/>
-      <c r="AZ43" s="112"/>
-      <c r="BA43" s="112"/>
-      <c r="BB43" s="112"/>
-      <c r="BC43" s="159"/>
+      <c r="AV43" s="116"/>
+      <c r="AW43" s="113"/>
+      <c r="AX43" s="113"/>
+      <c r="AY43" s="113"/>
+      <c r="AZ43" s="113"/>
+      <c r="BA43" s="113"/>
+      <c r="BB43" s="113"/>
+      <c r="BC43" s="117"/>
       <c r="BD43" s="28"/>
       <c r="BE43" s="28"/>
       <c r="BF43" s="28"/>
@@ -6199,13 +6199,13 @@
       <c r="AR44" s="28"/>
       <c r="AS44" s="99"/>
       <c r="AT44" s="56"/>
-      <c r="AU44" s="109"/>
-      <c r="AV44" s="118"/>
-      <c r="AW44" s="118"/>
-      <c r="AX44" s="118"/>
-      <c r="AY44" s="118"/>
-      <c r="AZ44" s="118"/>
-      <c r="BA44" s="110"/>
+      <c r="AU44" s="118"/>
+      <c r="AV44" s="119"/>
+      <c r="AW44" s="119"/>
+      <c r="AX44" s="119"/>
+      <c r="AY44" s="119"/>
+      <c r="AZ44" s="119"/>
+      <c r="BA44" s="120"/>
       <c r="BB44" s="105"/>
       <c r="BC44" s="98"/>
       <c r="BD44" s="57"/>
@@ -6292,15 +6292,15 @@
       <c r="AR45" s="67"/>
       <c r="AS45" s="67"/>
       <c r="AT45" s="67"/>
-      <c r="AU45" s="143"/>
-      <c r="AV45" s="156"/>
-      <c r="AW45" s="156"/>
-      <c r="AX45" s="156"/>
-      <c r="AY45" s="156"/>
-      <c r="AZ45" s="156"/>
-      <c r="BA45" s="156"/>
-      <c r="BB45" s="156"/>
-      <c r="BC45" s="157"/>
+      <c r="AU45" s="109"/>
+      <c r="AV45" s="110"/>
+      <c r="AW45" s="110"/>
+      <c r="AX45" s="110"/>
+      <c r="AY45" s="110"/>
+      <c r="AZ45" s="110"/>
+      <c r="BA45" s="110"/>
+      <c r="BB45" s="110"/>
+      <c r="BC45" s="111"/>
       <c r="BD45" s="101"/>
       <c r="BE45" s="42"/>
       <c r="BF45" s="28"/>
@@ -6389,13 +6389,13 @@
       <c r="AV46" s="100"/>
       <c r="AW46" s="78"/>
       <c r="AX46" s="56"/>
-      <c r="AY46" s="155"/>
-      <c r="AZ46" s="120"/>
-      <c r="BA46" s="120"/>
-      <c r="BB46" s="120"/>
-      <c r="BC46" s="120"/>
-      <c r="BD46" s="112"/>
-      <c r="BE46" s="115"/>
+      <c r="AY46" s="121"/>
+      <c r="AZ46" s="122"/>
+      <c r="BA46" s="122"/>
+      <c r="BB46" s="122"/>
+      <c r="BC46" s="122"/>
+      <c r="BD46" s="113"/>
+      <c r="BE46" s="114"/>
       <c r="BF46" s="38"/>
       <c r="BG46" s="28"/>
       <c r="BH46" s="28"/>
@@ -6479,12 +6479,12 @@
       <c r="AS47" s="28"/>
       <c r="AT47" s="57"/>
       <c r="AU47" s="51"/>
-      <c r="AV47" s="122"/>
-      <c r="AW47" s="112"/>
-      <c r="AX47" s="112"/>
-      <c r="AY47" s="118"/>
-      <c r="AZ47" s="118"/>
-      <c r="BA47" s="110"/>
+      <c r="AV47" s="115"/>
+      <c r="AW47" s="113"/>
+      <c r="AX47" s="113"/>
+      <c r="AY47" s="119"/>
+      <c r="AZ47" s="119"/>
+      <c r="BA47" s="120"/>
       <c r="BB47" s="98"/>
       <c r="BC47" s="98"/>
       <c r="BD47" s="78"/>
@@ -6575,12 +6575,12 @@
       <c r="AV48" s="40"/>
       <c r="AW48" s="57"/>
       <c r="AX48" s="66"/>
-      <c r="AY48" s="163"/>
-      <c r="AZ48" s="124"/>
-      <c r="BA48" s="124"/>
-      <c r="BB48" s="124"/>
-      <c r="BC48" s="124"/>
-      <c r="BD48" s="125"/>
+      <c r="AY48" s="127"/>
+      <c r="AZ48" s="128"/>
+      <c r="BA48" s="128"/>
+      <c r="BB48" s="128"/>
+      <c r="BC48" s="128"/>
+      <c r="BD48" s="129"/>
       <c r="BE48" s="106"/>
       <c r="BF48" s="28"/>
       <c r="BG48" s="28"/>
@@ -6614,7 +6614,7 @@
         <v>56</v>
       </c>
       <c r="B49" s="72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="73" t="s">
         <v>1</v>
@@ -6672,10 +6672,10 @@
       <c r="AX49" s="42"/>
       <c r="AY49" s="78"/>
       <c r="AZ49" s="56"/>
-      <c r="BA49" s="160"/>
-      <c r="BB49" s="161"/>
-      <c r="BC49" s="161"/>
-      <c r="BD49" s="162"/>
+      <c r="BA49" s="123"/>
+      <c r="BB49" s="124"/>
+      <c r="BC49" s="124"/>
+      <c r="BD49" s="125"/>
       <c r="BE49" s="38"/>
       <c r="BF49" s="28"/>
       <c r="BG49" s="28"/>
@@ -6759,12 +6759,12 @@
       <c r="AR50" s="28"/>
       <c r="AS50" s="28"/>
       <c r="AT50" s="66"/>
-      <c r="AU50" s="116"/>
-      <c r="AV50" s="112"/>
-      <c r="AW50" s="112"/>
-      <c r="AX50" s="112"/>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="115"/>
+      <c r="AU50" s="126"/>
+      <c r="AV50" s="113"/>
+      <c r="AW50" s="113"/>
+      <c r="AX50" s="113"/>
+      <c r="AY50" s="113"/>
+      <c r="AZ50" s="114"/>
       <c r="BA50" s="55"/>
       <c r="BB50" s="39"/>
       <c r="BC50" s="39"/>
@@ -6858,12 +6858,12 @@
       <c r="AX51" s="57"/>
       <c r="AY51" s="57"/>
       <c r="AZ51" s="66"/>
-      <c r="BA51" s="154"/>
-      <c r="BB51" s="112"/>
-      <c r="BC51" s="112"/>
-      <c r="BD51" s="112"/>
-      <c r="BE51" s="112"/>
-      <c r="BF51" s="115"/>
+      <c r="BA51" s="130"/>
+      <c r="BB51" s="113"/>
+      <c r="BC51" s="113"/>
+      <c r="BD51" s="113"/>
+      <c r="BE51" s="113"/>
+      <c r="BF51" s="114"/>
       <c r="BG51" s="38"/>
       <c r="BH51" s="28"/>
       <c r="BI51" s="44"/>
@@ -6899,83 +6899,83 @@
       <c r="D52" s="81"/>
       <c r="E52" s="82"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="132"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="133"/>
-      <c r="K52" s="133"/>
-      <c r="L52" s="133"/>
-      <c r="M52" s="133"/>
-      <c r="N52" s="133"/>
-      <c r="O52" s="133"/>
-      <c r="P52" s="133"/>
-      <c r="Q52" s="133"/>
-      <c r="R52" s="133"/>
-      <c r="S52" s="133"/>
-      <c r="T52" s="133"/>
-      <c r="U52" s="133"/>
-      <c r="V52" s="133"/>
-      <c r="W52" s="133"/>
-      <c r="X52" s="133"/>
-      <c r="Y52" s="133"/>
-      <c r="Z52" s="133"/>
-      <c r="AA52" s="133"/>
-      <c r="AB52" s="133"/>
-      <c r="AC52" s="133"/>
-      <c r="AD52" s="133"/>
-      <c r="AE52" s="133"/>
-      <c r="AF52" s="133"/>
-      <c r="AG52" s="133"/>
-      <c r="AH52" s="133"/>
-      <c r="AI52" s="133"/>
-      <c r="AJ52" s="133"/>
-      <c r="AK52" s="133"/>
-      <c r="AL52" s="133"/>
-      <c r="AM52" s="133"/>
-      <c r="AN52" s="133"/>
-      <c r="AO52" s="133"/>
-      <c r="AP52" s="133"/>
-      <c r="AQ52" s="133"/>
-      <c r="AR52" s="133"/>
-      <c r="AS52" s="133"/>
-      <c r="AT52" s="133"/>
-      <c r="AU52" s="133"/>
-      <c r="AV52" s="133"/>
-      <c r="AW52" s="133"/>
-      <c r="AX52" s="133"/>
-      <c r="AY52" s="133"/>
-      <c r="AZ52" s="133"/>
-      <c r="BA52" s="133"/>
-      <c r="BB52" s="133"/>
-      <c r="BC52" s="133"/>
-      <c r="BD52" s="133"/>
-      <c r="BE52" s="133"/>
-      <c r="BF52" s="133"/>
-      <c r="BG52" s="133"/>
-      <c r="BH52" s="133"/>
-      <c r="BI52" s="133"/>
-      <c r="BJ52" s="133"/>
-      <c r="BK52" s="133"/>
-      <c r="BL52" s="133"/>
-      <c r="BM52" s="133"/>
-      <c r="BN52" s="133"/>
-      <c r="BO52" s="133"/>
-      <c r="BP52" s="133"/>
-      <c r="BQ52" s="133"/>
-      <c r="BR52" s="133"/>
-      <c r="BS52" s="133"/>
-      <c r="BT52" s="133"/>
-      <c r="BU52" s="133"/>
-      <c r="BV52" s="133"/>
-      <c r="BW52" s="133"/>
-      <c r="BX52" s="133"/>
-      <c r="BY52" s="133"/>
-      <c r="BZ52" s="133"/>
-      <c r="CA52" s="133"/>
-      <c r="CB52" s="133"/>
-      <c r="CC52" s="133"/>
-      <c r="CD52" s="133"/>
-      <c r="CE52" s="134"/>
+      <c r="G52" s="131"/>
+      <c r="H52" s="132"/>
+      <c r="I52" s="132"/>
+      <c r="J52" s="132"/>
+      <c r="K52" s="132"/>
+      <c r="L52" s="132"/>
+      <c r="M52" s="132"/>
+      <c r="N52" s="132"/>
+      <c r="O52" s="132"/>
+      <c r="P52" s="132"/>
+      <c r="Q52" s="132"/>
+      <c r="R52" s="132"/>
+      <c r="S52" s="132"/>
+      <c r="T52" s="132"/>
+      <c r="U52" s="132"/>
+      <c r="V52" s="132"/>
+      <c r="W52" s="132"/>
+      <c r="X52" s="132"/>
+      <c r="Y52" s="132"/>
+      <c r="Z52" s="132"/>
+      <c r="AA52" s="132"/>
+      <c r="AB52" s="132"/>
+      <c r="AC52" s="132"/>
+      <c r="AD52" s="132"/>
+      <c r="AE52" s="132"/>
+      <c r="AF52" s="132"/>
+      <c r="AG52" s="132"/>
+      <c r="AH52" s="132"/>
+      <c r="AI52" s="132"/>
+      <c r="AJ52" s="132"/>
+      <c r="AK52" s="132"/>
+      <c r="AL52" s="132"/>
+      <c r="AM52" s="132"/>
+      <c r="AN52" s="132"/>
+      <c r="AO52" s="132"/>
+      <c r="AP52" s="132"/>
+      <c r="AQ52" s="132"/>
+      <c r="AR52" s="132"/>
+      <c r="AS52" s="132"/>
+      <c r="AT52" s="132"/>
+      <c r="AU52" s="132"/>
+      <c r="AV52" s="132"/>
+      <c r="AW52" s="132"/>
+      <c r="AX52" s="132"/>
+      <c r="AY52" s="132"/>
+      <c r="AZ52" s="132"/>
+      <c r="BA52" s="132"/>
+      <c r="BB52" s="132"/>
+      <c r="BC52" s="132"/>
+      <c r="BD52" s="132"/>
+      <c r="BE52" s="132"/>
+      <c r="BF52" s="132"/>
+      <c r="BG52" s="132"/>
+      <c r="BH52" s="132"/>
+      <c r="BI52" s="132"/>
+      <c r="BJ52" s="132"/>
+      <c r="BK52" s="132"/>
+      <c r="BL52" s="132"/>
+      <c r="BM52" s="132"/>
+      <c r="BN52" s="132"/>
+      <c r="BO52" s="132"/>
+      <c r="BP52" s="132"/>
+      <c r="BQ52" s="132"/>
+      <c r="BR52" s="132"/>
+      <c r="BS52" s="132"/>
+      <c r="BT52" s="132"/>
+      <c r="BU52" s="132"/>
+      <c r="BV52" s="132"/>
+      <c r="BW52" s="132"/>
+      <c r="BX52" s="132"/>
+      <c r="BY52" s="132"/>
+      <c r="BZ52" s="132"/>
+      <c r="CA52" s="132"/>
+      <c r="CB52" s="132"/>
+      <c r="CC52" s="132"/>
+      <c r="CD52" s="132"/>
+      <c r="CE52" s="133"/>
     </row>
     <row r="53" spans="1:83" ht="15" customHeight="1">
       <c r="A53" s="1"/>
@@ -7039,10 +7039,10 @@
       <c r="AY53" s="28"/>
       <c r="AZ53" s="28"/>
       <c r="BA53" s="67"/>
-      <c r="BB53" s="116"/>
-      <c r="BC53" s="112"/>
-      <c r="BD53" s="112"/>
-      <c r="BE53" s="115"/>
+      <c r="BB53" s="126"/>
+      <c r="BC53" s="113"/>
+      <c r="BD53" s="113"/>
+      <c r="BE53" s="114"/>
       <c r="BF53" s="41"/>
       <c r="BG53" s="42"/>
       <c r="BH53" s="42"/>
@@ -7136,11 +7136,11 @@
       <c r="BC54" s="40"/>
       <c r="BD54" s="57"/>
       <c r="BE54" s="56"/>
-      <c r="BF54" s="116"/>
-      <c r="BG54" s="112"/>
-      <c r="BH54" s="112"/>
-      <c r="BI54" s="112"/>
-      <c r="BJ54" s="115"/>
+      <c r="BF54" s="126"/>
+      <c r="BG54" s="113"/>
+      <c r="BH54" s="113"/>
+      <c r="BI54" s="113"/>
+      <c r="BJ54" s="114"/>
       <c r="BK54" s="41"/>
       <c r="BL54" s="42"/>
       <c r="BM54" s="28"/>
@@ -7228,14 +7228,14 @@
       <c r="BB55" s="44"/>
       <c r="BC55" s="44"/>
       <c r="BD55" s="67"/>
-      <c r="BE55" s="122"/>
-      <c r="BF55" s="112"/>
-      <c r="BG55" s="112"/>
-      <c r="BH55" s="112"/>
-      <c r="BI55" s="112"/>
-      <c r="BJ55" s="112"/>
-      <c r="BK55" s="112"/>
-      <c r="BL55" s="115"/>
+      <c r="BE55" s="115"/>
+      <c r="BF55" s="113"/>
+      <c r="BG55" s="113"/>
+      <c r="BH55" s="113"/>
+      <c r="BI55" s="113"/>
+      <c r="BJ55" s="113"/>
+      <c r="BK55" s="113"/>
+      <c r="BL55" s="114"/>
       <c r="BM55" s="38"/>
       <c r="BN55" s="28"/>
       <c r="BO55" s="28"/>
@@ -7322,13 +7322,13 @@
       <c r="BC56" s="44"/>
       <c r="BD56" s="28"/>
       <c r="BE56" s="66"/>
-      <c r="BF56" s="151"/>
-      <c r="BG56" s="112"/>
-      <c r="BH56" s="112"/>
-      <c r="BI56" s="112"/>
-      <c r="BJ56" s="112"/>
-      <c r="BK56" s="112"/>
-      <c r="BL56" s="115"/>
+      <c r="BF56" s="135"/>
+      <c r="BG56" s="113"/>
+      <c r="BH56" s="113"/>
+      <c r="BI56" s="113"/>
+      <c r="BJ56" s="113"/>
+      <c r="BK56" s="113"/>
+      <c r="BL56" s="114"/>
       <c r="BM56" s="41"/>
       <c r="BN56" s="86"/>
       <c r="BO56" s="42"/>
@@ -7419,12 +7419,12 @@
       <c r="BG57" s="57"/>
       <c r="BH57" s="57"/>
       <c r="BI57" s="51"/>
-      <c r="BJ57" s="111"/>
-      <c r="BK57" s="112"/>
-      <c r="BL57" s="112"/>
-      <c r="BM57" s="112"/>
-      <c r="BN57" s="112"/>
-      <c r="BO57" s="115"/>
+      <c r="BJ57" s="136"/>
+      <c r="BK57" s="113"/>
+      <c r="BL57" s="113"/>
+      <c r="BM57" s="113"/>
+      <c r="BN57" s="113"/>
+      <c r="BO57" s="114"/>
       <c r="BP57" s="53"/>
       <c r="BQ57" s="75"/>
       <c r="BR57" s="42"/>
@@ -7513,15 +7513,15 @@
       <c r="BH58" s="28"/>
       <c r="BI58" s="44"/>
       <c r="BJ58" s="51"/>
-      <c r="BK58" s="127"/>
-      <c r="BL58" s="112"/>
-      <c r="BM58" s="112"/>
-      <c r="BN58" s="112"/>
-      <c r="BO58" s="112"/>
-      <c r="BP58" s="112"/>
-      <c r="BQ58" s="112"/>
-      <c r="BR58" s="112"/>
-      <c r="BS58" s="115"/>
+      <c r="BK58" s="112"/>
+      <c r="BL58" s="113"/>
+      <c r="BM58" s="113"/>
+      <c r="BN58" s="113"/>
+      <c r="BO58" s="113"/>
+      <c r="BP58" s="113"/>
+      <c r="BQ58" s="113"/>
+      <c r="BR58" s="113"/>
+      <c r="BS58" s="114"/>
       <c r="BT58" s="38"/>
       <c r="BU58" s="28"/>
       <c r="BV58" s="28"/>
@@ -7607,12 +7607,12 @@
       <c r="BI59" s="44"/>
       <c r="BJ59" s="51"/>
       <c r="BK59" s="57"/>
-      <c r="BL59" s="152"/>
-      <c r="BM59" s="112"/>
-      <c r="BN59" s="112"/>
-      <c r="BO59" s="112"/>
-      <c r="BP59" s="112"/>
-      <c r="BQ59" s="153"/>
+      <c r="BL59" s="137"/>
+      <c r="BM59" s="113"/>
+      <c r="BN59" s="113"/>
+      <c r="BO59" s="113"/>
+      <c r="BP59" s="113"/>
+      <c r="BQ59" s="138"/>
       <c r="BR59" s="47"/>
       <c r="BS59" s="47"/>
       <c r="BT59" s="38"/>
@@ -7631,7 +7631,7 @@
     <row r="60" spans="1:83" ht="15" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="83" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C60" s="84" t="s">
         <v>3</v>
@@ -7701,13 +7701,13 @@
       <c r="BJ60" s="44"/>
       <c r="BK60" s="57"/>
       <c r="BL60" s="66"/>
-      <c r="BM60" s="130"/>
-      <c r="BN60" s="112"/>
-      <c r="BO60" s="112"/>
-      <c r="BP60" s="112"/>
-      <c r="BQ60" s="112"/>
-      <c r="BR60" s="112"/>
-      <c r="BS60" s="115"/>
+      <c r="BM60" s="139"/>
+      <c r="BN60" s="113"/>
+      <c r="BO60" s="113"/>
+      <c r="BP60" s="113"/>
+      <c r="BQ60" s="113"/>
+      <c r="BR60" s="113"/>
+      <c r="BS60" s="114"/>
       <c r="BT60" s="38"/>
       <c r="BU60" s="28"/>
       <c r="BV60" s="28"/>
@@ -7724,7 +7724,7 @@
     <row r="61" spans="1:83" ht="15" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="84" t="s">
         <v>5</v>
@@ -7794,11 +7794,11 @@
       <c r="BJ61" s="44"/>
       <c r="BK61" s="28"/>
       <c r="BL61" s="67"/>
-      <c r="BM61" s="127"/>
-      <c r="BN61" s="112"/>
-      <c r="BO61" s="112"/>
-      <c r="BP61" s="112"/>
-      <c r="BQ61" s="115"/>
+      <c r="BM61" s="112"/>
+      <c r="BN61" s="113"/>
+      <c r="BO61" s="113"/>
+      <c r="BP61" s="113"/>
+      <c r="BQ61" s="114"/>
       <c r="BR61" s="55"/>
       <c r="BS61" s="78"/>
       <c r="BT61" s="42"/>
@@ -7817,7 +7817,7 @@
     <row r="62" spans="1:83" ht="15" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="84" t="s">
         <v>7</v>
@@ -7888,13 +7888,13 @@
       <c r="BK62" s="28"/>
       <c r="BL62" s="28"/>
       <c r="BM62" s="66"/>
-      <c r="BN62" s="122"/>
-      <c r="BO62" s="112"/>
-      <c r="BP62" s="112"/>
-      <c r="BQ62" s="112"/>
-      <c r="BR62" s="112"/>
-      <c r="BS62" s="112"/>
-      <c r="BT62" s="115"/>
+      <c r="BN62" s="115"/>
+      <c r="BO62" s="113"/>
+      <c r="BP62" s="113"/>
+      <c r="BQ62" s="113"/>
+      <c r="BR62" s="113"/>
+      <c r="BS62" s="113"/>
+      <c r="BT62" s="114"/>
       <c r="BU62" s="38"/>
       <c r="BV62" s="28"/>
       <c r="BW62" s="44"/>
@@ -7910,7 +7910,7 @@
     <row r="63" spans="1:83" ht="15" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" s="84" t="s">
         <v>1</v>
@@ -7983,11 +7983,11 @@
       <c r="BM63" s="28"/>
       <c r="BN63" s="57"/>
       <c r="BO63" s="66"/>
-      <c r="BP63" s="137"/>
-      <c r="BQ63" s="112"/>
-      <c r="BR63" s="112"/>
-      <c r="BS63" s="112"/>
-      <c r="BT63" s="115"/>
+      <c r="BP63" s="134"/>
+      <c r="BQ63" s="113"/>
+      <c r="BR63" s="113"/>
+      <c r="BS63" s="113"/>
+      <c r="BT63" s="114"/>
       <c r="BU63" s="38"/>
       <c r="BV63" s="28"/>
       <c r="BW63" s="44"/>
@@ -8007,83 +8007,83 @@
       <c r="D64" s="90"/>
       <c r="E64" s="91"/>
       <c r="F64" s="92"/>
-      <c r="G64" s="132"/>
-      <c r="H64" s="133"/>
-      <c r="I64" s="133"/>
-      <c r="J64" s="133"/>
-      <c r="K64" s="133"/>
-      <c r="L64" s="133"/>
-      <c r="M64" s="133"/>
-      <c r="N64" s="133"/>
-      <c r="O64" s="133"/>
-      <c r="P64" s="133"/>
-      <c r="Q64" s="133"/>
-      <c r="R64" s="133"/>
-      <c r="S64" s="133"/>
-      <c r="T64" s="133"/>
-      <c r="U64" s="133"/>
-      <c r="V64" s="133"/>
-      <c r="W64" s="133"/>
-      <c r="X64" s="133"/>
-      <c r="Y64" s="133"/>
-      <c r="Z64" s="133"/>
-      <c r="AA64" s="133"/>
-      <c r="AB64" s="133"/>
-      <c r="AC64" s="133"/>
-      <c r="AD64" s="133"/>
-      <c r="AE64" s="133"/>
-      <c r="AF64" s="133"/>
-      <c r="AG64" s="133"/>
-      <c r="AH64" s="133"/>
-      <c r="AI64" s="133"/>
-      <c r="AJ64" s="133"/>
-      <c r="AK64" s="133"/>
-      <c r="AL64" s="133"/>
-      <c r="AM64" s="133"/>
-      <c r="AN64" s="133"/>
-      <c r="AO64" s="133"/>
-      <c r="AP64" s="133"/>
-      <c r="AQ64" s="133"/>
-      <c r="AR64" s="133"/>
-      <c r="AS64" s="133"/>
-      <c r="AT64" s="133"/>
-      <c r="AU64" s="133"/>
-      <c r="AV64" s="133"/>
-      <c r="AW64" s="133"/>
-      <c r="AX64" s="133"/>
-      <c r="AY64" s="133"/>
-      <c r="AZ64" s="133"/>
-      <c r="BA64" s="133"/>
-      <c r="BB64" s="133"/>
-      <c r="BC64" s="133"/>
-      <c r="BD64" s="133"/>
-      <c r="BE64" s="133"/>
-      <c r="BF64" s="133"/>
-      <c r="BG64" s="133"/>
-      <c r="BH64" s="133"/>
-      <c r="BI64" s="133"/>
-      <c r="BJ64" s="133"/>
-      <c r="BK64" s="133"/>
-      <c r="BL64" s="133"/>
-      <c r="BM64" s="133"/>
-      <c r="BN64" s="133"/>
-      <c r="BO64" s="133"/>
-      <c r="BP64" s="133"/>
-      <c r="BQ64" s="133"/>
-      <c r="BR64" s="133"/>
-      <c r="BS64" s="133"/>
-      <c r="BT64" s="133"/>
-      <c r="BU64" s="133"/>
-      <c r="BV64" s="133"/>
-      <c r="BW64" s="133"/>
-      <c r="BX64" s="133"/>
-      <c r="BY64" s="133"/>
-      <c r="BZ64" s="133"/>
-      <c r="CA64" s="133"/>
-      <c r="CB64" s="133"/>
-      <c r="CC64" s="133"/>
-      <c r="CD64" s="133"/>
-      <c r="CE64" s="134"/>
+      <c r="G64" s="131"/>
+      <c r="H64" s="132"/>
+      <c r="I64" s="132"/>
+      <c r="J64" s="132"/>
+      <c r="K64" s="132"/>
+      <c r="L64" s="132"/>
+      <c r="M64" s="132"/>
+      <c r="N64" s="132"/>
+      <c r="O64" s="132"/>
+      <c r="P64" s="132"/>
+      <c r="Q64" s="132"/>
+      <c r="R64" s="132"/>
+      <c r="S64" s="132"/>
+      <c r="T64" s="132"/>
+      <c r="U64" s="132"/>
+      <c r="V64" s="132"/>
+      <c r="W64" s="132"/>
+      <c r="X64" s="132"/>
+      <c r="Y64" s="132"/>
+      <c r="Z64" s="132"/>
+      <c r="AA64" s="132"/>
+      <c r="AB64" s="132"/>
+      <c r="AC64" s="132"/>
+      <c r="AD64" s="132"/>
+      <c r="AE64" s="132"/>
+      <c r="AF64" s="132"/>
+      <c r="AG64" s="132"/>
+      <c r="AH64" s="132"/>
+      <c r="AI64" s="132"/>
+      <c r="AJ64" s="132"/>
+      <c r="AK64" s="132"/>
+      <c r="AL64" s="132"/>
+      <c r="AM64" s="132"/>
+      <c r="AN64" s="132"/>
+      <c r="AO64" s="132"/>
+      <c r="AP64" s="132"/>
+      <c r="AQ64" s="132"/>
+      <c r="AR64" s="132"/>
+      <c r="AS64" s="132"/>
+      <c r="AT64" s="132"/>
+      <c r="AU64" s="132"/>
+      <c r="AV64" s="132"/>
+      <c r="AW64" s="132"/>
+      <c r="AX64" s="132"/>
+      <c r="AY64" s="132"/>
+      <c r="AZ64" s="132"/>
+      <c r="BA64" s="132"/>
+      <c r="BB64" s="132"/>
+      <c r="BC64" s="132"/>
+      <c r="BD64" s="132"/>
+      <c r="BE64" s="132"/>
+      <c r="BF64" s="132"/>
+      <c r="BG64" s="132"/>
+      <c r="BH64" s="132"/>
+      <c r="BI64" s="132"/>
+      <c r="BJ64" s="132"/>
+      <c r="BK64" s="132"/>
+      <c r="BL64" s="132"/>
+      <c r="BM64" s="132"/>
+      <c r="BN64" s="132"/>
+      <c r="BO64" s="132"/>
+      <c r="BP64" s="132"/>
+      <c r="BQ64" s="132"/>
+      <c r="BR64" s="132"/>
+      <c r="BS64" s="132"/>
+      <c r="BT64" s="132"/>
+      <c r="BU64" s="132"/>
+      <c r="BV64" s="132"/>
+      <c r="BW64" s="132"/>
+      <c r="BX64" s="132"/>
+      <c r="BY64" s="132"/>
+      <c r="BZ64" s="132"/>
+      <c r="CA64" s="132"/>
+      <c r="CB64" s="132"/>
+      <c r="CC64" s="132"/>
+      <c r="CD64" s="132"/>
+      <c r="CE64" s="133"/>
     </row>
     <row r="65" spans="1:5" ht="14.25" customHeight="1">
       <c r="A65" s="93"/>
@@ -9623,68 +9623,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="AU45:BC45"/>
-    <mergeCell ref="AV41:AZ41"/>
-    <mergeCell ref="AW42:BF42"/>
-    <mergeCell ref="AV43:BC43"/>
-    <mergeCell ref="AU44:BA44"/>
-    <mergeCell ref="AY46:BE46"/>
-    <mergeCell ref="AV47:BA47"/>
-    <mergeCell ref="BA49:BD49"/>
-    <mergeCell ref="AU50:AZ50"/>
-    <mergeCell ref="AY48:BD48"/>
-    <mergeCell ref="BA51:BF51"/>
-    <mergeCell ref="G52:CE52"/>
-    <mergeCell ref="BB53:BE53"/>
-    <mergeCell ref="BF54:BJ54"/>
-    <mergeCell ref="BN62:BT62"/>
-    <mergeCell ref="BP63:BT63"/>
-    <mergeCell ref="G64:CE64"/>
-    <mergeCell ref="BE55:BL55"/>
-    <mergeCell ref="BF56:BL56"/>
-    <mergeCell ref="BJ57:BO57"/>
-    <mergeCell ref="BK58:BS58"/>
-    <mergeCell ref="BL59:BQ59"/>
-    <mergeCell ref="BM60:BS60"/>
-    <mergeCell ref="BM61:BQ61"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="BD4:BJ4"/>
-    <mergeCell ref="BK4:BQ4"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BY4:CE4"/>
-    <mergeCell ref="G7:CE7"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="P15:T15"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="T18:Z18"/>
-    <mergeCell ref="V19:AA19"/>
-    <mergeCell ref="G20:CE20"/>
-    <mergeCell ref="AA21:AH21"/>
-    <mergeCell ref="AB22:AG22"/>
-    <mergeCell ref="AC23:AK23"/>
-    <mergeCell ref="AD24:AJ24"/>
-    <mergeCell ref="AI25:AK25"/>
-    <mergeCell ref="AE26:AJ26"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="AD27:AK27"/>
-    <mergeCell ref="AG28:AK28"/>
-    <mergeCell ref="G29:CE29"/>
     <mergeCell ref="AP30:AQ30"/>
     <mergeCell ref="AI32:AN32"/>
     <mergeCell ref="AJ33:AO33"/>
@@ -9696,6 +9634,68 @@
     <mergeCell ref="AS39:BC39"/>
     <mergeCell ref="AN31:AY31"/>
     <mergeCell ref="AP36:AZ36"/>
+    <mergeCell ref="AC23:AK23"/>
+    <mergeCell ref="AD24:AJ24"/>
+    <mergeCell ref="AI25:AK25"/>
+    <mergeCell ref="AE26:AJ26"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="AD27:AK27"/>
+    <mergeCell ref="AG28:AK28"/>
+    <mergeCell ref="G29:CE29"/>
+    <mergeCell ref="T18:Z18"/>
+    <mergeCell ref="V19:AA19"/>
+    <mergeCell ref="G20:CE20"/>
+    <mergeCell ref="AA21:AH21"/>
+    <mergeCell ref="AB22:AG22"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="P15:T15"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="BD4:BJ4"/>
+    <mergeCell ref="BK4:BQ4"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BY4:CE4"/>
+    <mergeCell ref="G7:CE7"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="BP63:BT63"/>
+    <mergeCell ref="G64:CE64"/>
+    <mergeCell ref="BE55:BL55"/>
+    <mergeCell ref="BF56:BL56"/>
+    <mergeCell ref="BJ57:BO57"/>
+    <mergeCell ref="BK58:BS58"/>
+    <mergeCell ref="BL59:BQ59"/>
+    <mergeCell ref="BM60:BS60"/>
+    <mergeCell ref="BM61:BQ61"/>
+    <mergeCell ref="BA51:BF51"/>
+    <mergeCell ref="G52:CE52"/>
+    <mergeCell ref="BB53:BE53"/>
+    <mergeCell ref="BF54:BJ54"/>
+    <mergeCell ref="BN62:BT62"/>
+    <mergeCell ref="AY46:BE46"/>
+    <mergeCell ref="AV47:BA47"/>
+    <mergeCell ref="BA49:BD49"/>
+    <mergeCell ref="AU50:AZ50"/>
+    <mergeCell ref="AY48:BD48"/>
+    <mergeCell ref="AU45:BC45"/>
+    <mergeCell ref="AV41:AZ41"/>
+    <mergeCell ref="AW42:BF42"/>
+    <mergeCell ref="AV43:BC43"/>
+    <mergeCell ref="AU44:BA44"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.34722222222222199" header="0" footer="0"/>

</xml_diff>

<commit_message>
Up up date Gantt-diagram-A.xlsx
</commit_message>
<xml_diff>
--- a/Gantt-diagram-A.xlsx
+++ b/Gantt-diagram-A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timea\Desktop\Rendszerfejlesztés1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A39255-B2D2-4C78-91F4-35E0BAF354FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7530825-0D66-4A73-816D-2E2A104B4CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,9 +176,6 @@
     <t>8.3.8. Regisztráltak lecke oldal kivitelezése</t>
   </si>
   <si>
-    <t xml:space="preserve">8.3.9. Email-es kiértesítés új időpontfoglalás esetén </t>
-  </si>
-  <si>
     <t>8.3.10. Foglalt időpontok megjelenítése, kezdő és a vég időponttal együtt</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>8.4.21. Bemutató elkészítése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.3.9. Visszajelzés új időpont foglalás esetén </t>
   </si>
 </sst>
 </file>
@@ -1959,7 +1959,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2034,6 +2037,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2082,6 +2088,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2107,7 +2114,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2125,9 +2131,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2136,9 +2139,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="45" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2164,19 +2164,19 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2401,8 +2401,8 @@
   <dimension ref="A1:CE1010"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM58" sqref="AM58"/>
+      <pane ySplit="5" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2514,10 +2514,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="185"/>
+      <c r="E2" s="187"/>
       <c r="F2" s="5"/>
       <c r="G2" s="18"/>
       <c r="H2" s="6"/>
@@ -2601,10 +2601,10 @@
       <c r="A3" s="16"/>
       <c r="B3" s="19"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="184">
+      <c r="D3" s="186">
         <v>45197</v>
       </c>
-      <c r="E3" s="185"/>
+      <c r="E3" s="187"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -2690,117 +2690,117 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="186"/>
-      <c r="G4" s="188">
+      <c r="F4" s="188"/>
+      <c r="G4" s="190">
         <f>G5</f>
         <v>45194</v>
       </c>
-      <c r="H4" s="189"/>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
-      <c r="K4" s="189"/>
-      <c r="L4" s="189"/>
-      <c r="M4" s="190"/>
-      <c r="N4" s="188">
+      <c r="H4" s="191"/>
+      <c r="I4" s="191"/>
+      <c r="J4" s="191"/>
+      <c r="K4" s="191"/>
+      <c r="L4" s="191"/>
+      <c r="M4" s="192"/>
+      <c r="N4" s="190">
         <f>N5</f>
         <v>45201</v>
       </c>
-      <c r="O4" s="189"/>
-      <c r="P4" s="189"/>
-      <c r="Q4" s="189"/>
-      <c r="R4" s="189"/>
-      <c r="S4" s="189"/>
-      <c r="T4" s="190"/>
-      <c r="U4" s="188">
+      <c r="O4" s="191"/>
+      <c r="P4" s="191"/>
+      <c r="Q4" s="191"/>
+      <c r="R4" s="191"/>
+      <c r="S4" s="191"/>
+      <c r="T4" s="192"/>
+      <c r="U4" s="190">
         <f>U5</f>
         <v>45208</v>
       </c>
-      <c r="V4" s="189"/>
-      <c r="W4" s="189"/>
-      <c r="X4" s="189"/>
-      <c r="Y4" s="189"/>
-      <c r="Z4" s="189"/>
-      <c r="AA4" s="190"/>
-      <c r="AB4" s="188">
+      <c r="V4" s="191"/>
+      <c r="W4" s="191"/>
+      <c r="X4" s="191"/>
+      <c r="Y4" s="191"/>
+      <c r="Z4" s="191"/>
+      <c r="AA4" s="192"/>
+      <c r="AB4" s="190">
         <f>AB5</f>
         <v>45215</v>
       </c>
-      <c r="AC4" s="189"/>
-      <c r="AD4" s="189"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="189"/>
-      <c r="AH4" s="190"/>
-      <c r="AI4" s="188">
+      <c r="AC4" s="191"/>
+      <c r="AD4" s="191"/>
+      <c r="AE4" s="191"/>
+      <c r="AF4" s="191"/>
+      <c r="AG4" s="191"/>
+      <c r="AH4" s="192"/>
+      <c r="AI4" s="190">
         <f>AI5</f>
         <v>45222</v>
       </c>
-      <c r="AJ4" s="189"/>
-      <c r="AK4" s="189"/>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="190"/>
-      <c r="AP4" s="188">
+      <c r="AJ4" s="191"/>
+      <c r="AK4" s="191"/>
+      <c r="AL4" s="191"/>
+      <c r="AM4" s="191"/>
+      <c r="AN4" s="191"/>
+      <c r="AO4" s="192"/>
+      <c r="AP4" s="190">
         <f>AP5</f>
         <v>45229</v>
       </c>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="189"/>
-      <c r="AS4" s="189"/>
-      <c r="AT4" s="189"/>
-      <c r="AU4" s="189"/>
-      <c r="AV4" s="190"/>
-      <c r="AW4" s="188">
+      <c r="AQ4" s="191"/>
+      <c r="AR4" s="191"/>
+      <c r="AS4" s="191"/>
+      <c r="AT4" s="191"/>
+      <c r="AU4" s="191"/>
+      <c r="AV4" s="192"/>
+      <c r="AW4" s="190">
         <f>AW5</f>
         <v>45236</v>
       </c>
-      <c r="AX4" s="189"/>
-      <c r="AY4" s="189"/>
-      <c r="AZ4" s="189"/>
-      <c r="BA4" s="189"/>
-      <c r="BB4" s="189"/>
-      <c r="BC4" s="190"/>
-      <c r="BD4" s="188">
+      <c r="AX4" s="191"/>
+      <c r="AY4" s="191"/>
+      <c r="AZ4" s="191"/>
+      <c r="BA4" s="191"/>
+      <c r="BB4" s="191"/>
+      <c r="BC4" s="192"/>
+      <c r="BD4" s="190">
         <f>BD5</f>
         <v>45243</v>
       </c>
-      <c r="BE4" s="189"/>
-      <c r="BF4" s="189"/>
-      <c r="BG4" s="189"/>
-      <c r="BH4" s="189"/>
-      <c r="BI4" s="189"/>
-      <c r="BJ4" s="190"/>
-      <c r="BK4" s="188">
+      <c r="BE4" s="191"/>
+      <c r="BF4" s="191"/>
+      <c r="BG4" s="191"/>
+      <c r="BH4" s="191"/>
+      <c r="BI4" s="191"/>
+      <c r="BJ4" s="192"/>
+      <c r="BK4" s="190">
         <f>BK5</f>
         <v>45250</v>
       </c>
-      <c r="BL4" s="189"/>
-      <c r="BM4" s="189"/>
-      <c r="BN4" s="189"/>
-      <c r="BO4" s="189"/>
-      <c r="BP4" s="189"/>
-      <c r="BQ4" s="190"/>
-      <c r="BR4" s="188">
+      <c r="BL4" s="191"/>
+      <c r="BM4" s="191"/>
+      <c r="BN4" s="191"/>
+      <c r="BO4" s="191"/>
+      <c r="BP4" s="191"/>
+      <c r="BQ4" s="192"/>
+      <c r="BR4" s="190">
         <f>BR5</f>
         <v>45257</v>
       </c>
-      <c r="BS4" s="189"/>
-      <c r="BT4" s="189"/>
-      <c r="BU4" s="189"/>
-      <c r="BV4" s="189"/>
-      <c r="BW4" s="189"/>
-      <c r="BX4" s="190"/>
-      <c r="BY4" s="188">
+      <c r="BS4" s="191"/>
+      <c r="BT4" s="191"/>
+      <c r="BU4" s="191"/>
+      <c r="BV4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="BX4" s="192"/>
+      <c r="BY4" s="190">
         <f>BY5</f>
         <v>45264</v>
       </c>
-      <c r="BZ4" s="189"/>
-      <c r="CA4" s="189"/>
-      <c r="CB4" s="189"/>
-      <c r="CC4" s="189"/>
-      <c r="CD4" s="189"/>
-      <c r="CE4" s="190"/>
+      <c r="BZ4" s="191"/>
+      <c r="CA4" s="191"/>
+      <c r="CB4" s="191"/>
+      <c r="CC4" s="191"/>
+      <c r="CD4" s="191"/>
+      <c r="CE4" s="192"/>
     </row>
     <row r="5" spans="1:83" ht="25.5" customHeight="1" thickBot="1">
       <c r="A5" s="1"/>
@@ -2816,7 +2816,7 @@
       <c r="E5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="187"/>
+      <c r="F5" s="189"/>
       <c r="G5" s="22">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2</f>
         <v>45194</v>
@@ -3220,83 +3220,83 @@
       <c r="D7" s="31"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="191"/>
-      <c r="H7" s="192"/>
-      <c r="I7" s="192"/>
-      <c r="J7" s="192"/>
-      <c r="K7" s="192"/>
-      <c r="L7" s="192"/>
-      <c r="M7" s="192"/>
-      <c r="N7" s="192"/>
-      <c r="O7" s="192"/>
-      <c r="P7" s="192"/>
-      <c r="Q7" s="192"/>
-      <c r="R7" s="192"/>
-      <c r="S7" s="192"/>
-      <c r="T7" s="192"/>
-      <c r="U7" s="192"/>
-      <c r="V7" s="192"/>
-      <c r="W7" s="192"/>
-      <c r="X7" s="192"/>
-      <c r="Y7" s="192"/>
-      <c r="Z7" s="192"/>
-      <c r="AA7" s="192"/>
-      <c r="AB7" s="192"/>
-      <c r="AC7" s="192"/>
-      <c r="AD7" s="192"/>
-      <c r="AE7" s="192"/>
-      <c r="AF7" s="192"/>
-      <c r="AG7" s="192"/>
-      <c r="AH7" s="192"/>
-      <c r="AI7" s="192"/>
-      <c r="AJ7" s="192"/>
-      <c r="AK7" s="192"/>
-      <c r="AL7" s="192"/>
-      <c r="AM7" s="192"/>
-      <c r="AN7" s="192"/>
-      <c r="AO7" s="192"/>
-      <c r="AP7" s="192"/>
-      <c r="AQ7" s="192"/>
-      <c r="AR7" s="192"/>
-      <c r="AS7" s="192"/>
-      <c r="AT7" s="192"/>
-      <c r="AU7" s="192"/>
-      <c r="AV7" s="192"/>
-      <c r="AW7" s="192"/>
-      <c r="AX7" s="192"/>
-      <c r="AY7" s="192"/>
-      <c r="AZ7" s="192"/>
-      <c r="BA7" s="192"/>
-      <c r="BB7" s="192"/>
-      <c r="BC7" s="192"/>
-      <c r="BD7" s="192"/>
-      <c r="BE7" s="192"/>
-      <c r="BF7" s="192"/>
-      <c r="BG7" s="192"/>
-      <c r="BH7" s="192"/>
-      <c r="BI7" s="192"/>
-      <c r="BJ7" s="192"/>
-      <c r="BK7" s="192"/>
-      <c r="BL7" s="192"/>
-      <c r="BM7" s="192"/>
-      <c r="BN7" s="192"/>
-      <c r="BO7" s="192"/>
-      <c r="BP7" s="192"/>
-      <c r="BQ7" s="192"/>
-      <c r="BR7" s="192"/>
-      <c r="BS7" s="192"/>
-      <c r="BT7" s="192"/>
-      <c r="BU7" s="192"/>
-      <c r="BV7" s="192"/>
-      <c r="BW7" s="192"/>
-      <c r="BX7" s="192"/>
-      <c r="BY7" s="192"/>
-      <c r="BZ7" s="192"/>
-      <c r="CA7" s="192"/>
-      <c r="CB7" s="192"/>
-      <c r="CC7" s="192"/>
-      <c r="CD7" s="192"/>
-      <c r="CE7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="194"/>
+      <c r="I7" s="194"/>
+      <c r="J7" s="194"/>
+      <c r="K7" s="194"/>
+      <c r="L7" s="194"/>
+      <c r="M7" s="194"/>
+      <c r="N7" s="194"/>
+      <c r="O7" s="194"/>
+      <c r="P7" s="194"/>
+      <c r="Q7" s="194"/>
+      <c r="R7" s="194"/>
+      <c r="S7" s="194"/>
+      <c r="T7" s="194"/>
+      <c r="U7" s="194"/>
+      <c r="V7" s="194"/>
+      <c r="W7" s="194"/>
+      <c r="X7" s="194"/>
+      <c r="Y7" s="194"/>
+      <c r="Z7" s="194"/>
+      <c r="AA7" s="194"/>
+      <c r="AB7" s="194"/>
+      <c r="AC7" s="194"/>
+      <c r="AD7" s="194"/>
+      <c r="AE7" s="194"/>
+      <c r="AF7" s="194"/>
+      <c r="AG7" s="194"/>
+      <c r="AH7" s="194"/>
+      <c r="AI7" s="194"/>
+      <c r="AJ7" s="194"/>
+      <c r="AK7" s="194"/>
+      <c r="AL7" s="194"/>
+      <c r="AM7" s="194"/>
+      <c r="AN7" s="194"/>
+      <c r="AO7" s="194"/>
+      <c r="AP7" s="194"/>
+      <c r="AQ7" s="194"/>
+      <c r="AR7" s="194"/>
+      <c r="AS7" s="194"/>
+      <c r="AT7" s="194"/>
+      <c r="AU7" s="194"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="AX7" s="194"/>
+      <c r="AY7" s="194"/>
+      <c r="AZ7" s="194"/>
+      <c r="BA7" s="194"/>
+      <c r="BB7" s="194"/>
+      <c r="BC7" s="194"/>
+      <c r="BD7" s="194"/>
+      <c r="BE7" s="194"/>
+      <c r="BF7" s="194"/>
+      <c r="BG7" s="194"/>
+      <c r="BH7" s="194"/>
+      <c r="BI7" s="194"/>
+      <c r="BJ7" s="194"/>
+      <c r="BK7" s="194"/>
+      <c r="BL7" s="194"/>
+      <c r="BM7" s="194"/>
+      <c r="BN7" s="194"/>
+      <c r="BO7" s="194"/>
+      <c r="BP7" s="194"/>
+      <c r="BQ7" s="194"/>
+      <c r="BR7" s="194"/>
+      <c r="BS7" s="194"/>
+      <c r="BT7" s="194"/>
+      <c r="BU7" s="194"/>
+      <c r="BV7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="BX7" s="194"/>
+      <c r="BY7" s="194"/>
+      <c r="BZ7" s="194"/>
+      <c r="CA7" s="194"/>
+      <c r="CB7" s="194"/>
+      <c r="CC7" s="194"/>
+      <c r="CD7" s="194"/>
+      <c r="CE7" s="195"/>
     </row>
     <row r="8" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
@@ -3316,8 +3316,8 @@
       <c r="G8" s="115"/>
       <c r="H8" s="132"/>
       <c r="I8" s="104"/>
-      <c r="J8" s="194"/>
-      <c r="K8" s="195"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="197"/>
       <c r="L8" s="105"/>
       <c r="M8" s="106"/>
       <c r="N8" s="103"/>
@@ -3409,9 +3409,9 @@
       <c r="G9" s="115"/>
       <c r="H9" s="133"/>
       <c r="I9" s="40"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="145"/>
-      <c r="L9" s="195"/>
+      <c r="J9" s="196"/>
+      <c r="K9" s="198"/>
+      <c r="L9" s="197"/>
       <c r="M9" s="92"/>
       <c r="N9" s="103"/>
       <c r="O9" s="103"/>
@@ -3504,8 +3504,8 @@
       <c r="I10" s="93"/>
       <c r="J10" s="90"/>
       <c r="K10" s="91"/>
-      <c r="L10" s="196"/>
-      <c r="M10" s="195"/>
+      <c r="L10" s="199"/>
+      <c r="M10" s="197"/>
       <c r="N10" s="103"/>
       <c r="O10" s="103"/>
       <c r="P10" s="103"/>
@@ -3596,8 +3596,8 @@
       <c r="H11" s="133"/>
       <c r="I11" s="93"/>
       <c r="J11" s="40"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="198"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="201"/>
       <c r="M11" s="41"/>
       <c r="N11" s="103"/>
       <c r="O11" s="103"/>
@@ -3692,10 +3692,10 @@
       <c r="K12" s="90"/>
       <c r="L12" s="85"/>
       <c r="M12" s="89"/>
-      <c r="N12" s="175"/>
-      <c r="O12" s="145"/>
-      <c r="P12" s="145"/>
-      <c r="Q12" s="195"/>
+      <c r="N12" s="177"/>
+      <c r="O12" s="198"/>
+      <c r="P12" s="198"/>
+      <c r="Q12" s="197"/>
       <c r="R12" s="93"/>
       <c r="S12" s="94"/>
       <c r="T12" s="94"/>
@@ -3783,11 +3783,11 @@
       <c r="I13" s="93"/>
       <c r="J13" s="88"/>
       <c r="K13" s="42"/>
-      <c r="L13" s="199"/>
-      <c r="M13" s="182"/>
-      <c r="N13" s="192"/>
-      <c r="O13" s="192"/>
-      <c r="P13" s="193"/>
+      <c r="L13" s="202"/>
+      <c r="M13" s="184"/>
+      <c r="N13" s="194"/>
+      <c r="O13" s="194"/>
+      <c r="P13" s="195"/>
       <c r="Q13" s="45"/>
       <c r="R13" s="88"/>
       <c r="S13" s="94"/>
@@ -3878,11 +3878,11 @@
       <c r="K14" s="93"/>
       <c r="L14" s="87"/>
       <c r="M14" s="87"/>
-      <c r="N14" s="178"/>
-      <c r="O14" s="173"/>
-      <c r="P14" s="173"/>
-      <c r="Q14" s="173"/>
-      <c r="R14" s="174"/>
+      <c r="N14" s="180"/>
+      <c r="O14" s="175"/>
+      <c r="P14" s="175"/>
+      <c r="Q14" s="175"/>
+      <c r="R14" s="176"/>
       <c r="S14" s="92"/>
       <c r="T14" s="85"/>
       <c r="U14" s="88"/>
@@ -3973,11 +3973,11 @@
       <c r="M15" s="94"/>
       <c r="N15" s="90"/>
       <c r="O15" s="114"/>
-      <c r="P15" s="200"/>
-      <c r="Q15" s="173"/>
-      <c r="R15" s="173"/>
-      <c r="S15" s="173"/>
-      <c r="T15" s="183"/>
+      <c r="P15" s="203"/>
+      <c r="Q15" s="175"/>
+      <c r="R15" s="175"/>
+      <c r="S15" s="175"/>
+      <c r="T15" s="185"/>
       <c r="U15" s="88"/>
       <c r="V15" s="88"/>
       <c r="W15" s="86"/>
@@ -4070,11 +4070,11 @@
       <c r="Q16" s="90"/>
       <c r="R16" s="90"/>
       <c r="S16" s="87"/>
-      <c r="T16" s="201"/>
-      <c r="U16" s="145"/>
-      <c r="V16" s="145"/>
-      <c r="W16" s="145"/>
-      <c r="X16" s="195"/>
+      <c r="T16" s="204"/>
+      <c r="U16" s="198"/>
+      <c r="V16" s="198"/>
+      <c r="W16" s="198"/>
+      <c r="X16" s="197"/>
       <c r="Y16" s="88"/>
       <c r="Z16" s="43"/>
       <c r="AA16" s="38"/>
@@ -4167,9 +4167,9 @@
       <c r="U17" s="45"/>
       <c r="V17" s="45"/>
       <c r="W17" s="46"/>
-      <c r="X17" s="202"/>
-      <c r="Y17" s="173"/>
-      <c r="Z17" s="174"/>
+      <c r="X17" s="205"/>
+      <c r="Y17" s="175"/>
+      <c r="Z17" s="176"/>
       <c r="AA17" s="38"/>
       <c r="AB17" s="28"/>
       <c r="AC17" s="28"/>
@@ -4256,13 +4256,13 @@
       <c r="Q18" s="93"/>
       <c r="R18" s="93"/>
       <c r="S18" s="87"/>
-      <c r="T18" s="203"/>
-      <c r="U18" s="173"/>
-      <c r="V18" s="173"/>
-      <c r="W18" s="173"/>
-      <c r="X18" s="173"/>
-      <c r="Y18" s="173"/>
-      <c r="Z18" s="174"/>
+      <c r="T18" s="206"/>
+      <c r="U18" s="175"/>
+      <c r="V18" s="175"/>
+      <c r="W18" s="175"/>
+      <c r="X18" s="175"/>
+      <c r="Y18" s="175"/>
+      <c r="Z18" s="176"/>
       <c r="AA18" s="38"/>
       <c r="AB18" s="28"/>
       <c r="AC18" s="28"/>
@@ -4352,12 +4352,12 @@
       <c r="S19" s="117"/>
       <c r="T19" s="117"/>
       <c r="U19" s="118"/>
-      <c r="V19" s="204"/>
-      <c r="W19" s="205"/>
-      <c r="X19" s="205"/>
-      <c r="Y19" s="205"/>
-      <c r="Z19" s="205"/>
-      <c r="AA19" s="206"/>
+      <c r="V19" s="207"/>
+      <c r="W19" s="146"/>
+      <c r="X19" s="146"/>
+      <c r="Y19" s="146"/>
+      <c r="Z19" s="146"/>
+      <c r="AA19" s="208"/>
       <c r="AB19" s="119"/>
       <c r="AC19" s="119"/>
       <c r="AD19" s="119"/>
@@ -4424,83 +4424,83 @@
       <c r="D20" s="50"/>
       <c r="E20" s="51"/>
       <c r="F20" s="37"/>
-      <c r="G20" s="191"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
-      <c r="K20" s="192"/>
-      <c r="L20" s="192"/>
-      <c r="M20" s="192"/>
-      <c r="N20" s="192"/>
-      <c r="O20" s="192"/>
-      <c r="P20" s="192"/>
-      <c r="Q20" s="192"/>
-      <c r="R20" s="192"/>
-      <c r="S20" s="192"/>
-      <c r="T20" s="192"/>
-      <c r="U20" s="192"/>
-      <c r="V20" s="192"/>
-      <c r="W20" s="192"/>
-      <c r="X20" s="192"/>
-      <c r="Y20" s="192"/>
-      <c r="Z20" s="192"/>
-      <c r="AA20" s="192"/>
-      <c r="AB20" s="192"/>
-      <c r="AC20" s="192"/>
-      <c r="AD20" s="192"/>
-      <c r="AE20" s="192"/>
-      <c r="AF20" s="192"/>
-      <c r="AG20" s="192"/>
-      <c r="AH20" s="192"/>
-      <c r="AI20" s="192"/>
-      <c r="AJ20" s="192"/>
-      <c r="AK20" s="192"/>
-      <c r="AL20" s="192"/>
-      <c r="AM20" s="192"/>
-      <c r="AN20" s="192"/>
-      <c r="AO20" s="192"/>
-      <c r="AP20" s="192"/>
-      <c r="AQ20" s="192"/>
-      <c r="AR20" s="192"/>
-      <c r="AS20" s="192"/>
-      <c r="AT20" s="192"/>
-      <c r="AU20" s="192"/>
-      <c r="AV20" s="192"/>
-      <c r="AW20" s="192"/>
-      <c r="AX20" s="192"/>
-      <c r="AY20" s="192"/>
-      <c r="AZ20" s="192"/>
-      <c r="BA20" s="192"/>
-      <c r="BB20" s="192"/>
-      <c r="BC20" s="192"/>
-      <c r="BD20" s="192"/>
-      <c r="BE20" s="192"/>
-      <c r="BF20" s="192"/>
-      <c r="BG20" s="192"/>
-      <c r="BH20" s="192"/>
-      <c r="BI20" s="192"/>
-      <c r="BJ20" s="192"/>
-      <c r="BK20" s="192"/>
-      <c r="BL20" s="192"/>
-      <c r="BM20" s="192"/>
-      <c r="BN20" s="192"/>
-      <c r="BO20" s="192"/>
-      <c r="BP20" s="192"/>
-      <c r="BQ20" s="192"/>
-      <c r="BR20" s="192"/>
-      <c r="BS20" s="192"/>
-      <c r="BT20" s="192"/>
-      <c r="BU20" s="192"/>
-      <c r="BV20" s="192"/>
-      <c r="BW20" s="192"/>
-      <c r="BX20" s="192"/>
-      <c r="BY20" s="192"/>
-      <c r="BZ20" s="192"/>
-      <c r="CA20" s="192"/>
-      <c r="CB20" s="192"/>
-      <c r="CC20" s="192"/>
-      <c r="CD20" s="192"/>
-      <c r="CE20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="194"/>
+      <c r="I20" s="194"/>
+      <c r="J20" s="194"/>
+      <c r="K20" s="194"/>
+      <c r="L20" s="194"/>
+      <c r="M20" s="194"/>
+      <c r="N20" s="194"/>
+      <c r="O20" s="194"/>
+      <c r="P20" s="194"/>
+      <c r="Q20" s="194"/>
+      <c r="R20" s="194"/>
+      <c r="S20" s="194"/>
+      <c r="T20" s="194"/>
+      <c r="U20" s="194"/>
+      <c r="V20" s="194"/>
+      <c r="W20" s="194"/>
+      <c r="X20" s="194"/>
+      <c r="Y20" s="194"/>
+      <c r="Z20" s="194"/>
+      <c r="AA20" s="194"/>
+      <c r="AB20" s="194"/>
+      <c r="AC20" s="194"/>
+      <c r="AD20" s="194"/>
+      <c r="AE20" s="194"/>
+      <c r="AF20" s="194"/>
+      <c r="AG20" s="194"/>
+      <c r="AH20" s="194"/>
+      <c r="AI20" s="194"/>
+      <c r="AJ20" s="194"/>
+      <c r="AK20" s="194"/>
+      <c r="AL20" s="194"/>
+      <c r="AM20" s="194"/>
+      <c r="AN20" s="194"/>
+      <c r="AO20" s="194"/>
+      <c r="AP20" s="194"/>
+      <c r="AQ20" s="194"/>
+      <c r="AR20" s="194"/>
+      <c r="AS20" s="194"/>
+      <c r="AT20" s="194"/>
+      <c r="AU20" s="194"/>
+      <c r="AV20" s="194"/>
+      <c r="AW20" s="194"/>
+      <c r="AX20" s="194"/>
+      <c r="AY20" s="194"/>
+      <c r="AZ20" s="194"/>
+      <c r="BA20" s="194"/>
+      <c r="BB20" s="194"/>
+      <c r="BC20" s="194"/>
+      <c r="BD20" s="194"/>
+      <c r="BE20" s="194"/>
+      <c r="BF20" s="194"/>
+      <c r="BG20" s="194"/>
+      <c r="BH20" s="194"/>
+      <c r="BI20" s="194"/>
+      <c r="BJ20" s="194"/>
+      <c r="BK20" s="194"/>
+      <c r="BL20" s="194"/>
+      <c r="BM20" s="194"/>
+      <c r="BN20" s="194"/>
+      <c r="BO20" s="194"/>
+      <c r="BP20" s="194"/>
+      <c r="BQ20" s="194"/>
+      <c r="BR20" s="194"/>
+      <c r="BS20" s="194"/>
+      <c r="BT20" s="194"/>
+      <c r="BU20" s="194"/>
+      <c r="BV20" s="194"/>
+      <c r="BW20" s="194"/>
+      <c r="BX20" s="194"/>
+      <c r="BY20" s="194"/>
+      <c r="BZ20" s="194"/>
+      <c r="CA20" s="194"/>
+      <c r="CB20" s="194"/>
+      <c r="CC20" s="194"/>
+      <c r="CD20" s="194"/>
+      <c r="CE20" s="195"/>
     </row>
     <row r="21" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A21" s="1"/>
@@ -4537,14 +4537,14 @@
       <c r="X21" s="110"/>
       <c r="Y21" s="110"/>
       <c r="Z21" s="122"/>
-      <c r="AA21" s="207"/>
-      <c r="AB21" s="208"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AA21" s="209"/>
+      <c r="AB21" s="210"/>
+      <c r="AC21" s="210"/>
+      <c r="AD21" s="210"/>
+      <c r="AE21" s="210"/>
+      <c r="AF21" s="210"/>
+      <c r="AG21" s="210"/>
+      <c r="AH21" s="211"/>
       <c r="AI21" s="103"/>
       <c r="AJ21" s="110"/>
       <c r="AK21" s="110"/>
@@ -4631,12 +4631,12 @@
       <c r="Y22" s="28"/>
       <c r="Z22" s="39"/>
       <c r="AA22" s="87"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="174"/>
+      <c r="AB22" s="212"/>
+      <c r="AC22" s="175"/>
+      <c r="AD22" s="175"/>
+      <c r="AE22" s="175"/>
+      <c r="AF22" s="175"/>
+      <c r="AG22" s="176"/>
       <c r="AH22" s="92"/>
       <c r="AI22" s="86"/>
       <c r="AJ22" s="86"/>
@@ -4725,15 +4725,15 @@
       <c r="Z23" s="39"/>
       <c r="AA23" s="39"/>
       <c r="AB23" s="55"/>
-      <c r="AC23" s="178"/>
-      <c r="AD23" s="182"/>
-      <c r="AE23" s="182"/>
-      <c r="AF23" s="182"/>
-      <c r="AG23" s="182"/>
-      <c r="AH23" s="182"/>
-      <c r="AI23" s="182"/>
-      <c r="AJ23" s="182"/>
-      <c r="AK23" s="174"/>
+      <c r="AC23" s="180"/>
+      <c r="AD23" s="184"/>
+      <c r="AE23" s="184"/>
+      <c r="AF23" s="184"/>
+      <c r="AG23" s="184"/>
+      <c r="AH23" s="184"/>
+      <c r="AI23" s="184"/>
+      <c r="AJ23" s="184"/>
+      <c r="AK23" s="176"/>
       <c r="AL23" s="93"/>
       <c r="AM23" s="28"/>
       <c r="AN23" s="39"/>
@@ -4819,13 +4819,13 @@
       <c r="AA24" s="39"/>
       <c r="AB24" s="28"/>
       <c r="AC24" s="55"/>
-      <c r="AD24" s="201"/>
-      <c r="AE24" s="145"/>
-      <c r="AF24" s="145"/>
-      <c r="AG24" s="145"/>
-      <c r="AH24" s="145"/>
-      <c r="AI24" s="145"/>
-      <c r="AJ24" s="195"/>
+      <c r="AD24" s="204"/>
+      <c r="AE24" s="198"/>
+      <c r="AF24" s="198"/>
+      <c r="AG24" s="198"/>
+      <c r="AH24" s="198"/>
+      <c r="AI24" s="198"/>
+      <c r="AJ24" s="197"/>
       <c r="AK24" s="90"/>
       <c r="AL24" s="28"/>
       <c r="AM24" s="28"/>
@@ -4917,9 +4917,9 @@
       <c r="AF25" s="47"/>
       <c r="AG25" s="47"/>
       <c r="AH25" s="55"/>
-      <c r="AI25" s="211"/>
-      <c r="AJ25" s="212"/>
-      <c r="AK25" s="174"/>
+      <c r="AI25" s="213"/>
+      <c r="AJ25" s="214"/>
+      <c r="AK25" s="176"/>
       <c r="AL25" s="93"/>
       <c r="AM25" s="28"/>
       <c r="AN25" s="39"/>
@@ -5006,12 +5006,12 @@
       <c r="AB26" s="28"/>
       <c r="AC26" s="28"/>
       <c r="AD26" s="28"/>
-      <c r="AE26" s="172"/>
-      <c r="AF26" s="173"/>
-      <c r="AG26" s="173"/>
-      <c r="AH26" s="173"/>
-      <c r="AI26" s="173"/>
-      <c r="AJ26" s="174"/>
+      <c r="AE26" s="174"/>
+      <c r="AF26" s="175"/>
+      <c r="AG26" s="175"/>
+      <c r="AH26" s="175"/>
+      <c r="AI26" s="175"/>
+      <c r="AJ26" s="176"/>
       <c r="AK26" s="45"/>
       <c r="AL26" s="28"/>
       <c r="AM26" s="28"/>
@@ -5098,14 +5098,14 @@
       <c r="AA27" s="39"/>
       <c r="AB27" s="28"/>
       <c r="AC27" s="56"/>
-      <c r="AD27" s="203"/>
-      <c r="AE27" s="173"/>
-      <c r="AF27" s="173"/>
-      <c r="AG27" s="182"/>
-      <c r="AH27" s="182"/>
-      <c r="AI27" s="182"/>
-      <c r="AJ27" s="182"/>
-      <c r="AK27" s="183"/>
+      <c r="AD27" s="206"/>
+      <c r="AE27" s="175"/>
+      <c r="AF27" s="175"/>
+      <c r="AG27" s="184"/>
+      <c r="AH27" s="184"/>
+      <c r="AI27" s="184"/>
+      <c r="AJ27" s="184"/>
+      <c r="AK27" s="185"/>
       <c r="AL27" s="93"/>
       <c r="AM27" s="28"/>
       <c r="AN27" s="39"/>
@@ -5167,7 +5167,7 @@
       <c r="E28" s="54">
         <v>45225</v>
       </c>
-      <c r="F28" s="213"/>
+      <c r="F28" s="215"/>
       <c r="G28" s="115"/>
       <c r="H28" s="119"/>
       <c r="I28" s="119"/>
@@ -5194,11 +5194,11 @@
       <c r="AD28" s="118"/>
       <c r="AE28" s="118"/>
       <c r="AF28" s="123"/>
-      <c r="AG28" s="194"/>
-      <c r="AH28" s="145"/>
-      <c r="AI28" s="145"/>
-      <c r="AJ28" s="145"/>
-      <c r="AK28" s="195"/>
+      <c r="AG28" s="196"/>
+      <c r="AH28" s="198"/>
+      <c r="AI28" s="198"/>
+      <c r="AJ28" s="198"/>
+      <c r="AK28" s="197"/>
       <c r="AL28" s="116"/>
       <c r="AM28" s="119"/>
       <c r="AN28" s="120"/>
@@ -5254,84 +5254,84 @@
       <c r="C29" s="58"/>
       <c r="D29" s="59"/>
       <c r="E29" s="60"/>
-      <c r="F29" s="214"/>
-      <c r="G29" s="191"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
-      <c r="K29" s="192"/>
-      <c r="L29" s="192"/>
-      <c r="M29" s="192"/>
-      <c r="N29" s="192"/>
-      <c r="O29" s="192"/>
-      <c r="P29" s="192"/>
-      <c r="Q29" s="192"/>
-      <c r="R29" s="192"/>
-      <c r="S29" s="192"/>
-      <c r="T29" s="192"/>
-      <c r="U29" s="192"/>
-      <c r="V29" s="192"/>
-      <c r="W29" s="192"/>
-      <c r="X29" s="192"/>
-      <c r="Y29" s="192"/>
-      <c r="Z29" s="192"/>
-      <c r="AA29" s="192"/>
-      <c r="AB29" s="192"/>
-      <c r="AC29" s="192"/>
-      <c r="AD29" s="192"/>
-      <c r="AE29" s="192"/>
-      <c r="AF29" s="192"/>
-      <c r="AG29" s="192"/>
-      <c r="AH29" s="192"/>
-      <c r="AI29" s="192"/>
-      <c r="AJ29" s="192"/>
-      <c r="AK29" s="192"/>
-      <c r="AL29" s="192"/>
-      <c r="AM29" s="192"/>
-      <c r="AN29" s="192"/>
-      <c r="AO29" s="192"/>
-      <c r="AP29" s="192"/>
-      <c r="AQ29" s="192"/>
-      <c r="AR29" s="192"/>
-      <c r="AS29" s="192"/>
-      <c r="AT29" s="192"/>
-      <c r="AU29" s="192"/>
-      <c r="AV29" s="192"/>
-      <c r="AW29" s="192"/>
-      <c r="AX29" s="192"/>
-      <c r="AY29" s="192"/>
-      <c r="AZ29" s="192"/>
-      <c r="BA29" s="192"/>
-      <c r="BB29" s="192"/>
-      <c r="BC29" s="192"/>
-      <c r="BD29" s="192"/>
-      <c r="BE29" s="192"/>
-      <c r="BF29" s="192"/>
-      <c r="BG29" s="192"/>
-      <c r="BH29" s="192"/>
-      <c r="BI29" s="192"/>
-      <c r="BJ29" s="192"/>
-      <c r="BK29" s="192"/>
-      <c r="BL29" s="192"/>
-      <c r="BM29" s="192"/>
-      <c r="BN29" s="192"/>
-      <c r="BO29" s="192"/>
-      <c r="BP29" s="192"/>
-      <c r="BQ29" s="192"/>
-      <c r="BR29" s="192"/>
-      <c r="BS29" s="192"/>
-      <c r="BT29" s="192"/>
-      <c r="BU29" s="192"/>
-      <c r="BV29" s="192"/>
-      <c r="BW29" s="192"/>
-      <c r="BX29" s="192"/>
-      <c r="BY29" s="192"/>
-      <c r="BZ29" s="192"/>
-      <c r="CA29" s="192"/>
-      <c r="CB29" s="192"/>
-      <c r="CC29" s="192"/>
-      <c r="CD29" s="192"/>
-      <c r="CE29" s="193"/>
+      <c r="F29" s="216"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="194"/>
+      <c r="I29" s="194"/>
+      <c r="J29" s="194"/>
+      <c r="K29" s="194"/>
+      <c r="L29" s="194"/>
+      <c r="M29" s="194"/>
+      <c r="N29" s="194"/>
+      <c r="O29" s="194"/>
+      <c r="P29" s="194"/>
+      <c r="Q29" s="194"/>
+      <c r="R29" s="194"/>
+      <c r="S29" s="194"/>
+      <c r="T29" s="194"/>
+      <c r="U29" s="194"/>
+      <c r="V29" s="194"/>
+      <c r="W29" s="194"/>
+      <c r="X29" s="194"/>
+      <c r="Y29" s="194"/>
+      <c r="Z29" s="194"/>
+      <c r="AA29" s="194"/>
+      <c r="AB29" s="194"/>
+      <c r="AC29" s="194"/>
+      <c r="AD29" s="194"/>
+      <c r="AE29" s="194"/>
+      <c r="AF29" s="194"/>
+      <c r="AG29" s="194"/>
+      <c r="AH29" s="194"/>
+      <c r="AI29" s="194"/>
+      <c r="AJ29" s="194"/>
+      <c r="AK29" s="194"/>
+      <c r="AL29" s="194"/>
+      <c r="AM29" s="194"/>
+      <c r="AN29" s="194"/>
+      <c r="AO29" s="194"/>
+      <c r="AP29" s="194"/>
+      <c r="AQ29" s="194"/>
+      <c r="AR29" s="194"/>
+      <c r="AS29" s="194"/>
+      <c r="AT29" s="194"/>
+      <c r="AU29" s="194"/>
+      <c r="AV29" s="194"/>
+      <c r="AW29" s="194"/>
+      <c r="AX29" s="194"/>
+      <c r="AY29" s="194"/>
+      <c r="AZ29" s="194"/>
+      <c r="BA29" s="194"/>
+      <c r="BB29" s="194"/>
+      <c r="BC29" s="194"/>
+      <c r="BD29" s="194"/>
+      <c r="BE29" s="194"/>
+      <c r="BF29" s="194"/>
+      <c r="BG29" s="194"/>
+      <c r="BH29" s="194"/>
+      <c r="BI29" s="194"/>
+      <c r="BJ29" s="194"/>
+      <c r="BK29" s="194"/>
+      <c r="BL29" s="194"/>
+      <c r="BM29" s="194"/>
+      <c r="BN29" s="194"/>
+      <c r="BO29" s="194"/>
+      <c r="BP29" s="194"/>
+      <c r="BQ29" s="194"/>
+      <c r="BR29" s="194"/>
+      <c r="BS29" s="194"/>
+      <c r="BT29" s="194"/>
+      <c r="BU29" s="194"/>
+      <c r="BV29" s="194"/>
+      <c r="BW29" s="194"/>
+      <c r="BX29" s="194"/>
+      <c r="BY29" s="194"/>
+      <c r="BZ29" s="194"/>
+      <c r="CA29" s="194"/>
+      <c r="CB29" s="194"/>
+      <c r="CC29" s="194"/>
+      <c r="CD29" s="194"/>
+      <c r="CE29" s="195"/>
     </row>
     <row r="30" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A30" s="1"/>
@@ -5429,7 +5429,7 @@
     <row r="31" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
       <c r="B31" s="61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="62" t="s">
         <v>3</v>
@@ -5474,18 +5474,18 @@
       <c r="AK31" s="28"/>
       <c r="AL31" s="28"/>
       <c r="AM31" s="56"/>
-      <c r="AN31" s="175"/>
-      <c r="AO31" s="176"/>
-      <c r="AP31" s="176"/>
-      <c r="AQ31" s="176"/>
-      <c r="AR31" s="176"/>
-      <c r="AS31" s="176"/>
-      <c r="AT31" s="176"/>
-      <c r="AU31" s="176"/>
-      <c r="AV31" s="176"/>
-      <c r="AW31" s="176"/>
-      <c r="AX31" s="176"/>
-      <c r="AY31" s="177"/>
+      <c r="AN31" s="177"/>
+      <c r="AO31" s="178"/>
+      <c r="AP31" s="178"/>
+      <c r="AQ31" s="178"/>
+      <c r="AR31" s="178"/>
+      <c r="AS31" s="178"/>
+      <c r="AT31" s="178"/>
+      <c r="AU31" s="178"/>
+      <c r="AV31" s="178"/>
+      <c r="AW31" s="178"/>
+      <c r="AX31" s="178"/>
+      <c r="AY31" s="179"/>
       <c r="AZ31" s="93"/>
       <c r="BA31" s="28"/>
       <c r="BB31" s="64"/>
@@ -5564,12 +5564,12 @@
       <c r="AF32" s="28"/>
       <c r="AG32" s="39"/>
       <c r="AH32" s="126"/>
-      <c r="AI32" s="197"/>
-      <c r="AJ32" s="173"/>
-      <c r="AK32" s="173"/>
-      <c r="AL32" s="173"/>
-      <c r="AM32" s="173"/>
-      <c r="AN32" s="198"/>
+      <c r="AI32" s="200"/>
+      <c r="AJ32" s="175"/>
+      <c r="AK32" s="175"/>
+      <c r="AL32" s="175"/>
+      <c r="AM32" s="175"/>
+      <c r="AN32" s="201"/>
       <c r="AO32" s="92"/>
       <c r="AP32" s="47"/>
       <c r="AQ32" s="47"/>
@@ -5658,12 +5658,12 @@
       <c r="AG33" s="39"/>
       <c r="AH33" s="39"/>
       <c r="AI33" s="55"/>
-      <c r="AJ33" s="215"/>
-      <c r="AK33" s="173"/>
-      <c r="AL33" s="173"/>
-      <c r="AM33" s="173"/>
-      <c r="AN33" s="173"/>
-      <c r="AO33" s="174"/>
+      <c r="AJ33" s="234"/>
+      <c r="AK33" s="175"/>
+      <c r="AL33" s="175"/>
+      <c r="AM33" s="175"/>
+      <c r="AN33" s="175"/>
+      <c r="AO33" s="176"/>
       <c r="AP33" s="88"/>
       <c r="AQ33" s="28"/>
       <c r="AR33" s="28"/>
@@ -5752,12 +5752,12 @@
       <c r="AH34" s="39"/>
       <c r="AI34" s="28"/>
       <c r="AJ34" s="55"/>
-      <c r="AK34" s="216"/>
-      <c r="AL34" s="173"/>
-      <c r="AM34" s="173"/>
-      <c r="AN34" s="173"/>
-      <c r="AO34" s="173"/>
-      <c r="AP34" s="174"/>
+      <c r="AK34" s="217"/>
+      <c r="AL34" s="175"/>
+      <c r="AM34" s="175"/>
+      <c r="AN34" s="175"/>
+      <c r="AO34" s="175"/>
+      <c r="AP34" s="176"/>
       <c r="AQ34" s="88"/>
       <c r="AR34" s="28"/>
       <c r="AS34" s="28"/>
@@ -5846,12 +5846,12 @@
       <c r="AI35" s="28"/>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="46"/>
-      <c r="AL35" s="197"/>
-      <c r="AM35" s="173"/>
-      <c r="AN35" s="173"/>
-      <c r="AO35" s="173"/>
-      <c r="AP35" s="182"/>
-      <c r="AQ35" s="183"/>
+      <c r="AL35" s="200"/>
+      <c r="AM35" s="175"/>
+      <c r="AN35" s="175"/>
+      <c r="AO35" s="175"/>
+      <c r="AP35" s="184"/>
+      <c r="AQ35" s="185"/>
       <c r="AR35" s="88"/>
       <c r="AS35" s="86"/>
       <c r="AT35" s="86"/>
@@ -5943,17 +5943,17 @@
       <c r="AM36" s="47"/>
       <c r="AN36" s="94"/>
       <c r="AO36" s="87"/>
-      <c r="AP36" s="175"/>
-      <c r="AQ36" s="176"/>
-      <c r="AR36" s="176"/>
-      <c r="AS36" s="176"/>
-      <c r="AT36" s="176"/>
-      <c r="AU36" s="176"/>
-      <c r="AV36" s="176"/>
-      <c r="AW36" s="176"/>
-      <c r="AX36" s="176"/>
-      <c r="AY36" s="176"/>
-      <c r="AZ36" s="177"/>
+      <c r="AP36" s="177"/>
+      <c r="AQ36" s="178"/>
+      <c r="AR36" s="178"/>
+      <c r="AS36" s="178"/>
+      <c r="AT36" s="178"/>
+      <c r="AU36" s="178"/>
+      <c r="AV36" s="178"/>
+      <c r="AW36" s="178"/>
+      <c r="AX36" s="178"/>
+      <c r="AY36" s="178"/>
+      <c r="AZ36" s="179"/>
       <c r="BA36" s="88"/>
       <c r="BB36" s="64"/>
       <c r="BC36" s="64"/>
@@ -6042,17 +6042,17 @@
       <c r="AS37" s="66"/>
       <c r="AT37" s="66"/>
       <c r="AU37" s="89"/>
-      <c r="AV37" s="217"/>
-      <c r="AW37" s="212"/>
-      <c r="AX37" s="212"/>
-      <c r="AY37" s="212"/>
-      <c r="AZ37" s="212"/>
-      <c r="BA37" s="173"/>
-      <c r="BB37" s="173"/>
-      <c r="BC37" s="173"/>
-      <c r="BD37" s="173"/>
-      <c r="BE37" s="173"/>
-      <c r="BF37" s="174"/>
+      <c r="AV37" s="218"/>
+      <c r="AW37" s="214"/>
+      <c r="AX37" s="214"/>
+      <c r="AY37" s="214"/>
+      <c r="AZ37" s="214"/>
+      <c r="BA37" s="175"/>
+      <c r="BB37" s="175"/>
+      <c r="BC37" s="175"/>
+      <c r="BD37" s="175"/>
+      <c r="BE37" s="175"/>
+      <c r="BF37" s="176"/>
       <c r="BG37" s="93"/>
       <c r="BH37" s="28"/>
       <c r="BI37" s="39"/>
@@ -6082,7 +6082,7 @@
     <row r="38" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="1"/>
       <c r="B38" s="61" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C38" s="62" t="s">
         <v>4</v>
@@ -6131,17 +6131,17 @@
       <c r="AO38" s="39"/>
       <c r="AP38" s="28"/>
       <c r="AQ38" s="56"/>
-      <c r="AR38" s="200"/>
-      <c r="AS38" s="173"/>
-      <c r="AT38" s="173"/>
-      <c r="AU38" s="173"/>
-      <c r="AV38" s="173"/>
-      <c r="AW38" s="173"/>
-      <c r="AX38" s="173"/>
-      <c r="AY38" s="173"/>
-      <c r="AZ38" s="173"/>
-      <c r="BA38" s="173"/>
-      <c r="BB38" s="174"/>
+      <c r="AR38" s="203"/>
+      <c r="AS38" s="175"/>
+      <c r="AT38" s="175"/>
+      <c r="AU38" s="175"/>
+      <c r="AV38" s="175"/>
+      <c r="AW38" s="175"/>
+      <c r="AX38" s="175"/>
+      <c r="AY38" s="175"/>
+      <c r="AZ38" s="175"/>
+      <c r="BA38" s="175"/>
+      <c r="BB38" s="176"/>
       <c r="BC38" s="92"/>
       <c r="BD38" s="47"/>
       <c r="BE38" s="47"/>
@@ -6175,7 +6175,7 @@
     <row r="39" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A39" s="1"/>
       <c r="B39" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="62" t="s">
         <v>7</v>
@@ -6225,17 +6225,17 @@
       <c r="AP39" s="28"/>
       <c r="AQ39" s="28"/>
       <c r="AR39" s="55"/>
-      <c r="AS39" s="218"/>
-      <c r="AT39" s="173"/>
-      <c r="AU39" s="173"/>
-      <c r="AV39" s="173"/>
-      <c r="AW39" s="173"/>
-      <c r="AX39" s="173"/>
-      <c r="AY39" s="173"/>
-      <c r="AZ39" s="173"/>
-      <c r="BA39" s="173"/>
-      <c r="BB39" s="173"/>
-      <c r="BC39" s="174"/>
+      <c r="AS39" s="219"/>
+      <c r="AT39" s="175"/>
+      <c r="AU39" s="175"/>
+      <c r="AV39" s="175"/>
+      <c r="AW39" s="175"/>
+      <c r="AX39" s="175"/>
+      <c r="AY39" s="175"/>
+      <c r="AZ39" s="175"/>
+      <c r="BA39" s="175"/>
+      <c r="BB39" s="175"/>
+      <c r="BC39" s="176"/>
       <c r="BD39" s="88"/>
       <c r="BE39" s="28"/>
       <c r="BF39" s="28"/>
@@ -6268,7 +6268,7 @@
     <row r="40" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
       <c r="B40" s="61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="62" t="s">
         <v>4</v>
@@ -6319,17 +6319,17 @@
       <c r="AQ40" s="28"/>
       <c r="AR40" s="28"/>
       <c r="AS40" s="55"/>
-      <c r="AT40" s="200"/>
-      <c r="AU40" s="173"/>
-      <c r="AV40" s="173"/>
-      <c r="AW40" s="173"/>
-      <c r="AX40" s="173"/>
-      <c r="AY40" s="173"/>
-      <c r="AZ40" s="173"/>
-      <c r="BA40" s="173"/>
-      <c r="BB40" s="173"/>
-      <c r="BC40" s="173"/>
-      <c r="BD40" s="174"/>
+      <c r="AT40" s="203"/>
+      <c r="AU40" s="175"/>
+      <c r="AV40" s="175"/>
+      <c r="AW40" s="175"/>
+      <c r="AX40" s="175"/>
+      <c r="AY40" s="175"/>
+      <c r="AZ40" s="175"/>
+      <c r="BA40" s="175"/>
+      <c r="BB40" s="175"/>
+      <c r="BC40" s="175"/>
+      <c r="BD40" s="176"/>
       <c r="BE40" s="93"/>
       <c r="BF40" s="28"/>
       <c r="BG40" s="28"/>
@@ -6361,7 +6361,7 @@
     <row r="41" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A41" s="1"/>
       <c r="B41" s="61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="62" t="s">
         <v>5</v>
@@ -6414,11 +6414,11 @@
       <c r="AS41" s="28"/>
       <c r="AT41" s="47"/>
       <c r="AU41" s="87"/>
-      <c r="AV41" s="172"/>
-      <c r="AW41" s="173"/>
-      <c r="AX41" s="173"/>
-      <c r="AY41" s="173"/>
-      <c r="AZ41" s="174"/>
+      <c r="AV41" s="174"/>
+      <c r="AW41" s="175"/>
+      <c r="AX41" s="175"/>
+      <c r="AY41" s="175"/>
+      <c r="AZ41" s="176"/>
       <c r="BA41" s="45"/>
       <c r="BB41" s="85"/>
       <c r="BC41" s="85"/>
@@ -6454,7 +6454,7 @@
     <row r="42" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A42" s="1"/>
       <c r="B42" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="62" t="s">
         <v>7</v>
@@ -6508,16 +6508,16 @@
       <c r="AT42" s="28"/>
       <c r="AU42" s="89"/>
       <c r="AV42" s="89"/>
-      <c r="AW42" s="178"/>
-      <c r="AX42" s="173"/>
-      <c r="AY42" s="173"/>
-      <c r="AZ42" s="173"/>
-      <c r="BA42" s="173"/>
-      <c r="BB42" s="173"/>
-      <c r="BC42" s="173"/>
-      <c r="BD42" s="173"/>
-      <c r="BE42" s="173"/>
-      <c r="BF42" s="174"/>
+      <c r="AW42" s="180"/>
+      <c r="AX42" s="175"/>
+      <c r="AY42" s="175"/>
+      <c r="AZ42" s="175"/>
+      <c r="BA42" s="175"/>
+      <c r="BB42" s="175"/>
+      <c r="BC42" s="175"/>
+      <c r="BD42" s="175"/>
+      <c r="BE42" s="175"/>
+      <c r="BF42" s="176"/>
       <c r="BG42" s="88"/>
       <c r="BH42" s="86"/>
       <c r="BI42" s="64"/>
@@ -6547,7 +6547,7 @@
     <row r="43" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A43" s="1"/>
       <c r="B43" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="62" t="s">
         <v>2</v>
@@ -6600,14 +6600,14 @@
       <c r="AS43" s="28"/>
       <c r="AT43" s="28"/>
       <c r="AU43" s="43"/>
-      <c r="AV43" s="179"/>
-      <c r="AW43" s="173"/>
-      <c r="AX43" s="173"/>
-      <c r="AY43" s="173"/>
-      <c r="AZ43" s="173"/>
-      <c r="BA43" s="173"/>
-      <c r="BB43" s="173"/>
-      <c r="BC43" s="180"/>
+      <c r="AV43" s="181"/>
+      <c r="AW43" s="175"/>
+      <c r="AX43" s="175"/>
+      <c r="AY43" s="175"/>
+      <c r="AZ43" s="175"/>
+      <c r="BA43" s="175"/>
+      <c r="BB43" s="175"/>
+      <c r="BC43" s="182"/>
       <c r="BD43" s="28"/>
       <c r="BE43" s="28"/>
       <c r="BF43" s="28"/>
@@ -6640,7 +6640,7 @@
     <row r="44" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A44" s="1"/>
       <c r="B44" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="62" t="s">
         <v>1</v>
@@ -6692,13 +6692,13 @@
       <c r="AR44" s="28"/>
       <c r="AS44" s="86"/>
       <c r="AT44" s="46"/>
-      <c r="AU44" s="181"/>
-      <c r="AV44" s="182"/>
-      <c r="AW44" s="182"/>
-      <c r="AX44" s="182"/>
-      <c r="AY44" s="182"/>
-      <c r="AZ44" s="182"/>
-      <c r="BA44" s="183"/>
+      <c r="AU44" s="183"/>
+      <c r="AV44" s="184"/>
+      <c r="AW44" s="184"/>
+      <c r="AX44" s="184"/>
+      <c r="AY44" s="184"/>
+      <c r="AZ44" s="184"/>
+      <c r="BA44" s="185"/>
       <c r="BB44" s="92"/>
       <c r="BC44" s="85"/>
       <c r="BD44" s="47"/>
@@ -6733,7 +6733,7 @@
     <row r="45" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A45" s="1"/>
       <c r="B45" s="61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="62" t="s">
         <v>3</v>
@@ -6785,15 +6785,15 @@
       <c r="AR45" s="56"/>
       <c r="AS45" s="56"/>
       <c r="AT45" s="56"/>
-      <c r="AU45" s="175"/>
-      <c r="AV45" s="176"/>
-      <c r="AW45" s="176"/>
-      <c r="AX45" s="176"/>
-      <c r="AY45" s="176"/>
-      <c r="AZ45" s="176"/>
-      <c r="BA45" s="176"/>
-      <c r="BB45" s="176"/>
-      <c r="BC45" s="177"/>
+      <c r="AU45" s="177"/>
+      <c r="AV45" s="178"/>
+      <c r="AW45" s="178"/>
+      <c r="AX45" s="178"/>
+      <c r="AY45" s="178"/>
+      <c r="AZ45" s="178"/>
+      <c r="BA45" s="178"/>
+      <c r="BB45" s="178"/>
+      <c r="BC45" s="179"/>
       <c r="BD45" s="88"/>
       <c r="BE45" s="86"/>
       <c r="BF45" s="28"/>
@@ -6826,7 +6826,7 @@
     <row r="46" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A46" s="1"/>
       <c r="B46" s="61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="62" t="s">
         <v>4</v>
@@ -6882,12 +6882,12 @@
       <c r="AV46" s="87"/>
       <c r="AW46" s="66"/>
       <c r="AX46" s="46"/>
-      <c r="AY46" s="231"/>
-      <c r="AZ46" s="145"/>
-      <c r="BA46" s="145"/>
-      <c r="BB46" s="145"/>
-      <c r="BC46" s="145"/>
-      <c r="BD46" s="195"/>
+      <c r="AY46" s="233"/>
+      <c r="AZ46" s="198"/>
+      <c r="BA46" s="198"/>
+      <c r="BB46" s="198"/>
+      <c r="BC46" s="198"/>
+      <c r="BD46" s="197"/>
       <c r="BE46" s="100"/>
       <c r="BF46" s="93"/>
       <c r="BG46" s="28"/>
@@ -6919,7 +6919,7 @@
     <row r="47" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="1"/>
       <c r="B47" s="61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="62" t="s">
         <v>7</v>
@@ -6972,12 +6972,12 @@
       <c r="AS47" s="28"/>
       <c r="AT47" s="47"/>
       <c r="AU47" s="87"/>
-      <c r="AV47" s="178"/>
-      <c r="AW47" s="173"/>
-      <c r="AX47" s="173"/>
-      <c r="AY47" s="182"/>
-      <c r="AZ47" s="182"/>
-      <c r="BA47" s="183"/>
+      <c r="AV47" s="180"/>
+      <c r="AW47" s="175"/>
+      <c r="AX47" s="175"/>
+      <c r="AY47" s="184"/>
+      <c r="AZ47" s="184"/>
+      <c r="BA47" s="185"/>
       <c r="BB47" s="85"/>
       <c r="BC47" s="85"/>
       <c r="BD47" s="66"/>
@@ -7012,7 +7012,7 @@
     <row r="48" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A48" s="1"/>
       <c r="B48" s="61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="62" t="s">
         <v>5</v>
@@ -7068,11 +7068,11 @@
       <c r="AV48" s="94"/>
       <c r="AW48" s="47"/>
       <c r="AX48" s="55"/>
-      <c r="AY48" s="172"/>
-      <c r="AZ48" s="173"/>
-      <c r="BA48" s="173"/>
-      <c r="BB48" s="173"/>
-      <c r="BC48" s="174"/>
+      <c r="AY48" s="174"/>
+      <c r="AZ48" s="175"/>
+      <c r="BA48" s="175"/>
+      <c r="BB48" s="175"/>
+      <c r="BC48" s="176"/>
       <c r="BD48" s="101"/>
       <c r="BE48" s="93"/>
       <c r="BF48" s="28"/>
@@ -7104,10 +7104,10 @@
     </row>
     <row r="49" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A49" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" s="62" t="s">
         <v>1</v>
@@ -7165,10 +7165,10 @@
       <c r="AX49" s="86"/>
       <c r="AY49" s="66"/>
       <c r="AZ49" s="46"/>
-      <c r="BA49" s="154"/>
-      <c r="BB49" s="155"/>
-      <c r="BC49" s="155"/>
-      <c r="BD49" s="230"/>
+      <c r="BA49" s="155"/>
+      <c r="BB49" s="156"/>
+      <c r="BC49" s="156"/>
+      <c r="BD49" s="232"/>
       <c r="BE49" s="93"/>
       <c r="BF49" s="28"/>
       <c r="BG49" s="28"/>
@@ -7200,7 +7200,7 @@
     <row r="50" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A50" s="1"/>
       <c r="B50" s="61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="62" t="s">
         <v>6</v>
@@ -7252,12 +7252,12 @@
       <c r="AR50" s="28"/>
       <c r="AS50" s="28"/>
       <c r="AT50" s="55"/>
-      <c r="AU50" s="216"/>
-      <c r="AV50" s="173"/>
-      <c r="AW50" s="173"/>
-      <c r="AX50" s="173"/>
-      <c r="AY50" s="173"/>
-      <c r="AZ50" s="174"/>
+      <c r="AU50" s="217"/>
+      <c r="AV50" s="175"/>
+      <c r="AW50" s="175"/>
+      <c r="AX50" s="175"/>
+      <c r="AY50" s="175"/>
+      <c r="AZ50" s="176"/>
       <c r="BA50" s="45"/>
       <c r="BB50" s="85"/>
       <c r="BC50" s="85"/>
@@ -7293,7 +7293,7 @@
     <row r="51" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A51" s="1"/>
       <c r="B51" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="62" t="s">
         <v>1</v>
@@ -7386,94 +7386,94 @@
     <row r="52" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A52" s="1"/>
       <c r="B52" s="67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="68"/>
       <c r="D52" s="69"/>
       <c r="E52" s="70"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="191"/>
-      <c r="H52" s="192"/>
-      <c r="I52" s="192"/>
-      <c r="J52" s="192"/>
-      <c r="K52" s="192"/>
-      <c r="L52" s="192"/>
-      <c r="M52" s="192"/>
-      <c r="N52" s="192"/>
-      <c r="O52" s="192"/>
-      <c r="P52" s="192"/>
-      <c r="Q52" s="192"/>
-      <c r="R52" s="192"/>
-      <c r="S52" s="192"/>
-      <c r="T52" s="192"/>
-      <c r="U52" s="192"/>
-      <c r="V52" s="192"/>
-      <c r="W52" s="192"/>
-      <c r="X52" s="192"/>
-      <c r="Y52" s="192"/>
-      <c r="Z52" s="192"/>
-      <c r="AA52" s="192"/>
-      <c r="AB52" s="192"/>
-      <c r="AC52" s="192"/>
-      <c r="AD52" s="192"/>
-      <c r="AE52" s="192"/>
-      <c r="AF52" s="192"/>
-      <c r="AG52" s="192"/>
-      <c r="AH52" s="192"/>
-      <c r="AI52" s="192"/>
-      <c r="AJ52" s="192"/>
-      <c r="AK52" s="192"/>
-      <c r="AL52" s="192"/>
-      <c r="AM52" s="192"/>
-      <c r="AN52" s="192"/>
-      <c r="AO52" s="192"/>
-      <c r="AP52" s="192"/>
-      <c r="AQ52" s="192"/>
-      <c r="AR52" s="192"/>
-      <c r="AS52" s="192"/>
-      <c r="AT52" s="192"/>
-      <c r="AU52" s="192"/>
-      <c r="AV52" s="192"/>
-      <c r="AW52" s="192"/>
-      <c r="AX52" s="192"/>
-      <c r="AY52" s="192"/>
-      <c r="AZ52" s="192"/>
-      <c r="BA52" s="192"/>
-      <c r="BB52" s="192"/>
-      <c r="BC52" s="192"/>
-      <c r="BD52" s="192"/>
-      <c r="BE52" s="192"/>
-      <c r="BF52" s="192"/>
-      <c r="BG52" s="192"/>
-      <c r="BH52" s="192"/>
-      <c r="BI52" s="192"/>
-      <c r="BJ52" s="192"/>
-      <c r="BK52" s="192"/>
-      <c r="BL52" s="192"/>
-      <c r="BM52" s="192"/>
-      <c r="BN52" s="192"/>
-      <c r="BO52" s="192"/>
-      <c r="BP52" s="192"/>
-      <c r="BQ52" s="192"/>
-      <c r="BR52" s="192"/>
-      <c r="BS52" s="192"/>
-      <c r="BT52" s="192"/>
-      <c r="BU52" s="192"/>
-      <c r="BV52" s="192"/>
-      <c r="BW52" s="192"/>
-      <c r="BX52" s="192"/>
-      <c r="BY52" s="192"/>
-      <c r="BZ52" s="192"/>
-      <c r="CA52" s="192"/>
-      <c r="CB52" s="192"/>
-      <c r="CC52" s="192"/>
-      <c r="CD52" s="192"/>
-      <c r="CE52" s="193"/>
+      <c r="G52" s="193"/>
+      <c r="H52" s="194"/>
+      <c r="I52" s="194"/>
+      <c r="J52" s="194"/>
+      <c r="K52" s="194"/>
+      <c r="L52" s="194"/>
+      <c r="M52" s="194"/>
+      <c r="N52" s="194"/>
+      <c r="O52" s="194"/>
+      <c r="P52" s="194"/>
+      <c r="Q52" s="194"/>
+      <c r="R52" s="194"/>
+      <c r="S52" s="194"/>
+      <c r="T52" s="194"/>
+      <c r="U52" s="194"/>
+      <c r="V52" s="194"/>
+      <c r="W52" s="194"/>
+      <c r="X52" s="194"/>
+      <c r="Y52" s="194"/>
+      <c r="Z52" s="194"/>
+      <c r="AA52" s="194"/>
+      <c r="AB52" s="194"/>
+      <c r="AC52" s="194"/>
+      <c r="AD52" s="194"/>
+      <c r="AE52" s="194"/>
+      <c r="AF52" s="194"/>
+      <c r="AG52" s="194"/>
+      <c r="AH52" s="194"/>
+      <c r="AI52" s="194"/>
+      <c r="AJ52" s="194"/>
+      <c r="AK52" s="194"/>
+      <c r="AL52" s="194"/>
+      <c r="AM52" s="194"/>
+      <c r="AN52" s="194"/>
+      <c r="AO52" s="194"/>
+      <c r="AP52" s="194"/>
+      <c r="AQ52" s="194"/>
+      <c r="AR52" s="194"/>
+      <c r="AS52" s="194"/>
+      <c r="AT52" s="194"/>
+      <c r="AU52" s="194"/>
+      <c r="AV52" s="194"/>
+      <c r="AW52" s="194"/>
+      <c r="AX52" s="194"/>
+      <c r="AY52" s="194"/>
+      <c r="AZ52" s="194"/>
+      <c r="BA52" s="194"/>
+      <c r="BB52" s="194"/>
+      <c r="BC52" s="194"/>
+      <c r="BD52" s="194"/>
+      <c r="BE52" s="194"/>
+      <c r="BF52" s="194"/>
+      <c r="BG52" s="194"/>
+      <c r="BH52" s="194"/>
+      <c r="BI52" s="194"/>
+      <c r="BJ52" s="194"/>
+      <c r="BK52" s="194"/>
+      <c r="BL52" s="194"/>
+      <c r="BM52" s="194"/>
+      <c r="BN52" s="194"/>
+      <c r="BO52" s="194"/>
+      <c r="BP52" s="194"/>
+      <c r="BQ52" s="194"/>
+      <c r="BR52" s="194"/>
+      <c r="BS52" s="194"/>
+      <c r="BT52" s="194"/>
+      <c r="BU52" s="194"/>
+      <c r="BV52" s="194"/>
+      <c r="BW52" s="194"/>
+      <c r="BX52" s="194"/>
+      <c r="BY52" s="194"/>
+      <c r="BZ52" s="194"/>
+      <c r="CA52" s="194"/>
+      <c r="CB52" s="194"/>
+      <c r="CC52" s="194"/>
+      <c r="CD52" s="194"/>
+      <c r="CE52" s="195"/>
     </row>
     <row r="53" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A53" s="1"/>
       <c r="B53" s="71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="72" t="s">
         <v>8</v>
@@ -7566,7 +7566,7 @@
     <row r="54" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A54" s="1"/>
       <c r="B54" s="71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="72" t="s">
         <v>6</v>
@@ -7659,7 +7659,7 @@
     <row r="55" spans="1:83" ht="15.75" thickBot="1">
       <c r="A55" s="1"/>
       <c r="B55" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="72" t="s">
         <v>7</v>
@@ -7752,7 +7752,7 @@
     <row r="56" spans="1:83" ht="15.75" thickBot="1">
       <c r="A56" s="1"/>
       <c r="B56" s="71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" s="72" t="s">
         <v>6</v>
@@ -7845,7 +7845,7 @@
     <row r="57" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A57" s="1"/>
       <c r="B57" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="72" t="s">
         <v>3</v>
@@ -7915,13 +7915,13 @@
       <c r="BJ57" s="94"/>
       <c r="BK57" s="28"/>
       <c r="BL57" s="86"/>
-      <c r="BM57" s="233"/>
-      <c r="BN57" s="234"/>
-      <c r="BO57" s="234"/>
-      <c r="BP57" s="176"/>
-      <c r="BQ57" s="176"/>
-      <c r="BR57" s="176"/>
-      <c r="BS57" s="177"/>
+      <c r="BM57" s="230"/>
+      <c r="BN57" s="231"/>
+      <c r="BO57" s="231"/>
+      <c r="BP57" s="178"/>
+      <c r="BQ57" s="178"/>
+      <c r="BR57" s="178"/>
+      <c r="BS57" s="179"/>
       <c r="BT57" s="93"/>
       <c r="BU57" s="28"/>
       <c r="BV57" s="28"/>
@@ -7938,7 +7938,7 @@
     <row r="58" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A58" s="1"/>
       <c r="B58" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="72" t="s">
         <v>1</v>
@@ -8007,10 +8007,10 @@
       <c r="BI58" s="39"/>
       <c r="BJ58" s="87"/>
       <c r="BK58" s="56"/>
-      <c r="BL58" s="151"/>
-      <c r="BM58" s="152"/>
-      <c r="BN58" s="152"/>
-      <c r="BO58" s="153"/>
+      <c r="BL58" s="152"/>
+      <c r="BM58" s="153"/>
+      <c r="BN58" s="153"/>
+      <c r="BO58" s="154"/>
       <c r="BP58" s="92"/>
       <c r="BQ58" s="85"/>
       <c r="BR58" s="90"/>
@@ -8031,7 +8031,7 @@
     <row r="59" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A59" s="1"/>
       <c r="B59" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="72" t="s">
         <v>5</v>
@@ -8101,11 +8101,11 @@
       <c r="BJ59" s="39"/>
       <c r="BK59" s="28"/>
       <c r="BL59" s="55"/>
-      <c r="BM59" s="232"/>
-      <c r="BN59" s="205"/>
-      <c r="BO59" s="205"/>
-      <c r="BP59" s="146"/>
-      <c r="BQ59" s="147"/>
+      <c r="BM59" s="145"/>
+      <c r="BN59" s="146"/>
+      <c r="BO59" s="146"/>
+      <c r="BP59" s="147"/>
+      <c r="BQ59" s="148"/>
       <c r="BR59" s="45"/>
       <c r="BS59" s="66"/>
       <c r="BT59" s="86"/>
@@ -8124,7 +8124,7 @@
     <row r="60" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A60" s="1"/>
       <c r="B60" s="99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="97" t="s">
         <v>7</v>
@@ -8217,7 +8217,7 @@
     <row r="61" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A61" s="1"/>
       <c r="B61" s="99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" s="97" t="s">
         <v>1</v>
@@ -8293,10 +8293,10 @@
       <c r="BP61" s="85"/>
       <c r="BQ61" s="85"/>
       <c r="BR61" s="91"/>
-      <c r="BS61" s="151"/>
-      <c r="BT61" s="152"/>
-      <c r="BU61" s="152"/>
-      <c r="BV61" s="153"/>
+      <c r="BS61" s="152"/>
+      <c r="BT61" s="153"/>
+      <c r="BU61" s="153"/>
+      <c r="BV61" s="154"/>
       <c r="BW61" s="38"/>
       <c r="BX61" s="39"/>
       <c r="BY61" s="28"/>
@@ -8310,7 +8310,7 @@
     <row r="62" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A62" s="1"/>
       <c r="B62" s="96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62" s="97" t="s">
         <v>2</v>
@@ -8381,11 +8381,11 @@
       <c r="BK62" s="28"/>
       <c r="BL62" s="28"/>
       <c r="BM62" s="56"/>
-      <c r="BN62" s="168"/>
-      <c r="BO62" s="169"/>
-      <c r="BP62" s="169"/>
-      <c r="BQ62" s="169"/>
-      <c r="BR62" s="219"/>
+      <c r="BN62" s="169"/>
+      <c r="BO62" s="170"/>
+      <c r="BP62" s="170"/>
+      <c r="BQ62" s="170"/>
+      <c r="BR62" s="173"/>
       <c r="BS62" s="45"/>
       <c r="BT62" s="66"/>
       <c r="BU62" s="66"/>
@@ -8403,7 +8403,7 @@
     <row r="63" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A63" s="1"/>
       <c r="B63" s="96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" s="97" t="s">
         <v>8</v>
@@ -8496,7 +8496,7 @@
     <row r="64" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="1"/>
       <c r="B64" s="96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="97" t="s">
         <v>2</v>
@@ -8570,10 +8570,10 @@
       <c r="BN64" s="47"/>
       <c r="BO64" s="55"/>
       <c r="BP64" s="89"/>
-      <c r="BQ64" s="168"/>
-      <c r="BR64" s="169"/>
-      <c r="BS64" s="170"/>
-      <c r="BT64" s="171"/>
+      <c r="BQ64" s="169"/>
+      <c r="BR64" s="170"/>
+      <c r="BS64" s="171"/>
+      <c r="BT64" s="172"/>
       <c r="BU64" s="45"/>
       <c r="BV64" s="86"/>
       <c r="BW64" s="39"/>
@@ -8589,7 +8589,7 @@
     <row r="65" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A65" s="1"/>
       <c r="B65" s="96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="97" t="s">
         <v>5</v>
@@ -8664,11 +8664,11 @@
       <c r="BO65" s="55"/>
       <c r="BP65" s="64"/>
       <c r="BQ65" s="89"/>
-      <c r="BR65" s="165"/>
-      <c r="BS65" s="166"/>
-      <c r="BT65" s="166"/>
-      <c r="BU65" s="166"/>
-      <c r="BV65" s="167"/>
+      <c r="BR65" s="166"/>
+      <c r="BS65" s="167"/>
+      <c r="BT65" s="167"/>
+      <c r="BU65" s="167"/>
+      <c r="BV65" s="168"/>
       <c r="BW65" s="38"/>
       <c r="BX65" s="39"/>
       <c r="BY65" s="28"/>
@@ -8682,7 +8682,7 @@
     <row r="66" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A66" s="1"/>
       <c r="B66" s="96" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="97" t="s">
         <v>4</v>
@@ -8755,10 +8755,10 @@
       <c r="BM66" s="28"/>
       <c r="BN66" s="47"/>
       <c r="BO66" s="55"/>
-      <c r="BP66" s="160"/>
-      <c r="BQ66" s="161"/>
-      <c r="BR66" s="163"/>
-      <c r="BS66" s="164"/>
+      <c r="BP66" s="161"/>
+      <c r="BQ66" s="162"/>
+      <c r="BR66" s="164"/>
+      <c r="BS66" s="165"/>
       <c r="BT66" s="90"/>
       <c r="BU66" s="47"/>
       <c r="BV66" s="47"/>
@@ -8775,7 +8775,7 @@
     <row r="67" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A67" s="1"/>
       <c r="B67" s="96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="97" t="s">
         <v>6</v>
@@ -8868,7 +8868,7 @@
     <row r="68" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A68" s="1"/>
       <c r="B68" s="96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="97" t="s">
         <v>6</v>
@@ -8961,7 +8961,7 @@
     <row r="69" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A69" s="1"/>
       <c r="B69" s="96" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" s="97" t="s">
         <v>4</v>
@@ -9035,11 +9035,11 @@
       <c r="BN69" s="28"/>
       <c r="BO69" s="55"/>
       <c r="BP69" s="89"/>
-      <c r="BQ69" s="160"/>
-      <c r="BR69" s="161"/>
-      <c r="BS69" s="161"/>
-      <c r="BT69" s="161"/>
-      <c r="BU69" s="162"/>
+      <c r="BQ69" s="161"/>
+      <c r="BR69" s="162"/>
+      <c r="BS69" s="162"/>
+      <c r="BT69" s="162"/>
+      <c r="BU69" s="163"/>
       <c r="BV69" s="93"/>
       <c r="BW69" s="39"/>
       <c r="BX69" s="39"/>
@@ -9054,7 +9054,7 @@
     <row r="70" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A70" s="1"/>
       <c r="B70" s="96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="97" t="s">
         <v>3</v>
@@ -9127,11 +9127,11 @@
       <c r="BM70" s="28"/>
       <c r="BN70" s="28"/>
       <c r="BO70" s="56"/>
-      <c r="BP70" s="148"/>
-      <c r="BQ70" s="149"/>
-      <c r="BR70" s="149"/>
-      <c r="BS70" s="149"/>
-      <c r="BT70" s="150"/>
+      <c r="BP70" s="149"/>
+      <c r="BQ70" s="150"/>
+      <c r="BR70" s="150"/>
+      <c r="BS70" s="150"/>
+      <c r="BT70" s="151"/>
       <c r="BU70" s="90"/>
       <c r="BV70" s="28"/>
       <c r="BW70" s="39"/>
@@ -9147,7 +9147,7 @@
     <row r="71" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A71" s="1"/>
       <c r="B71" s="74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="72" t="s">
         <v>7</v>
@@ -9222,9 +9222,9 @@
       <c r="BO71" s="28"/>
       <c r="BP71" s="94"/>
       <c r="BQ71" s="87"/>
-      <c r="BR71" s="157"/>
-      <c r="BS71" s="158"/>
-      <c r="BT71" s="159"/>
+      <c r="BR71" s="158"/>
+      <c r="BS71" s="159"/>
+      <c r="BT71" s="160"/>
       <c r="BU71" s="93"/>
       <c r="BV71" s="86"/>
       <c r="BW71" s="64"/>
@@ -9240,7 +9240,7 @@
     <row r="72" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A72" s="1"/>
       <c r="B72" s="96" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="97" t="s">
         <v>1</v>
@@ -9319,10 +9319,10 @@
       <c r="BS72" s="119"/>
       <c r="BT72" s="119"/>
       <c r="BU72" s="130"/>
-      <c r="BV72" s="151"/>
-      <c r="BW72" s="152"/>
-      <c r="BX72" s="152"/>
-      <c r="BY72" s="153"/>
+      <c r="BV72" s="152"/>
+      <c r="BW72" s="153"/>
+      <c r="BX72" s="153"/>
+      <c r="BY72" s="154"/>
       <c r="BZ72" s="88"/>
       <c r="CA72" s="28"/>
       <c r="CB72" s="28"/>
@@ -9333,7 +9333,7 @@
     <row r="73" spans="1:83" ht="15" customHeight="1" thickBot="1">
       <c r="A73" s="1"/>
       <c r="B73" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" s="72" t="s">
         <v>1</v>
@@ -9414,9 +9414,9 @@
       <c r="BU73" s="28"/>
       <c r="BV73" s="47"/>
       <c r="BW73" s="87"/>
-      <c r="BX73" s="154"/>
-      <c r="BY73" s="155"/>
-      <c r="BZ73" s="156"/>
+      <c r="BX73" s="155"/>
+      <c r="BY73" s="156"/>
+      <c r="BZ73" s="157"/>
       <c r="CA73" s="93"/>
       <c r="CB73" s="28"/>
       <c r="CC73" s="28"/>

</xml_diff>